<commit_message>
Update the Desin Tasks of this Week
Update the Desin Tasks of this Week
</commit_message>
<xml_diff>
--- a/PM/Project schedule.xlsx
+++ b/PM/Project schedule.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="101">
   <si>
     <t>HELP</t>
   </si>
@@ -300,6 +300,49 @@
   </si>
   <si>
     <t>Allaa Gamal</t>
+  </si>
+  <si>
+    <t>HLD</t>
+  </si>
+  <si>
+    <t>GUI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Udate Project Plan </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Detailed Design </t>
+  </si>
+  <si>
+    <t>Alaa Gamal</t>
+  </si>
+  <si>
+    <t>Data Flow Model</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Design Document </t>
+  </si>
+  <si>
+    <t>Sondos Mahmoud</t>
+  </si>
+  <si>
+    <t>Update Schedule</t>
+  </si>
+  <si>
+    <t>Update RTM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Software Peer Review Sheet </t>
+  </si>
+  <si>
+    <t>Update Responsibility Assignment</t>
+  </si>
+  <si>
+    <t>Salsabeel
+Hassan
+Sondos
+Khadija
+Ahmed</t>
   </si>
 </sst>
 </file>
@@ -738,7 +781,7 @@
     </xf>
     <xf numFmtId="9" fontId="25" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -922,6 +965,9 @@
     <xf numFmtId="0" fontId="12" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" customBuiltin="1"/>
@@ -1102,9 +1148,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:f>ProjectTimeline!$A$32:$B$86</c:f>
+              <c:f>ProjectTimeline!$A$32:$B$102</c:f>
               <c:multiLvlStrCache>
-                <c:ptCount val="50"/>
+                <c:ptCount val="66"/>
                 <c:lvl>
                   <c:pt idx="5">
                     <c:v>Responsibility Assignment Matrix</c:v>
@@ -1138,6 +1184,36 @@
                   </c:pt>
                   <c:pt idx="26">
                     <c:v>SRS Peer Review</c:v>
+                  </c:pt>
+                  <c:pt idx="31">
+                    <c:v>Udate Project Plan </c:v>
+                  </c:pt>
+                  <c:pt idx="33">
+                    <c:v>GUI</c:v>
+                  </c:pt>
+                  <c:pt idx="35">
+                    <c:v>HLD</c:v>
+                  </c:pt>
+                  <c:pt idx="37">
+                    <c:v>Data Flow Model</c:v>
+                  </c:pt>
+                  <c:pt idx="39">
+                    <c:v>Detailed Design </c:v>
+                  </c:pt>
+                  <c:pt idx="41">
+                    <c:v>Design Document </c:v>
+                  </c:pt>
+                  <c:pt idx="43">
+                    <c:v>Update Schedule</c:v>
+                  </c:pt>
+                  <c:pt idx="45">
+                    <c:v>Update RTM</c:v>
+                  </c:pt>
+                  <c:pt idx="47">
+                    <c:v>Update Responsibility Assignment</c:v>
+                  </c:pt>
+                  <c:pt idx="49">
+                    <c:v>Software Peer Review Sheet </c:v>
                   </c:pt>
                 </c:lvl>
                 <c:lvl>
@@ -1150,13 +1226,13 @@
                   <c:pt idx="30">
                     <c:v>Design</c:v>
                   </c:pt>
-                  <c:pt idx="35">
+                  <c:pt idx="51">
                     <c:v>Development</c:v>
                   </c:pt>
-                  <c:pt idx="44">
+                  <c:pt idx="60">
                     <c:v>Testing</c:v>
                   </c:pt>
-                  <c:pt idx="49">
+                  <c:pt idx="65">
                     <c:v>Delivery</c:v>
                   </c:pt>
                 </c:lvl>
@@ -1165,10 +1241,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>ProjectTimeline!$F$32:$F$86</c:f>
+              <c:f>ProjectTimeline!$F$32:$F$102</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="55"/>
+                <c:ptCount val="71"/>
                 <c:pt idx="5" formatCode="m/d/yy;@">
                   <c:v>43582</c:v>
                 </c:pt>
@@ -1202,40 +1278,64 @@
                 <c:pt idx="26" formatCode="m/d/yy;@">
                   <c:v>43586</c:v>
                 </c:pt>
-                <c:pt idx="30" formatCode="m/d/yy;@">
-                  <c:v>43589</c:v>
-                </c:pt>
                 <c:pt idx="31" formatCode="m/d/yy;@">
-                  <c:v>0</c:v>
+                  <c:v>43590</c:v>
+                </c:pt>
+                <c:pt idx="33" formatCode="m/d/yy;@">
+                  <c:v>43590</c:v>
                 </c:pt>
                 <c:pt idx="35" formatCode="m/d/yy;@">
+                  <c:v>43590</c:v>
+                </c:pt>
+                <c:pt idx="37" formatCode="m/d/yy;@">
+                  <c:v>43591</c:v>
+                </c:pt>
+                <c:pt idx="39" formatCode="m/d/yy;@">
+                  <c:v>43591</c:v>
+                </c:pt>
+                <c:pt idx="41" formatCode="m/d/yy;@">
+                  <c:v>43592</c:v>
+                </c:pt>
+                <c:pt idx="43" formatCode="m/d/yy;@">
+                  <c:v>43594</c:v>
+                </c:pt>
+                <c:pt idx="45" formatCode="m/d/yy;@">
+                  <c:v>43594</c:v>
+                </c:pt>
+                <c:pt idx="47" formatCode="m/d/yy;@">
+                  <c:v>43594</c:v>
+                </c:pt>
+                <c:pt idx="49" formatCode="m/d/yy;@">
+                  <c:v>43594</c:v>
+                </c:pt>
+                <c:pt idx="51" formatCode="m/d/yy;@">
                   <c:v>43596</c:v>
                 </c:pt>
-                <c:pt idx="36" formatCode="m/d/yy;@">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="37" formatCode="m/d/yy;@">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="42" formatCode="m/d/yy;@">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="43" formatCode="m/d/yy;@">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="44" formatCode="m/d/yy;@">
+                <c:pt idx="52" formatCode="m/d/yy;@">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="53" formatCode="m/d/yy;@">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="58" formatCode="m/d/yy;@">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="59" formatCode="m/d/yy;@">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="60" formatCode="m/d/yy;@">
                   <c:v>43603</c:v>
                 </c:pt>
-                <c:pt idx="45" formatCode="m/d/yy;@">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="46" formatCode="m/d/yy;@">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="49" formatCode="m/d/yy;@">
+                <c:pt idx="61" formatCode="m/d/yy;@">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="62" formatCode="m/d/yy;@">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="65" formatCode="m/d/yy;@">
                   <c:v>43610</c:v>
                 </c:pt>
-                <c:pt idx="53" formatCode="m/d/yy;@">
+                <c:pt idx="69" formatCode="m/d/yy;@">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -1273,9 +1373,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:f>ProjectTimeline!$A$32:$B$86</c:f>
+              <c:f>ProjectTimeline!$A$32:$B$102</c:f>
               <c:multiLvlStrCache>
-                <c:ptCount val="50"/>
+                <c:ptCount val="66"/>
                 <c:lvl>
                   <c:pt idx="5">
                     <c:v>Responsibility Assignment Matrix</c:v>
@@ -1309,6 +1409,36 @@
                   </c:pt>
                   <c:pt idx="26">
                     <c:v>SRS Peer Review</c:v>
+                  </c:pt>
+                  <c:pt idx="31">
+                    <c:v>Udate Project Plan </c:v>
+                  </c:pt>
+                  <c:pt idx="33">
+                    <c:v>GUI</c:v>
+                  </c:pt>
+                  <c:pt idx="35">
+                    <c:v>HLD</c:v>
+                  </c:pt>
+                  <c:pt idx="37">
+                    <c:v>Data Flow Model</c:v>
+                  </c:pt>
+                  <c:pt idx="39">
+                    <c:v>Detailed Design </c:v>
+                  </c:pt>
+                  <c:pt idx="41">
+                    <c:v>Design Document </c:v>
+                  </c:pt>
+                  <c:pt idx="43">
+                    <c:v>Update Schedule</c:v>
+                  </c:pt>
+                  <c:pt idx="45">
+                    <c:v>Update RTM</c:v>
+                  </c:pt>
+                  <c:pt idx="47">
+                    <c:v>Update Responsibility Assignment</c:v>
+                  </c:pt>
+                  <c:pt idx="49">
+                    <c:v>Software Peer Review Sheet </c:v>
                   </c:pt>
                 </c:lvl>
                 <c:lvl>
@@ -1321,13 +1451,13 @@
                   <c:pt idx="30">
                     <c:v>Design</c:v>
                   </c:pt>
-                  <c:pt idx="35">
+                  <c:pt idx="51">
                     <c:v>Development</c:v>
                   </c:pt>
-                  <c:pt idx="44">
+                  <c:pt idx="60">
                     <c:v>Testing</c:v>
                   </c:pt>
-                  <c:pt idx="49">
+                  <c:pt idx="65">
                     <c:v>Delivery</c:v>
                   </c:pt>
                 </c:lvl>
@@ -1336,10 +1466,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>ProjectTimeline!$G$32:$G$86</c:f>
+              <c:f>ProjectTimeline!$G$32:$G$102</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="55"/>
+                <c:ptCount val="71"/>
                 <c:pt idx="5">
                   <c:v>5</c:v>
                 </c:pt>
@@ -1373,40 +1503,64 @@
                 <c:pt idx="26">
                   <c:v>0</c:v>
                 </c:pt>
-                <c:pt idx="30">
-                  <c:v>0</c:v>
-                </c:pt>
                 <c:pt idx="31">
                   <c:v>0</c:v>
                 </c:pt>
+                <c:pt idx="33">
+                  <c:v>0</c:v>
+                </c:pt>
                 <c:pt idx="35">
                   <c:v>0</c:v>
                 </c:pt>
-                <c:pt idx="36">
-                  <c:v>0</c:v>
-                </c:pt>
                 <c:pt idx="37">
                   <c:v>0</c:v>
                 </c:pt>
-                <c:pt idx="42">
+                <c:pt idx="39">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="41">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="43">
                   <c:v>0</c:v>
                 </c:pt>
-                <c:pt idx="44">
-                  <c:v>0</c:v>
-                </c:pt>
                 <c:pt idx="45">
                   <c:v>0</c:v>
                 </c:pt>
-                <c:pt idx="46">
+                <c:pt idx="47">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="49">
                   <c:v>0</c:v>
                 </c:pt>
+                <c:pt idx="51">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>0</c:v>
+                </c:pt>
                 <c:pt idx="53">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="69">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -1444,9 +1598,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:f>ProjectTimeline!$A$32:$B$86</c:f>
+              <c:f>ProjectTimeline!$A$32:$B$102</c:f>
               <c:multiLvlStrCache>
-                <c:ptCount val="50"/>
+                <c:ptCount val="66"/>
                 <c:lvl>
                   <c:pt idx="5">
                     <c:v>Responsibility Assignment Matrix</c:v>
@@ -1480,6 +1634,36 @@
                   </c:pt>
                   <c:pt idx="26">
                     <c:v>SRS Peer Review</c:v>
+                  </c:pt>
+                  <c:pt idx="31">
+                    <c:v>Udate Project Plan </c:v>
+                  </c:pt>
+                  <c:pt idx="33">
+                    <c:v>GUI</c:v>
+                  </c:pt>
+                  <c:pt idx="35">
+                    <c:v>HLD</c:v>
+                  </c:pt>
+                  <c:pt idx="37">
+                    <c:v>Data Flow Model</c:v>
+                  </c:pt>
+                  <c:pt idx="39">
+                    <c:v>Detailed Design </c:v>
+                  </c:pt>
+                  <c:pt idx="41">
+                    <c:v>Design Document </c:v>
+                  </c:pt>
+                  <c:pt idx="43">
+                    <c:v>Update Schedule</c:v>
+                  </c:pt>
+                  <c:pt idx="45">
+                    <c:v>Update RTM</c:v>
+                  </c:pt>
+                  <c:pt idx="47">
+                    <c:v>Update Responsibility Assignment</c:v>
+                  </c:pt>
+                  <c:pt idx="49">
+                    <c:v>Software Peer Review Sheet </c:v>
                   </c:pt>
                 </c:lvl>
                 <c:lvl>
@@ -1492,13 +1676,13 @@
                   <c:pt idx="30">
                     <c:v>Design</c:v>
                   </c:pt>
-                  <c:pt idx="35">
+                  <c:pt idx="51">
                     <c:v>Development</c:v>
                   </c:pt>
-                  <c:pt idx="44">
+                  <c:pt idx="60">
                     <c:v>Testing</c:v>
                   </c:pt>
-                  <c:pt idx="49">
+                  <c:pt idx="65">
                     <c:v>Delivery</c:v>
                   </c:pt>
                 </c:lvl>
@@ -1507,10 +1691,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>ProjectTimeline!$H$32:$H$86</c:f>
+              <c:f>ProjectTimeline!$H$32:$H$102</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="55"/>
+                <c:ptCount val="71"/>
                 <c:pt idx="5">
                   <c:v>0</c:v>
                 </c:pt>
@@ -1544,40 +1728,64 @@
                 <c:pt idx="26">
                   <c:v>2</c:v>
                 </c:pt>
-                <c:pt idx="30">
-                  <c:v>0</c:v>
-                </c:pt>
                 <c:pt idx="31">
                   <c:v>0</c:v>
                 </c:pt>
+                <c:pt idx="33">
+                  <c:v>0</c:v>
+                </c:pt>
                 <c:pt idx="35">
                   <c:v>0</c:v>
                 </c:pt>
-                <c:pt idx="36">
-                  <c:v>0</c:v>
-                </c:pt>
                 <c:pt idx="37">
                   <c:v>0</c:v>
                 </c:pt>
-                <c:pt idx="42">
+                <c:pt idx="39">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="41">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="43">
                   <c:v>0</c:v>
                 </c:pt>
-                <c:pt idx="44">
-                  <c:v>0</c:v>
-                </c:pt>
                 <c:pt idx="45">
                   <c:v>0</c:v>
                 </c:pt>
-                <c:pt idx="46">
+                <c:pt idx="47">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="49">
                   <c:v>0</c:v>
                 </c:pt>
+                <c:pt idx="51">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>0</c:v>
+                </c:pt>
                 <c:pt idx="53">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="69">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -1615,9 +1823,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:f>ProjectTimeline!$A$32:$B$86</c:f>
+              <c:f>ProjectTimeline!$A$32:$B$102</c:f>
               <c:multiLvlStrCache>
-                <c:ptCount val="50"/>
+                <c:ptCount val="66"/>
                 <c:lvl>
                   <c:pt idx="5">
                     <c:v>Responsibility Assignment Matrix</c:v>
@@ -1651,6 +1859,36 @@
                   </c:pt>
                   <c:pt idx="26">
                     <c:v>SRS Peer Review</c:v>
+                  </c:pt>
+                  <c:pt idx="31">
+                    <c:v>Udate Project Plan </c:v>
+                  </c:pt>
+                  <c:pt idx="33">
+                    <c:v>GUI</c:v>
+                  </c:pt>
+                  <c:pt idx="35">
+                    <c:v>HLD</c:v>
+                  </c:pt>
+                  <c:pt idx="37">
+                    <c:v>Data Flow Model</c:v>
+                  </c:pt>
+                  <c:pt idx="39">
+                    <c:v>Detailed Design </c:v>
+                  </c:pt>
+                  <c:pt idx="41">
+                    <c:v>Design Document </c:v>
+                  </c:pt>
+                  <c:pt idx="43">
+                    <c:v>Update Schedule</c:v>
+                  </c:pt>
+                  <c:pt idx="45">
+                    <c:v>Update RTM</c:v>
+                  </c:pt>
+                  <c:pt idx="47">
+                    <c:v>Update Responsibility Assignment</c:v>
+                  </c:pt>
+                  <c:pt idx="49">
+                    <c:v>Software Peer Review Sheet </c:v>
                   </c:pt>
                 </c:lvl>
                 <c:lvl>
@@ -1663,13 +1901,13 @@
                   <c:pt idx="30">
                     <c:v>Design</c:v>
                   </c:pt>
-                  <c:pt idx="35">
+                  <c:pt idx="51">
                     <c:v>Development</c:v>
                   </c:pt>
-                  <c:pt idx="44">
+                  <c:pt idx="60">
                     <c:v>Testing</c:v>
                   </c:pt>
-                  <c:pt idx="49">
+                  <c:pt idx="65">
                     <c:v>Delivery</c:v>
                   </c:pt>
                 </c:lvl>
@@ -1678,10 +1916,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>ProjectTimeline!$I$32:$I$86</c:f>
+              <c:f>ProjectTimeline!$I$32:$I$102</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="55"/>
+                <c:ptCount val="71"/>
                 <c:pt idx="5">
                   <c:v>0</c:v>
                 </c:pt>
@@ -1715,40 +1953,64 @@
                 <c:pt idx="26">
                   <c:v>0</c:v>
                 </c:pt>
-                <c:pt idx="30">
-                  <c:v>9</c:v>
-                </c:pt>
                 <c:pt idx="31">
-                  <c:v>0</c:v>
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>0</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>0</c:v>
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="49">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="52">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="53">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="69">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -1786,9 +2048,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:f>ProjectTimeline!$A$32:$B$86</c:f>
+              <c:f>ProjectTimeline!$A$32:$B$102</c:f>
               <c:multiLvlStrCache>
-                <c:ptCount val="50"/>
+                <c:ptCount val="66"/>
                 <c:lvl>
                   <c:pt idx="5">
                     <c:v>Responsibility Assignment Matrix</c:v>
@@ -1822,6 +2084,36 @@
                   </c:pt>
                   <c:pt idx="26">
                     <c:v>SRS Peer Review</c:v>
+                  </c:pt>
+                  <c:pt idx="31">
+                    <c:v>Udate Project Plan </c:v>
+                  </c:pt>
+                  <c:pt idx="33">
+                    <c:v>GUI</c:v>
+                  </c:pt>
+                  <c:pt idx="35">
+                    <c:v>HLD</c:v>
+                  </c:pt>
+                  <c:pt idx="37">
+                    <c:v>Data Flow Model</c:v>
+                  </c:pt>
+                  <c:pt idx="39">
+                    <c:v>Detailed Design </c:v>
+                  </c:pt>
+                  <c:pt idx="41">
+                    <c:v>Design Document </c:v>
+                  </c:pt>
+                  <c:pt idx="43">
+                    <c:v>Update Schedule</c:v>
+                  </c:pt>
+                  <c:pt idx="45">
+                    <c:v>Update RTM</c:v>
+                  </c:pt>
+                  <c:pt idx="47">
+                    <c:v>Update Responsibility Assignment</c:v>
+                  </c:pt>
+                  <c:pt idx="49">
+                    <c:v>Software Peer Review Sheet </c:v>
                   </c:pt>
                 </c:lvl>
                 <c:lvl>
@@ -1834,13 +2126,13 @@
                   <c:pt idx="30">
                     <c:v>Design</c:v>
                   </c:pt>
-                  <c:pt idx="35">
+                  <c:pt idx="51">
                     <c:v>Development</c:v>
                   </c:pt>
-                  <c:pt idx="44">
+                  <c:pt idx="60">
                     <c:v>Testing</c:v>
                   </c:pt>
-                  <c:pt idx="49">
+                  <c:pt idx="65">
                     <c:v>Delivery</c:v>
                   </c:pt>
                 </c:lvl>
@@ -1849,10 +2141,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>ProjectTimeline!$J$32:$J$86</c:f>
+              <c:f>ProjectTimeline!$J$32:$J$102</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="55"/>
+                <c:ptCount val="71"/>
                 <c:pt idx="5">
                   <c:v>0</c:v>
                 </c:pt>
@@ -1886,40 +2178,64 @@
                 <c:pt idx="26">
                   <c:v>0</c:v>
                 </c:pt>
-                <c:pt idx="30">
-                  <c:v>0</c:v>
-                </c:pt>
                 <c:pt idx="31">
                   <c:v>0</c:v>
                 </c:pt>
+                <c:pt idx="33">
+                  <c:v>0</c:v>
+                </c:pt>
                 <c:pt idx="35">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="51">
                   <c:v>10</c:v>
                 </c:pt>
-                <c:pt idx="36">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="49">
+                <c:pt idx="52">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="53">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="69">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -1957,9 +2273,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:f>ProjectTimeline!$A$32:$B$86</c:f>
+              <c:f>ProjectTimeline!$A$32:$B$102</c:f>
               <c:multiLvlStrCache>
-                <c:ptCount val="50"/>
+                <c:ptCount val="66"/>
                 <c:lvl>
                   <c:pt idx="5">
                     <c:v>Responsibility Assignment Matrix</c:v>
@@ -1993,6 +2309,36 @@
                   </c:pt>
                   <c:pt idx="26">
                     <c:v>SRS Peer Review</c:v>
+                  </c:pt>
+                  <c:pt idx="31">
+                    <c:v>Udate Project Plan </c:v>
+                  </c:pt>
+                  <c:pt idx="33">
+                    <c:v>GUI</c:v>
+                  </c:pt>
+                  <c:pt idx="35">
+                    <c:v>HLD</c:v>
+                  </c:pt>
+                  <c:pt idx="37">
+                    <c:v>Data Flow Model</c:v>
+                  </c:pt>
+                  <c:pt idx="39">
+                    <c:v>Detailed Design </c:v>
+                  </c:pt>
+                  <c:pt idx="41">
+                    <c:v>Design Document </c:v>
+                  </c:pt>
+                  <c:pt idx="43">
+                    <c:v>Update Schedule</c:v>
+                  </c:pt>
+                  <c:pt idx="45">
+                    <c:v>Update RTM</c:v>
+                  </c:pt>
+                  <c:pt idx="47">
+                    <c:v>Update Responsibility Assignment</c:v>
+                  </c:pt>
+                  <c:pt idx="49">
+                    <c:v>Software Peer Review Sheet </c:v>
                   </c:pt>
                 </c:lvl>
                 <c:lvl>
@@ -2005,13 +2351,13 @@
                   <c:pt idx="30">
                     <c:v>Design</c:v>
                   </c:pt>
-                  <c:pt idx="35">
+                  <c:pt idx="51">
                     <c:v>Development</c:v>
                   </c:pt>
-                  <c:pt idx="44">
+                  <c:pt idx="60">
                     <c:v>Testing</c:v>
                   </c:pt>
-                  <c:pt idx="49">
+                  <c:pt idx="65">
                     <c:v>Delivery</c:v>
                   </c:pt>
                 </c:lvl>
@@ -2020,10 +2366,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>ProjectTimeline!$K$32:$K$86</c:f>
+              <c:f>ProjectTimeline!$K$32:$K$102</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="55"/>
+                <c:ptCount val="71"/>
                 <c:pt idx="5">
                   <c:v>0</c:v>
                 </c:pt>
@@ -2057,40 +2403,64 @@
                 <c:pt idx="26">
                   <c:v>0</c:v>
                 </c:pt>
-                <c:pt idx="30">
-                  <c:v>0</c:v>
-                </c:pt>
                 <c:pt idx="31">
                   <c:v>0</c:v>
                 </c:pt>
+                <c:pt idx="33">
+                  <c:v>0</c:v>
+                </c:pt>
                 <c:pt idx="35">
                   <c:v>0</c:v>
                 </c:pt>
-                <c:pt idx="36">
-                  <c:v>0</c:v>
-                </c:pt>
                 <c:pt idx="37">
                   <c:v>0</c:v>
                 </c:pt>
-                <c:pt idx="42">
+                <c:pt idx="39">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="41">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="43">
                   <c:v>0</c:v>
                 </c:pt>
-                <c:pt idx="44">
-                  <c:v>0</c:v>
-                </c:pt>
                 <c:pt idx="45">
                   <c:v>0</c:v>
                 </c:pt>
-                <c:pt idx="46">
+                <c:pt idx="47">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="49">
                   <c:v>0</c:v>
                 </c:pt>
+                <c:pt idx="51">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>0</c:v>
+                </c:pt>
                 <c:pt idx="53">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="69">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -2128,9 +2498,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:f>ProjectTimeline!$A$32:$B$86</c:f>
+              <c:f>ProjectTimeline!$A$32:$B$102</c:f>
               <c:multiLvlStrCache>
-                <c:ptCount val="50"/>
+                <c:ptCount val="66"/>
                 <c:lvl>
                   <c:pt idx="5">
                     <c:v>Responsibility Assignment Matrix</c:v>
@@ -2164,6 +2534,36 @@
                   </c:pt>
                   <c:pt idx="26">
                     <c:v>SRS Peer Review</c:v>
+                  </c:pt>
+                  <c:pt idx="31">
+                    <c:v>Udate Project Plan </c:v>
+                  </c:pt>
+                  <c:pt idx="33">
+                    <c:v>GUI</c:v>
+                  </c:pt>
+                  <c:pt idx="35">
+                    <c:v>HLD</c:v>
+                  </c:pt>
+                  <c:pt idx="37">
+                    <c:v>Data Flow Model</c:v>
+                  </c:pt>
+                  <c:pt idx="39">
+                    <c:v>Detailed Design </c:v>
+                  </c:pt>
+                  <c:pt idx="41">
+                    <c:v>Design Document </c:v>
+                  </c:pt>
+                  <c:pt idx="43">
+                    <c:v>Update Schedule</c:v>
+                  </c:pt>
+                  <c:pt idx="45">
+                    <c:v>Update RTM</c:v>
+                  </c:pt>
+                  <c:pt idx="47">
+                    <c:v>Update Responsibility Assignment</c:v>
+                  </c:pt>
+                  <c:pt idx="49">
+                    <c:v>Software Peer Review Sheet </c:v>
                   </c:pt>
                 </c:lvl>
                 <c:lvl>
@@ -2176,13 +2576,13 @@
                   <c:pt idx="30">
                     <c:v>Design</c:v>
                   </c:pt>
-                  <c:pt idx="35">
+                  <c:pt idx="51">
                     <c:v>Development</c:v>
                   </c:pt>
-                  <c:pt idx="44">
+                  <c:pt idx="60">
                     <c:v>Testing</c:v>
                   </c:pt>
-                  <c:pt idx="49">
+                  <c:pt idx="65">
                     <c:v>Delivery</c:v>
                   </c:pt>
                 </c:lvl>
@@ -2191,10 +2591,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>ProjectTimeline!$L$32:$L$86</c:f>
+              <c:f>ProjectTimeline!$L$32:$L$102</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="55"/>
+                <c:ptCount val="71"/>
                 <c:pt idx="5">
                   <c:v>0</c:v>
                 </c:pt>
@@ -2228,40 +2628,64 @@
                 <c:pt idx="26">
                   <c:v>0</c:v>
                 </c:pt>
-                <c:pt idx="30">
-                  <c:v>0</c:v>
-                </c:pt>
                 <c:pt idx="31">
                   <c:v>0</c:v>
                 </c:pt>
+                <c:pt idx="33">
+                  <c:v>0</c:v>
+                </c:pt>
                 <c:pt idx="35">
                   <c:v>0</c:v>
                 </c:pt>
-                <c:pt idx="36">
-                  <c:v>0</c:v>
-                </c:pt>
                 <c:pt idx="37">
                   <c:v>0</c:v>
                 </c:pt>
-                <c:pt idx="42">
+                <c:pt idx="39">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="41">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="43">
                   <c:v>0</c:v>
                 </c:pt>
-                <c:pt idx="44">
+                <c:pt idx="45">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="60">
                   <c:v>11</c:v>
                 </c:pt>
-                <c:pt idx="45">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="53">
+                <c:pt idx="61">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="69">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -2283,8 +2707,8 @@
         </c:dLbls>
         <c:gapWidth val="20"/>
         <c:overlap val="100"/>
-        <c:axId val="490438736"/>
-        <c:axId val="490434928"/>
+        <c:axId val="-1614170272"/>
+        <c:axId val="-1614175168"/>
       </c:barChart>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
@@ -2294,7 +2718,7 @@
           <c:order val="7"/>
           <c:tx>
             <c:strRef>
-              <c:f>ProjectTimeline!$B$91</c:f>
+              <c:f>ProjectTimeline!$B$107</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2385,7 +2809,7 @@
           </c:dLbls>
           <c:xVal>
             <c:numRef>
-              <c:f>(ProjectTimeline!$C$91,ProjectTimeline!$C$91)</c:f>
+              <c:f>(ProjectTimeline!$C$107,ProjectTimeline!$C$107)</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy;@</c:formatCode>
                 <c:ptCount val="2"/>
@@ -2400,7 +2824,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>ProjectTimeline!$D$91:$E$91</c:f>
+              <c:f>ProjectTimeline!$D$107:$E$107</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="2"/>
@@ -2425,7 +2849,7 @@
           <c:order val="8"/>
           <c:tx>
             <c:strRef>
-              <c:f>ProjectTimeline!$B$92</c:f>
+              <c:f>ProjectTimeline!$B$108</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2540,7 +2964,7 @@
           </c:dLbls>
           <c:xVal>
             <c:numRef>
-              <c:f>(ProjectTimeline!$C$92,ProjectTimeline!$C$92)</c:f>
+              <c:f>(ProjectTimeline!$C$108,ProjectTimeline!$C$108)</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy;@</c:formatCode>
                 <c:ptCount val="2"/>
@@ -2555,7 +2979,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>ProjectTimeline!$D$92:$E$92</c:f>
+              <c:f>ProjectTimeline!$D$108:$E$108</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="2"/>
@@ -2580,7 +3004,7 @@
           <c:order val="9"/>
           <c:tx>
             <c:strRef>
-              <c:f>ProjectTimeline!$B$93</c:f>
+              <c:f>ProjectTimeline!$B$109</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2671,7 +3095,7 @@
           </c:dLbls>
           <c:xVal>
             <c:numRef>
-              <c:f>(ProjectTimeline!$C$93,ProjectTimeline!$C$93)</c:f>
+              <c:f>(ProjectTimeline!$C$109,ProjectTimeline!$C$109)</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy;@</c:formatCode>
                 <c:ptCount val="2"/>
@@ -2686,7 +3110,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>ProjectTimeline!$D$93:$E$93</c:f>
+              <c:f>ProjectTimeline!$D$109:$E$109</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="2"/>
@@ -2711,7 +3135,7 @@
           <c:order val="10"/>
           <c:tx>
             <c:strRef>
-              <c:f>ProjectTimeline!$B$94</c:f>
+              <c:f>ProjectTimeline!$B$110</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2802,7 +3226,7 @@
           </c:dLbls>
           <c:xVal>
             <c:numRef>
-              <c:f>(ProjectTimeline!$C$94,ProjectTimeline!$C$94)</c:f>
+              <c:f>(ProjectTimeline!$C$110,ProjectTimeline!$C$110)</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy;@</c:formatCode>
                 <c:ptCount val="2"/>
@@ -2817,7 +3241,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>ProjectTimeline!$D$94:$E$94</c:f>
+              <c:f>ProjectTimeline!$D$110:$E$110</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="2"/>
@@ -2845,11 +3269,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="490436016"/>
-        <c:axId val="490435472"/>
+        <c:axId val="-1614175712"/>
+        <c:axId val="-1614162656"/>
       </c:scatterChart>
       <c:catAx>
-        <c:axId val="490438736"/>
+        <c:axId val="-1614170272"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -2906,7 +3330,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="490434928"/>
+        <c:crossAx val="-1614175168"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2916,7 +3340,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="490434928"/>
+        <c:axId val="-1614175168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="43646"/>
@@ -2975,13 +3399,13 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="490438736"/>
+        <c:crossAx val="-1614170272"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="30"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="490435472"/>
+        <c:axId val="-1614162656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -2992,13 +3416,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="490436016"/>
+        <c:crossAx val="-1614175712"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="1"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="490436016"/>
+        <c:axId val="-1614175712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3008,7 +3432,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="490435472"/>
+        <c:crossAx val="-1614162656"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4011,10 +4435,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:O94"/>
+  <dimension ref="A1:O110"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A57" zoomScaleNormal="100" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="C81" sqref="C81"/>
+    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A61" zoomScaleNormal="100" zoomScalePageLayoutView="85" workbookViewId="0">
+      <selection activeCell="M81" sqref="M81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -4206,11 +4630,11 @@
         <v>21</v>
       </c>
       <c r="F37" s="64">
-        <f t="shared" ref="F37:F78" si="0">IF(ISBLANK(C37),0,C37)</f>
+        <f t="shared" ref="F37:F94" si="0">IF(ISBLANK(C37),0,C37)</f>
         <v>43582</v>
       </c>
       <c r="G37" s="65">
-        <f t="shared" ref="G37:L85" si="1">IF(ISBLANK($D37),0,IF($E37=G$31,$D37-$C37+1,0))</f>
+        <f t="shared" ref="G37:L101" si="1">IF(ISBLANK($D37),0,IF($E37=G$31,$D37-$C37+1,0))</f>
         <v>5</v>
       </c>
       <c r="H37" s="65">
@@ -4898,56 +5322,35 @@
         <v>58</v>
       </c>
       <c r="B62" s="31"/>
-      <c r="C62" s="32">
-        <v>43589</v>
-      </c>
-      <c r="D62" s="33">
-        <v>43597</v>
-      </c>
-      <c r="E62" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="F62" s="64">
-        <f t="shared" si="0"/>
-        <v>43589</v>
-      </c>
-      <c r="G62" s="65">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="H62" s="65">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="I62" s="65">
-        <f>IF(ISBLANK($D62),0,IF($E62=I$31,$D62-$C62+1,0))</f>
-        <v>9</v>
-      </c>
-      <c r="J62" s="65">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="K62" s="65">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="L62" s="66">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
+      <c r="C62" s="32"/>
+      <c r="D62" s="33"/>
+      <c r="E62" s="12"/>
+      <c r="F62" s="64"/>
+      <c r="G62" s="65"/>
+      <c r="H62" s="65"/>
+      <c r="I62" s="65"/>
+      <c r="J62" s="65"/>
+      <c r="K62" s="65"/>
+      <c r="L62" s="66"/>
       <c r="M62" s="66"/>
     </row>
     <row r="63" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A63" s="30"/>
-      <c r="B63" s="31"/>
-      <c r="C63" s="32"/>
-      <c r="D63" s="33"/>
+      <c r="B63" s="31" t="s">
+        <v>90</v>
+      </c>
+      <c r="C63" s="32">
+        <v>43590</v>
+      </c>
+      <c r="D63" s="33">
+        <v>43593</v>
+      </c>
       <c r="E63" s="12" t="s">
         <v>20</v>
       </c>
       <c r="F63" s="64">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>43590</v>
       </c>
       <c r="G63" s="65">
         <f t="shared" si="1"/>
@@ -4959,7 +5362,7 @@
       </c>
       <c r="I63" s="65">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="J63" s="65">
         <f t="shared" si="1"/>
@@ -4973,7 +5376,9 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="M63" s="66"/>
+      <c r="M63" s="66" t="s">
+        <v>78</v>
+      </c>
     </row>
     <row r="64" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A64" s="30"/>
@@ -4992,18 +5397,42 @@
     </row>
     <row r="65" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A65" s="30"/>
-      <c r="B65" s="31"/>
-      <c r="C65" s="32"/>
-      <c r="D65" s="33"/>
-      <c r="E65" s="12"/>
-      <c r="F65" s="64"/>
-      <c r="G65" s="65"/>
-      <c r="H65" s="65"/>
-      <c r="I65" s="65"/>
-      <c r="J65" s="65"/>
-      <c r="K65" s="65"/>
-      <c r="L65" s="66"/>
-      <c r="M65" s="66"/>
+      <c r="B65" s="31" t="s">
+        <v>89</v>
+      </c>
+      <c r="C65" s="32">
+        <v>43590</v>
+      </c>
+      <c r="D65" s="33">
+        <v>43594</v>
+      </c>
+      <c r="E65" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="F65" s="64">
+        <v>43590</v>
+      </c>
+      <c r="G65" s="65">
+        <v>0</v>
+      </c>
+      <c r="H65" s="65">
+        <v>0</v>
+      </c>
+      <c r="I65" s="65">
+        <v>5</v>
+      </c>
+      <c r="J65" s="65">
+        <v>0</v>
+      </c>
+      <c r="K65" s="65">
+        <v>0</v>
+      </c>
+      <c r="L65" s="66">
+        <v>0</v>
+      </c>
+      <c r="M65" s="66" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="66" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A66" s="30"/>
@@ -5021,22 +5450,22 @@
       <c r="M66" s="66"/>
     </row>
     <row r="67" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A67" s="30" t="s">
-        <v>61</v>
-      </c>
-      <c r="B67" s="31"/>
+      <c r="A67" s="30"/>
+      <c r="B67" s="31" t="s">
+        <v>88</v>
+      </c>
       <c r="C67" s="32">
-        <v>43596</v>
+        <v>43590</v>
       </c>
       <c r="D67" s="33">
-        <v>43605</v>
+        <v>43594</v>
       </c>
       <c r="E67" s="12" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="F67" s="64">
-        <f t="shared" si="0"/>
-        <v>43596</v>
+        <f t="shared" ref="F67" si="2">IF(ISBLANK(C67),0,C67)</f>
+        <v>43590</v>
       </c>
       <c r="G67" s="65">
         <f t="shared" si="1"/>
@@ -5048,11 +5477,11 @@
       </c>
       <c r="I67" s="65">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="J67" s="65">
         <f t="shared" si="1"/>
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="K67" s="65">
         <f t="shared" si="1"/>
@@ -5062,83 +5491,63 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="M67" s="66"/>
+      <c r="M67" s="66" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="68" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A68" s="30"/>
       <c r="B68" s="31"/>
       <c r="C68" s="32"/>
       <c r="D68" s="33"/>
-      <c r="E68" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="F68" s="64">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G68" s="65">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="H68" s="65">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="I68" s="65">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J68" s="65">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="K68" s="65">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="L68" s="66">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
+      <c r="E68" s="12"/>
+      <c r="F68" s="64"/>
+      <c r="G68" s="65"/>
+      <c r="H68" s="65"/>
+      <c r="I68" s="65"/>
+      <c r="J68" s="65"/>
+      <c r="K68" s="65"/>
+      <c r="L68" s="66"/>
       <c r="M68" s="66"/>
     </row>
     <row r="69" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A69" s="30"/>
-      <c r="B69" s="31"/>
-      <c r="C69" s="32"/>
-      <c r="D69" s="33"/>
+      <c r="B69" s="31" t="s">
+        <v>93</v>
+      </c>
+      <c r="C69" s="32">
+        <v>43591</v>
+      </c>
+      <c r="D69" s="33">
+        <v>43594</v>
+      </c>
       <c r="E69" s="12" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="F69" s="64">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <v>43591</v>
       </c>
       <c r="G69" s="65">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H69" s="65">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="I69" s="65">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="J69" s="65">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K69" s="65">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="L69" s="66">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="M69" s="66"/>
+        <v>0</v>
+      </c>
+      <c r="M69" s="66" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="70" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A70" s="30"/>
@@ -5157,18 +5566,42 @@
     </row>
     <row r="71" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A71" s="30"/>
-      <c r="B71" s="31"/>
-      <c r="C71" s="32"/>
-      <c r="D71" s="33"/>
-      <c r="E71" s="12"/>
-      <c r="F71" s="64"/>
-      <c r="G71" s="65"/>
-      <c r="H71" s="65"/>
-      <c r="I71" s="65"/>
-      <c r="J71" s="65"/>
-      <c r="K71" s="65"/>
-      <c r="L71" s="66"/>
-      <c r="M71" s="66"/>
+      <c r="B71" s="31" t="s">
+        <v>91</v>
+      </c>
+      <c r="C71" s="32">
+        <v>43591</v>
+      </c>
+      <c r="D71" s="33">
+        <v>43594</v>
+      </c>
+      <c r="E71" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="F71" s="64">
+        <v>43591</v>
+      </c>
+      <c r="G71" s="65">
+        <v>0</v>
+      </c>
+      <c r="H71" s="65">
+        <v>0</v>
+      </c>
+      <c r="I71" s="65">
+        <v>4</v>
+      </c>
+      <c r="J71" s="65">
+        <v>0</v>
+      </c>
+      <c r="K71" s="65">
+        <v>0</v>
+      </c>
+      <c r="L71" s="66">
+        <v>0</v>
+      </c>
+      <c r="M71" s="66" t="s">
+        <v>92</v>
+      </c>
     </row>
     <row r="72" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A72" s="30"/>
@@ -5187,68 +5620,75 @@
     </row>
     <row r="73" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A73" s="30"/>
-      <c r="B73" s="31"/>
-      <c r="C73" s="32"/>
-      <c r="D73" s="33"/>
-      <c r="E73" s="12"/>
-      <c r="F73" s="64"/>
-      <c r="G73" s="65"/>
-      <c r="H73" s="65"/>
-      <c r="I73" s="65"/>
-      <c r="J73" s="65"/>
-      <c r="K73" s="65"/>
-      <c r="L73" s="66"/>
-      <c r="M73" s="66"/>
+      <c r="B73" s="31" t="s">
+        <v>94</v>
+      </c>
+      <c r="C73" s="32">
+        <v>43592</v>
+      </c>
+      <c r="D73" s="33">
+        <v>43595</v>
+      </c>
+      <c r="E73" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="F73" s="64">
+        <v>43592</v>
+      </c>
+      <c r="G73" s="65">
+        <v>0</v>
+      </c>
+      <c r="H73" s="65">
+        <v>0</v>
+      </c>
+      <c r="I73" s="65">
+        <v>4</v>
+      </c>
+      <c r="J73" s="65">
+        <v>0</v>
+      </c>
+      <c r="K73" s="65">
+        <v>0</v>
+      </c>
+      <c r="L73" s="66">
+        <v>0</v>
+      </c>
+      <c r="M73" s="66" t="s">
+        <v>92</v>
+      </c>
     </row>
     <row r="74" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A74" s="30"/>
       <c r="B74" s="31"/>
       <c r="C74" s="32"/>
       <c r="D74" s="33"/>
-      <c r="E74" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="F74" s="64">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G74" s="65">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="H74" s="65">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="I74" s="65">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J74" s="65">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="K74" s="65">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="L74" s="66">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
+      <c r="E74" s="12"/>
+      <c r="F74" s="64"/>
+      <c r="G74" s="65"/>
+      <c r="H74" s="65"/>
+      <c r="I74" s="65"/>
+      <c r="J74" s="65"/>
+      <c r="K74" s="65"/>
+      <c r="L74" s="66"/>
       <c r="M74" s="66"/>
     </row>
     <row r="75" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A75" s="30"/>
-      <c r="B75" s="31"/>
-      <c r="C75" s="32"/>
-      <c r="D75" s="33"/>
+      <c r="B75" s="31" t="s">
+        <v>96</v>
+      </c>
+      <c r="C75" s="32">
+        <v>43594</v>
+      </c>
+      <c r="D75" s="33">
+        <v>43594</v>
+      </c>
       <c r="E75" s="12" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="F75" s="64">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f>IF(ISBLANK(C75),0,C75)</f>
+        <v>43594</v>
       </c>
       <c r="G75" s="65">
         <f t="shared" si="1"/>
@@ -5259,8 +5699,7 @@
         <v>0</v>
       </c>
       <c r="I75" s="65">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J75" s="65">
         <f t="shared" si="1"/>
@@ -5274,151 +5713,124 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="M75" s="66"/>
+      <c r="M75" s="66" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="76" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A76" s="30" t="s">
-        <v>62</v>
-      </c>
+      <c r="A76" s="30"/>
       <c r="B76" s="31"/>
-      <c r="C76" s="32">
-        <v>43603</v>
-      </c>
-      <c r="D76" s="33">
-        <v>43613</v>
-      </c>
-      <c r="E76" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="F76" s="64">
-        <f>IF(ISBLANK(C76),0,C76)</f>
-        <v>43603</v>
-      </c>
-      <c r="G76" s="65">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="H76" s="65">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="I76" s="65">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J76" s="65">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="K76" s="65">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="L76" s="66">
-        <f t="shared" si="1"/>
-        <v>11</v>
-      </c>
+      <c r="C76" s="32"/>
+      <c r="D76" s="33"/>
+      <c r="E76" s="12"/>
+      <c r="F76" s="64"/>
+      <c r="G76" s="65"/>
+      <c r="H76" s="65"/>
+      <c r="I76" s="65"/>
+      <c r="J76" s="65"/>
+      <c r="K76" s="65"/>
+      <c r="L76" s="66"/>
       <c r="M76" s="66"/>
     </row>
     <row r="77" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A77" s="30"/>
-      <c r="B77" s="31"/>
-      <c r="C77" s="32"/>
-      <c r="D77" s="33"/>
+      <c r="B77" s="31" t="s">
+        <v>97</v>
+      </c>
+      <c r="C77" s="32">
+        <v>43594</v>
+      </c>
+      <c r="D77" s="33">
+        <v>43595</v>
+      </c>
       <c r="E77" s="12" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F77" s="64">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <v>43594</v>
       </c>
       <c r="G77" s="65">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H77" s="65">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="I77" s="65">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J77" s="65">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K77" s="65">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="L77" s="66">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="M77" s="66"/>
+        <v>0</v>
+      </c>
+      <c r="M77" s="66" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="78" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A78" s="30"/>
       <c r="B78" s="31"/>
       <c r="C78" s="32"/>
       <c r="D78" s="33"/>
-      <c r="E78" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="F78" s="64">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G78" s="65">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="H78" s="65">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="I78" s="65">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J78" s="65">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="K78" s="65">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="L78" s="66">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
+      <c r="E78" s="12"/>
+      <c r="F78" s="64"/>
+      <c r="G78" s="65"/>
+      <c r="H78" s="65"/>
+      <c r="I78" s="65"/>
+      <c r="J78" s="65"/>
+      <c r="K78" s="65"/>
+      <c r="L78" s="66"/>
       <c r="M78" s="66"/>
     </row>
     <row r="79" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A79" s="30"/>
-      <c r="B79" s="31"/>
-      <c r="C79" s="32"/>
-      <c r="D79" s="33"/>
-      <c r="E79" s="12"/>
-      <c r="F79" s="64"/>
-      <c r="G79" s="65"/>
-      <c r="H79" s="65"/>
-      <c r="I79" s="65"/>
-      <c r="J79" s="65"/>
-      <c r="K79" s="65"/>
-      <c r="L79" s="66"/>
-      <c r="M79" s="66"/>
+      <c r="B79" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="C79" s="32">
+        <v>43594</v>
+      </c>
+      <c r="D79" s="33">
+        <v>43594</v>
+      </c>
+      <c r="E79" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="F79" s="64">
+        <v>43594</v>
+      </c>
+      <c r="G79" s="65">
+        <v>0</v>
+      </c>
+      <c r="H79" s="65">
+        <v>0</v>
+      </c>
+      <c r="I79" s="65">
+        <v>1</v>
+      </c>
+      <c r="J79" s="65">
+        <v>0</v>
+      </c>
+      <c r="K79" s="65">
+        <v>0</v>
+      </c>
+      <c r="L79" s="66">
+        <v>0</v>
+      </c>
+      <c r="M79" s="66" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="80" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A80" s="30"/>
       <c r="B80" s="31"/>
       <c r="C80" s="32"/>
       <c r="D80" s="33"/>
-      <c r="E80" s="12" t="s">
-        <v>22</v>
-      </c>
+      <c r="E80" s="12"/>
       <c r="F80" s="64"/>
       <c r="G80" s="65"/>
       <c r="H80" s="65"/>
@@ -5428,58 +5840,51 @@
       <c r="L80" s="66"/>
       <c r="M80" s="66"/>
     </row>
-    <row r="81" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A81" s="30" t="s">
-        <v>84</v>
-      </c>
-      <c r="B81" s="31"/>
+    <row r="81" spans="1:13" s="7" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="A81" s="30"/>
+      <c r="B81" s="31" t="s">
+        <v>98</v>
+      </c>
       <c r="C81" s="32">
-        <v>43610</v>
+        <v>43594</v>
       </c>
       <c r="D81" s="33">
-        <v>43613</v>
+        <v>43595</v>
       </c>
       <c r="E81" s="12" t="s">
-        <v>83</v>
+        <v>20</v>
       </c>
       <c r="F81" s="64">
-        <f t="shared" ref="F81" si="2">IF(ISBLANK(C81),0,C81)</f>
-        <v>43610</v>
+        <v>43594</v>
       </c>
       <c r="G81" s="65">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H81" s="65">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="I81" s="65">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J81" s="65">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K81" s="65">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="L81" s="66">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="M81" s="66"/>
+        <v>0</v>
+      </c>
+      <c r="M81" s="69" t="s">
+        <v>100</v>
+      </c>
     </row>
     <row r="82" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A82" s="30"/>
       <c r="B82" s="31"/>
       <c r="C82" s="32"/>
       <c r="D82" s="33"/>
-      <c r="E82" s="12" t="s">
-        <v>83</v>
-      </c>
+      <c r="E82" s="12"/>
       <c r="F82" s="64"/>
       <c r="G82" s="65"/>
       <c r="H82" s="65"/>
@@ -5490,20 +5895,47 @@
       <c r="M82" s="66"/>
     </row>
     <row r="83" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A83" s="30"/>
+      <c r="A83" s="30" t="s">
+        <v>61</v>
+      </c>
       <c r="B83" s="31"/>
-      <c r="C83" s="32"/>
-      <c r="D83" s="33"/>
+      <c r="C83" s="32">
+        <v>43596</v>
+      </c>
+      <c r="D83" s="33">
+        <v>43605</v>
+      </c>
       <c r="E83" s="12" t="s">
-        <v>83</v>
-      </c>
-      <c r="F83" s="64"/>
-      <c r="G83" s="65"/>
-      <c r="H83" s="65"/>
-      <c r="I83" s="65"/>
-      <c r="J83" s="65"/>
-      <c r="K83" s="65"/>
-      <c r="L83" s="66"/>
+        <v>24</v>
+      </c>
+      <c r="F83" s="64">
+        <f t="shared" si="0"/>
+        <v>43596</v>
+      </c>
+      <c r="G83" s="65">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H83" s="65">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I83" s="65">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J83" s="65">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="K83" s="65">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L83" s="66">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="M83" s="66"/>
     </row>
     <row r="84" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
@@ -5512,15 +5944,36 @@
       <c r="C84" s="32"/>
       <c r="D84" s="33"/>
       <c r="E84" s="12" t="s">
-        <v>83</v>
-      </c>
-      <c r="F84" s="64"/>
-      <c r="G84" s="65"/>
-      <c r="H84" s="65"/>
-      <c r="I84" s="65"/>
-      <c r="J84" s="65"/>
-      <c r="K84" s="65"/>
-      <c r="L84" s="66"/>
+        <v>24</v>
+      </c>
+      <c r="F84" s="64">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G84" s="65">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H84" s="65">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I84" s="65">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J84" s="65">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K84" s="65">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L84" s="66">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="M84" s="66"/>
     </row>
     <row r="85" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
@@ -5529,128 +5982,549 @@
       <c r="C85" s="32"/>
       <c r="D85" s="33"/>
       <c r="E85" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="F85" s="64">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G85" s="65">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H85" s="65">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I85" s="65">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J85" s="65">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K85" s="65">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L85" s="66">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M85" s="66"/>
+    </row>
+    <row r="86" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A86" s="30"/>
+      <c r="B86" s="31"/>
+      <c r="C86" s="32"/>
+      <c r="D86" s="33"/>
+      <c r="E86" s="12"/>
+      <c r="F86" s="64"/>
+      <c r="G86" s="65"/>
+      <c r="H86" s="65"/>
+      <c r="I86" s="65"/>
+      <c r="J86" s="65"/>
+      <c r="K86" s="65"/>
+      <c r="L86" s="66"/>
+      <c r="M86" s="66"/>
+    </row>
+    <row r="87" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A87" s="30"/>
+      <c r="B87" s="31"/>
+      <c r="C87" s="32"/>
+      <c r="D87" s="33"/>
+      <c r="E87" s="12"/>
+      <c r="F87" s="64"/>
+      <c r="G87" s="65"/>
+      <c r="H87" s="65"/>
+      <c r="I87" s="65"/>
+      <c r="J87" s="65"/>
+      <c r="K87" s="65"/>
+      <c r="L87" s="66"/>
+      <c r="M87" s="66"/>
+    </row>
+    <row r="88" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A88" s="30"/>
+      <c r="B88" s="31"/>
+      <c r="C88" s="32"/>
+      <c r="D88" s="33"/>
+      <c r="E88" s="12"/>
+      <c r="F88" s="64"/>
+      <c r="G88" s="65"/>
+      <c r="H88" s="65"/>
+      <c r="I88" s="65"/>
+      <c r="J88" s="65"/>
+      <c r="K88" s="65"/>
+      <c r="L88" s="66"/>
+      <c r="M88" s="66"/>
+    </row>
+    <row r="89" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A89" s="30"/>
+      <c r="B89" s="31"/>
+      <c r="C89" s="32"/>
+      <c r="D89" s="33"/>
+      <c r="E89" s="12"/>
+      <c r="F89" s="64"/>
+      <c r="G89" s="65"/>
+      <c r="H89" s="65"/>
+      <c r="I89" s="65"/>
+      <c r="J89" s="65"/>
+      <c r="K89" s="65"/>
+      <c r="L89" s="66"/>
+      <c r="M89" s="66"/>
+    </row>
+    <row r="90" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A90" s="30"/>
+      <c r="B90" s="31"/>
+      <c r="C90" s="32"/>
+      <c r="D90" s="33"/>
+      <c r="E90" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="F90" s="64">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G90" s="65">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H90" s="65">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I90" s="65">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J90" s="65">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K90" s="65">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L90" s="66">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M90" s="66"/>
+    </row>
+    <row r="91" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A91" s="30"/>
+      <c r="B91" s="31"/>
+      <c r="C91" s="32"/>
+      <c r="D91" s="33"/>
+      <c r="E91" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="F91" s="64">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G91" s="65">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H91" s="65">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I91" s="65">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J91" s="65">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K91" s="65">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L91" s="66">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M91" s="66"/>
+    </row>
+    <row r="92" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A92" s="30" t="s">
+        <v>62</v>
+      </c>
+      <c r="B92" s="31"/>
+      <c r="C92" s="32">
+        <v>43603</v>
+      </c>
+      <c r="D92" s="33">
+        <v>43613</v>
+      </c>
+      <c r="E92" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="F92" s="64">
+        <f>IF(ISBLANK(C92),0,C92)</f>
+        <v>43603</v>
+      </c>
+      <c r="G92" s="65">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H92" s="65">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I92" s="65">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J92" s="65">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K92" s="65">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L92" s="66">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+      <c r="M92" s="66"/>
+    </row>
+    <row r="93" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A93" s="30"/>
+      <c r="B93" s="31"/>
+      <c r="C93" s="32"/>
+      <c r="D93" s="33"/>
+      <c r="E93" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="F93" s="64">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G93" s="65">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H93" s="65">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I93" s="65">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J93" s="65">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K93" s="65">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L93" s="66">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M93" s="66"/>
+    </row>
+    <row r="94" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A94" s="30"/>
+      <c r="B94" s="31"/>
+      <c r="C94" s="32"/>
+      <c r="D94" s="33"/>
+      <c r="E94" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="F94" s="64">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G94" s="65">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H94" s="65">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I94" s="65">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J94" s="65">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K94" s="65">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L94" s="66">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M94" s="66"/>
+    </row>
+    <row r="95" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A95" s="30"/>
+      <c r="B95" s="31"/>
+      <c r="C95" s="32"/>
+      <c r="D95" s="33"/>
+      <c r="E95" s="12"/>
+      <c r="F95" s="64"/>
+      <c r="G95" s="65"/>
+      <c r="H95" s="65"/>
+      <c r="I95" s="65"/>
+      <c r="J95" s="65"/>
+      <c r="K95" s="65"/>
+      <c r="L95" s="66"/>
+      <c r="M95" s="66"/>
+    </row>
+    <row r="96" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A96" s="30"/>
+      <c r="B96" s="31"/>
+      <c r="C96" s="32"/>
+      <c r="D96" s="33"/>
+      <c r="E96" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="F96" s="64"/>
+      <c r="G96" s="65"/>
+      <c r="H96" s="65"/>
+      <c r="I96" s="65"/>
+      <c r="J96" s="65"/>
+      <c r="K96" s="65"/>
+      <c r="L96" s="66"/>
+      <c r="M96" s="66"/>
+    </row>
+    <row r="97" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A97" s="30" t="s">
+        <v>84</v>
+      </c>
+      <c r="B97" s="31"/>
+      <c r="C97" s="32">
+        <v>43610</v>
+      </c>
+      <c r="D97" s="33">
+        <v>43613</v>
+      </c>
+      <c r="E97" s="12" t="s">
         <v>83</v>
       </c>
-      <c r="F85" s="64">
-        <f>IF(ISBLANK(C85),0,C85)</f>
-        <v>0</v>
-      </c>
-      <c r="G85" s="65">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="H85" s="65">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="I85" s="65">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J85" s="65">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="K85" s="65">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="L85" s="66">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="M85" s="66"/>
-    </row>
-    <row r="86" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A86" s="24"/>
-      <c r="B86" s="25"/>
-      <c r="C86" s="26" t="s">
+      <c r="F97" s="64">
+        <f t="shared" ref="F97" si="3">IF(ISBLANK(C97),0,C97)</f>
+        <v>43610</v>
+      </c>
+      <c r="G97" s="65">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H97" s="65">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I97" s="65">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J97" s="65">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K97" s="65">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L97" s="66">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M97" s="66"/>
+    </row>
+    <row r="98" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A98" s="30"/>
+      <c r="B98" s="31"/>
+      <c r="C98" s="32"/>
+      <c r="D98" s="33"/>
+      <c r="E98" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="F98" s="64"/>
+      <c r="G98" s="65"/>
+      <c r="H98" s="65"/>
+      <c r="I98" s="65"/>
+      <c r="J98" s="65"/>
+      <c r="K98" s="65"/>
+      <c r="L98" s="66"/>
+      <c r="M98" s="66"/>
+    </row>
+    <row r="99" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A99" s="30"/>
+      <c r="B99" s="31"/>
+      <c r="C99" s="32"/>
+      <c r="D99" s="33"/>
+      <c r="E99" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="F99" s="64"/>
+      <c r="G99" s="65"/>
+      <c r="H99" s="65"/>
+      <c r="I99" s="65"/>
+      <c r="J99" s="65"/>
+      <c r="K99" s="65"/>
+      <c r="L99" s="66"/>
+      <c r="M99" s="66"/>
+    </row>
+    <row r="100" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A100" s="30"/>
+      <c r="B100" s="31"/>
+      <c r="C100" s="32"/>
+      <c r="D100" s="33"/>
+      <c r="E100" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="F100" s="64"/>
+      <c r="G100" s="65"/>
+      <c r="H100" s="65"/>
+      <c r="I100" s="65"/>
+      <c r="J100" s="65"/>
+      <c r="K100" s="65"/>
+      <c r="L100" s="66"/>
+      <c r="M100" s="66"/>
+    </row>
+    <row r="101" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A101" s="30"/>
+      <c r="B101" s="31"/>
+      <c r="C101" s="32"/>
+      <c r="D101" s="33"/>
+      <c r="E101" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="F101" s="64">
+        <f>IF(ISBLANK(C101),0,C101)</f>
+        <v>0</v>
+      </c>
+      <c r="G101" s="65">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H101" s="65">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I101" s="65">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J101" s="65">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K101" s="65">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L101" s="66">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M101" s="66"/>
+    </row>
+    <row r="102" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A102" s="24"/>
+      <c r="B102" s="25"/>
+      <c r="C102" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="D86" s="27"/>
-      <c r="E86" s="27"/>
-      <c r="F86" s="28"/>
-      <c r="G86" s="28"/>
-      <c r="H86" s="28"/>
-      <c r="I86" s="28"/>
-      <c r="J86" s="28"/>
-      <c r="K86" s="28"/>
-      <c r="L86" s="29"/>
-      <c r="M86" s="29"/>
-    </row>
-    <row r="90" spans="1:13" ht="24" x14ac:dyDescent="0.2">
-      <c r="B90" s="19" t="s">
+      <c r="D102" s="27"/>
+      <c r="E102" s="27"/>
+      <c r="F102" s="28"/>
+      <c r="G102" s="28"/>
+      <c r="H102" s="28"/>
+      <c r="I102" s="28"/>
+      <c r="J102" s="28"/>
+      <c r="K102" s="28"/>
+      <c r="L102" s="29"/>
+      <c r="M102" s="29"/>
+    </row>
+    <row r="106" spans="1:13" ht="24" x14ac:dyDescent="0.2">
+      <c r="B106" s="19" t="s">
         <v>46</v>
       </c>
-      <c r="C90" s="19" t="s">
+      <c r="C106" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="D90" s="60" t="s">
+      <c r="D106" s="60" t="s">
         <v>48</v>
       </c>
-      <c r="E90" s="60" t="s">
+      <c r="E106" s="60" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="91" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B91" s="31" t="s">
+    <row r="107" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B107" s="31" t="s">
         <v>42</v>
       </c>
-      <c r="C91" s="57">
+      <c r="C107" s="57">
         <v>43589</v>
       </c>
-      <c r="D91" s="58">
+      <c r="D107" s="58">
         <v>0.5</v>
       </c>
-      <c r="E91" s="58">
+      <c r="E107" s="58">
         <v>0.95</v>
       </c>
     </row>
-    <row r="92" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B92" s="31" t="s">
+    <row r="108" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B108" s="31" t="s">
         <v>43</v>
       </c>
-      <c r="C92" s="57">
+      <c r="C108" s="57">
         <v>43596</v>
       </c>
-      <c r="D92" s="58">
+      <c r="D108" s="58">
         <v>0.25</v>
       </c>
-      <c r="E92" s="58">
+      <c r="E108" s="58">
         <v>0.95</v>
       </c>
     </row>
-    <row r="93" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B93" s="31" t="s">
+    <row r="109" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B109" s="31" t="s">
         <v>44</v>
       </c>
-      <c r="C93" s="57">
+      <c r="C109" s="57">
         <v>43603</v>
       </c>
-      <c r="D93" s="58">
+      <c r="D109" s="58">
         <v>0.1</v>
       </c>
-      <c r="E93" s="58">
+      <c r="E109" s="58">
         <v>0.95</v>
       </c>
     </row>
-    <row r="94" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B94" s="31" t="s">
+    <row r="110" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B110" s="31" t="s">
         <v>45</v>
       </c>
-      <c r="C94" s="57">
+      <c r="C110" s="57">
         <v>43610</v>
       </c>
-      <c r="D94" s="58">
+      <c r="D110" s="58">
         <v>0.3</v>
       </c>
-      <c r="E94" s="58">
+      <c r="E110" s="58">
         <v>0.95</v>
       </c>
     </row>
   </sheetData>
-  <dataValidations disablePrompts="1" count="1">
-    <dataValidation type="list" allowBlank="1" sqref="E32:E85">
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" sqref="E32:E101">
       <formula1>$G$31:$L$31</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
increase some rows heights
</commit_message>
<xml_diff>
--- a/PM/Project schedule.xlsx
+++ b/PM/Project schedule.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC\Documents\GitHub\Internet-Banking-System\PM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ITI\Internet-Banking-System\Internet-Banking-System\PM\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="9045"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="9048"/>
   </bookViews>
   <sheets>
     <sheet name="ProjectTimeline" sheetId="8" r:id="rId1"/>
@@ -2707,8 +2707,8 @@
         </c:dLbls>
         <c:gapWidth val="20"/>
         <c:overlap val="100"/>
-        <c:axId val="-1643671296"/>
-        <c:axId val="-1292824464"/>
+        <c:axId val="260196208"/>
+        <c:axId val="260196592"/>
       </c:barChart>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
@@ -3269,11 +3269,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1292818480"/>
-        <c:axId val="-1292821744"/>
+        <c:axId val="260197360"/>
+        <c:axId val="260196976"/>
       </c:scatterChart>
       <c:catAx>
-        <c:axId val="-1643671296"/>
+        <c:axId val="260196208"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -3330,7 +3330,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1292824464"/>
+        <c:crossAx val="260196592"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3340,7 +3340,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1292824464"/>
+        <c:axId val="260196592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="43646"/>
@@ -3399,13 +3399,13 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1643671296"/>
+        <c:crossAx val="260196208"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="30"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1292821744"/>
+        <c:axId val="260196976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -3416,13 +3416,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1292818480"/>
+        <c:crossAx val="260197360"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="1"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1292818480"/>
+        <c:axId val="260197360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3432,7 +3432,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1292821744"/>
+        <c:crossAx val="260196976"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4041,7 +4041,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F44686F1-DCE1-4D18-A327-C5E0B87F1EF6}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{F44686F1-DCE1-4D18-A327-C5E0B87F1EF6}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4091,7 +4091,7 @@
         <xdr:cNvPr id="5" name="Chart 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{83273588-A5A1-4D9D-B78C-30406444437C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{83273588-A5A1-4D9D-B78C-30406444437C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4134,7 +4134,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F5E0D6A9-E059-4B8E-90BD-4CA99306D6EF}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{F5E0D6A9-E059-4B8E-90BD-4CA99306D6EF}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4437,25 +4437,25 @@
   </sheetPr>
   <dimension ref="A1:O110"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A29" zoomScaleNormal="100" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="G47" sqref="G47"/>
+    <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScaleNormal="100" zoomScalePageLayoutView="85" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15" customWidth="1"/>
-    <col min="2" max="2" width="29.75" customWidth="1"/>
-    <col min="3" max="3" width="9.75" style="9" customWidth="1"/>
-    <col min="4" max="4" width="9.75" customWidth="1"/>
-    <col min="5" max="5" width="11.375" customWidth="1"/>
+    <col min="2" max="2" width="29.69921875" customWidth="1"/>
+    <col min="3" max="3" width="9.69921875" style="9" customWidth="1"/>
+    <col min="4" max="4" width="9.69921875" customWidth="1"/>
+    <col min="5" max="5" width="11.3984375" customWidth="1"/>
     <col min="6" max="6" width="8" customWidth="1"/>
-    <col min="7" max="7" width="6.875" customWidth="1"/>
+    <col min="7" max="7" width="6.8984375" customWidth="1"/>
     <col min="8" max="12" width="6" customWidth="1"/>
     <col min="13" max="13" width="14.5" customWidth="1"/>
     <col min="15" max="15" width="22.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:15" ht="24.6" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>82</v>
       </c>
@@ -4472,7 +4472,7 @@
       <c r="L1" s="2"/>
       <c r="M1" s="2"/>
     </row>
-    <row r="2" spans="1:15" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:15" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H2" s="18" t="s">
         <v>16</v>
       </c>
@@ -4480,12 +4480,15 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="O3" s="11" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:15" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="1:15" ht="86.4" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="28" spans="1:13" ht="115.8" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="1:13" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B30" s="59" t="s">
         <v>10</v>
       </c>
@@ -4502,7 +4505,7 @@
       <c r="K30" s="62"/>
       <c r="L30" s="63"/>
     </row>
-    <row r="31" spans="1:13" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:13" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="19" t="s">
         <v>26</v>
       </c>
@@ -4543,7 +4546,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="32" spans="1:13" s="7" customFormat="1" ht="15" hidden="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:13" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" s="30"/>
       <c r="B32" s="31"/>
       <c r="C32" s="32"/>
@@ -4557,7 +4560,7 @@
       <c r="K32" s="13"/>
       <c r="L32" s="14"/>
     </row>
-    <row r="33" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="30"/>
       <c r="B33" s="31"/>
       <c r="C33" s="32"/>
@@ -4571,7 +4574,7 @@
       <c r="K33" s="13"/>
       <c r="L33" s="14"/>
     </row>
-    <row r="34" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="30"/>
       <c r="B34" s="31"/>
       <c r="C34" s="32"/>
@@ -4585,7 +4588,7 @@
       <c r="K34" s="13"/>
       <c r="L34" s="14"/>
     </row>
-    <row r="35" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="30"/>
       <c r="B35" s="31"/>
       <c r="C35" s="32"/>
@@ -4599,7 +4602,7 @@
       <c r="K35" s="13"/>
       <c r="L35" s="14"/>
     </row>
-    <row r="36" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="30" t="s">
         <v>60</v>
       </c>
@@ -4616,7 +4619,7 @@
       <c r="L36" s="66"/>
       <c r="M36" s="66"/>
     </row>
-    <row r="37" spans="1:13" s="7" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:13" s="7" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B37" s="31" t="s">
         <v>64</v>
       </c>
@@ -4661,7 +4664,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="38" spans="1:13" s="7" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:13" s="7" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="30"/>
       <c r="B38" s="31"/>
       <c r="C38" s="32"/>
@@ -4676,7 +4679,7 @@
       <c r="L38" s="66"/>
       <c r="M38" s="66"/>
     </row>
-    <row r="39" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="30"/>
       <c r="B39" s="31" t="s">
         <v>73</v>
@@ -4716,7 +4719,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="40" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="30"/>
       <c r="B40" s="31"/>
       <c r="C40" s="32"/>
@@ -4731,7 +4734,7 @@
       <c r="L40" s="66"/>
       <c r="M40" s="66"/>
     </row>
-    <row r="41" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="30"/>
       <c r="B41" s="31" t="s">
         <v>70</v>
@@ -4776,7 +4779,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="42" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="30"/>
       <c r="B42" s="31"/>
       <c r="C42" s="32"/>
@@ -4791,7 +4794,7 @@
       <c r="L42" s="66"/>
       <c r="M42" s="66"/>
     </row>
-    <row r="43" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="30"/>
       <c r="B43" s="31" t="s">
         <v>71</v>
@@ -4836,7 +4839,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="44" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="30"/>
       <c r="B44" s="31"/>
       <c r="C44" s="32"/>
@@ -4851,7 +4854,7 @@
       <c r="L44" s="66"/>
       <c r="M44" s="66"/>
     </row>
-    <row r="45" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="30"/>
       <c r="B45" s="31" t="s">
         <v>85</v>
@@ -4890,7 +4893,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="46" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="30"/>
       <c r="B46" s="31"/>
       <c r="C46" s="32"/>
@@ -4905,7 +4908,7 @@
       <c r="L46" s="66"/>
       <c r="M46" s="66"/>
     </row>
-    <row r="47" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="30"/>
       <c r="B47" s="31" t="s">
         <v>81</v>
@@ -4949,7 +4952,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="48" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="30"/>
       <c r="B48" s="31"/>
       <c r="C48" s="32"/>
@@ -4964,7 +4967,7 @@
       <c r="L48" s="66"/>
       <c r="M48" s="66"/>
     </row>
-    <row r="49" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" s="30" t="s">
         <v>59</v>
       </c>
@@ -4981,7 +4984,7 @@
       <c r="L49" s="66"/>
       <c r="M49" s="66"/>
     </row>
-    <row r="50" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A50" s="30"/>
       <c r="B50" s="31" t="s">
         <v>69</v>
@@ -5027,7 +5030,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="51" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A51" s="30"/>
       <c r="B51" s="31"/>
       <c r="C51" s="32"/>
@@ -5042,7 +5045,7 @@
       <c r="L51" s="66"/>
       <c r="M51" s="66"/>
     </row>
-    <row r="52" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A52" s="30"/>
       <c r="B52" s="31" t="s">
         <v>67</v>
@@ -5088,7 +5091,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="53" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A53" s="30"/>
       <c r="B53" s="31"/>
       <c r="C53" s="32"/>
@@ -5103,7 +5106,7 @@
       <c r="L53" s="66"/>
       <c r="M53" s="66"/>
     </row>
-    <row r="54" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A54" s="30"/>
       <c r="B54" s="31" t="s">
         <v>66</v>
@@ -5149,7 +5152,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="55" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A55" s="30"/>
       <c r="B55" s="31"/>
       <c r="C55" s="32"/>
@@ -5164,7 +5167,7 @@
       <c r="L55" s="66"/>
       <c r="M55" s="66"/>
     </row>
-    <row r="56" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A56" s="30"/>
       <c r="B56" s="31" t="s">
         <v>68</v>
@@ -5210,7 +5213,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="57" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A57" s="30"/>
       <c r="B57" s="31"/>
       <c r="C57" s="32"/>
@@ -5225,7 +5228,7 @@
       <c r="L57" s="66"/>
       <c r="M57" s="66"/>
     </row>
-    <row r="58" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A58" s="30"/>
       <c r="B58" s="31" t="s">
         <v>77</v>
@@ -5271,7 +5274,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="59" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A59" s="30"/>
       <c r="B59" s="31"/>
       <c r="C59" s="32"/>
@@ -5286,7 +5289,7 @@
       <c r="L59" s="66"/>
       <c r="M59" s="66"/>
     </row>
-    <row r="60" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A60" s="30"/>
       <c r="B60" s="31"/>
       <c r="C60" s="32"/>
@@ -5301,7 +5304,7 @@
       <c r="L60" s="66"/>
       <c r="M60" s="66"/>
     </row>
-    <row r="61" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A61" s="30"/>
       <c r="B61" s="31"/>
       <c r="C61" s="32"/>
@@ -5316,7 +5319,7 @@
       <c r="L61" s="66"/>
       <c r="M61" s="66"/>
     </row>
-    <row r="62" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A62" s="30" t="s">
         <v>58</v>
       </c>
@@ -5333,7 +5336,7 @@
       <c r="L62" s="66"/>
       <c r="M62" s="66"/>
     </row>
-    <row r="63" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A63" s="30"/>
       <c r="B63" s="31" t="s">
         <v>90</v>
@@ -5378,7 +5381,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="64" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A64" s="30"/>
       <c r="B64" s="31"/>
       <c r="C64" s="32"/>
@@ -5393,7 +5396,7 @@
       <c r="L64" s="66"/>
       <c r="M64" s="66"/>
     </row>
-    <row r="65" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A65" s="30"/>
       <c r="B65" s="31" t="s">
         <v>89</v>
@@ -5432,7 +5435,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="66" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A66" s="30"/>
       <c r="B66" s="31"/>
       <c r="C66" s="32"/>
@@ -5447,7 +5450,7 @@
       <c r="L66" s="66"/>
       <c r="M66" s="66"/>
     </row>
-    <row r="67" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A67" s="30"/>
       <c r="B67" s="31" t="s">
         <v>88</v>
@@ -5492,7 +5495,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="68" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A68" s="30"/>
       <c r="B68" s="31"/>
       <c r="C68" s="32"/>
@@ -5507,7 +5510,7 @@
       <c r="L68" s="66"/>
       <c r="M68" s="66"/>
     </row>
-    <row r="69" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A69" s="30"/>
       <c r="B69" s="31" t="s">
         <v>93</v>
@@ -5546,7 +5549,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="70" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A70" s="30"/>
       <c r="B70" s="31"/>
       <c r="C70" s="32"/>
@@ -5561,7 +5564,7 @@
       <c r="L70" s="66"/>
       <c r="M70" s="66"/>
     </row>
-    <row r="71" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A71" s="30"/>
       <c r="B71" s="31" t="s">
         <v>91</v>
@@ -5600,7 +5603,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="72" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A72" s="30"/>
       <c r="B72" s="31"/>
       <c r="C72" s="32"/>
@@ -5615,7 +5618,7 @@
       <c r="L72" s="66"/>
       <c r="M72" s="66"/>
     </row>
-    <row r="73" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A73" s="30"/>
       <c r="B73" s="31" t="s">
         <v>94</v>
@@ -5654,7 +5657,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="74" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A74" s="30"/>
       <c r="B74" s="31"/>
       <c r="C74" s="32"/>
@@ -5669,7 +5672,7 @@
       <c r="L74" s="66"/>
       <c r="M74" s="66"/>
     </row>
-    <row r="75" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A75" s="30"/>
       <c r="B75" s="31" t="s">
         <v>96</v>
@@ -5714,7 +5717,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="76" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A76" s="30"/>
       <c r="B76" s="31"/>
       <c r="C76" s="32"/>
@@ -5729,7 +5732,7 @@
       <c r="L76" s="66"/>
       <c r="M76" s="66"/>
     </row>
-    <row r="77" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A77" s="30"/>
       <c r="B77" s="31" t="s">
         <v>97</v>
@@ -5768,7 +5771,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="78" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A78" s="30"/>
       <c r="B78" s="31"/>
       <c r="C78" s="32"/>
@@ -5783,7 +5786,7 @@
       <c r="L78" s="66"/>
       <c r="M78" s="66"/>
     </row>
-    <row r="79" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A79" s="30"/>
       <c r="B79" s="31" t="s">
         <v>99</v>
@@ -5822,7 +5825,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="80" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A80" s="30"/>
       <c r="B80" s="31"/>
       <c r="C80" s="32"/>
@@ -5837,7 +5840,7 @@
       <c r="L80" s="66"/>
       <c r="M80" s="66"/>
     </row>
-    <row r="81" spans="1:13" s="7" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:13" s="7" customFormat="1" ht="66" x14ac:dyDescent="0.25">
       <c r="A81" s="30"/>
       <c r="B81" s="31" t="s">
         <v>98</v>
@@ -5876,7 +5879,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="82" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A82" s="30"/>
       <c r="B82" s="31"/>
       <c r="C82" s="32"/>
@@ -5891,7 +5894,7 @@
       <c r="L82" s="66"/>
       <c r="M82" s="66"/>
     </row>
-    <row r="83" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A83" s="30" t="s">
         <v>61</v>
       </c>
@@ -5935,7 +5938,7 @@
       </c>
       <c r="M83" s="66"/>
     </row>
-    <row r="84" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A84" s="30"/>
       <c r="B84" s="31"/>
       <c r="C84" s="32"/>
@@ -5973,7 +5976,7 @@
       </c>
       <c r="M84" s="66"/>
     </row>
-    <row r="85" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A85" s="30"/>
       <c r="B85" s="31"/>
       <c r="C85" s="32"/>
@@ -6011,7 +6014,7 @@
       </c>
       <c r="M85" s="66"/>
     </row>
-    <row r="86" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A86" s="30"/>
       <c r="B86" s="31"/>
       <c r="C86" s="32"/>
@@ -6026,7 +6029,7 @@
       <c r="L86" s="66"/>
       <c r="M86" s="66"/>
     </row>
-    <row r="87" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A87" s="30"/>
       <c r="B87" s="31"/>
       <c r="C87" s="32"/>
@@ -6041,7 +6044,7 @@
       <c r="L87" s="66"/>
       <c r="M87" s="66"/>
     </row>
-    <row r="88" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A88" s="30"/>
       <c r="B88" s="31"/>
       <c r="C88" s="32"/>
@@ -6056,7 +6059,7 @@
       <c r="L88" s="66"/>
       <c r="M88" s="66"/>
     </row>
-    <row r="89" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A89" s="30"/>
       <c r="B89" s="31"/>
       <c r="C89" s="32"/>
@@ -6071,7 +6074,7 @@
       <c r="L89" s="66"/>
       <c r="M89" s="66"/>
     </row>
-    <row r="90" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A90" s="30"/>
       <c r="B90" s="31"/>
       <c r="C90" s="32"/>
@@ -6109,7 +6112,7 @@
       </c>
       <c r="M90" s="66"/>
     </row>
-    <row r="91" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A91" s="30"/>
       <c r="B91" s="31"/>
       <c r="C91" s="32"/>
@@ -6147,7 +6150,7 @@
       </c>
       <c r="M91" s="66"/>
     </row>
-    <row r="92" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A92" s="30" t="s">
         <v>62</v>
       </c>
@@ -6191,7 +6194,7 @@
       </c>
       <c r="M92" s="66"/>
     </row>
-    <row r="93" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A93" s="30"/>
       <c r="B93" s="31"/>
       <c r="C93" s="32"/>
@@ -6229,7 +6232,7 @@
       </c>
       <c r="M93" s="66"/>
     </row>
-    <row r="94" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A94" s="30"/>
       <c r="B94" s="31"/>
       <c r="C94" s="32"/>
@@ -6267,7 +6270,7 @@
       </c>
       <c r="M94" s="66"/>
     </row>
-    <row r="95" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A95" s="30"/>
       <c r="B95" s="31"/>
       <c r="C95" s="32"/>
@@ -6282,7 +6285,7 @@
       <c r="L95" s="66"/>
       <c r="M95" s="66"/>
     </row>
-    <row r="96" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A96" s="30"/>
       <c r="B96" s="31"/>
       <c r="C96" s="32"/>
@@ -6299,7 +6302,7 @@
       <c r="L96" s="66"/>
       <c r="M96" s="66"/>
     </row>
-    <row r="97" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A97" s="30" t="s">
         <v>84</v>
       </c>
@@ -6343,7 +6346,7 @@
       </c>
       <c r="M97" s="66"/>
     </row>
-    <row r="98" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A98" s="30"/>
       <c r="B98" s="31"/>
       <c r="C98" s="32"/>
@@ -6360,7 +6363,7 @@
       <c r="L98" s="66"/>
       <c r="M98" s="66"/>
     </row>
-    <row r="99" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A99" s="30"/>
       <c r="B99" s="31"/>
       <c r="C99" s="32"/>
@@ -6377,7 +6380,7 @@
       <c r="L99" s="66"/>
       <c r="M99" s="66"/>
     </row>
-    <row r="100" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A100" s="30"/>
       <c r="B100" s="31"/>
       <c r="C100" s="32"/>
@@ -6394,7 +6397,7 @@
       <c r="L100" s="66"/>
       <c r="M100" s="66"/>
     </row>
-    <row r="101" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A101" s="30"/>
       <c r="B101" s="31"/>
       <c r="C101" s="32"/>
@@ -6432,7 +6435,7 @@
       </c>
       <c r="M101" s="66"/>
     </row>
-    <row r="102" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:13" s="7" customFormat="1" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A102" s="24"/>
       <c r="B102" s="25"/>
       <c r="C102" s="26" t="s">
@@ -6449,7 +6452,7 @@
       <c r="L102" s="29"/>
       <c r="M102" s="29"/>
     </row>
-    <row r="106" spans="1:13" ht="24" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:13" ht="22.8" x14ac:dyDescent="0.25">
       <c r="B106" s="19" t="s">
         <v>46</v>
       </c>
@@ -6463,7 +6466,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="107" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B107" s="31" t="s">
         <v>42</v>
       </c>
@@ -6477,7 +6480,7 @@
         <v>0.95</v>
       </c>
     </row>
-    <row r="108" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B108" s="31" t="s">
         <v>43</v>
       </c>
@@ -6491,7 +6494,7 @@
         <v>0.95</v>
       </c>
     </row>
-    <row r="109" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B109" s="31" t="s">
         <v>44</v>
       </c>
@@ -6505,7 +6508,7 @@
         <v>0.95</v>
       </c>
     </row>
-    <row r="110" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B110" s="31" t="s">
         <v>45</v>
       </c>
@@ -6543,21 +6546,21 @@
       <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9" customWidth="1"/>
     <col min="2" max="2" width="68.5" customWidth="1"/>
     <col min="3" max="3" width="6" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="49" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="50"/>
       <c r="C1" s="50"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="46" t="s">
         <v>34</v>
       </c>
@@ -6565,10 +6568,10 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C3" s="48"/>
     </row>
-    <row r="4" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="54" t="s">
         <v>1</v>
       </c>
@@ -6576,202 +6579,202 @@
       <c r="C4" s="56"/>
       <c r="D4" s="3"/>
     </row>
-    <row r="5" spans="1:4" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" ht="41.4" x14ac:dyDescent="0.25">
       <c r="B5" s="5" t="s">
         <v>53</v>
       </c>
       <c r="D5" s="3"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B6" s="5"/>
       <c r="D6" s="3"/>
     </row>
-    <row r="7" spans="1:4" ht="57" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" ht="55.2" x14ac:dyDescent="0.25">
       <c r="B7" s="5" t="s">
         <v>40</v>
       </c>
       <c r="D7" s="3"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B8" s="5"/>
       <c r="D8" s="3"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B9" s="15"/>
       <c r="D9" s="3"/>
     </row>
-    <row r="10" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B10" s="17" t="s">
         <v>32</v>
       </c>
       <c r="D10" s="3"/>
     </row>
-    <row r="11" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B11" s="16" t="s">
         <v>15</v>
       </c>
       <c r="D11" s="3"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B12" s="15"/>
       <c r="D12" s="3"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B13" s="5"/>
       <c r="D13" s="3"/>
     </row>
-    <row r="14" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="54" t="s">
         <v>39</v>
       </c>
       <c r="B14" s="55"/>
       <c r="C14" s="56"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B15" s="5"/>
       <c r="D15" s="3"/>
     </row>
-    <row r="16" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>55</v>
       </c>
       <c r="B16" s="5"/>
       <c r="D16" s="3"/>
     </row>
-    <row r="17" spans="1:4" ht="57" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" ht="55.2" x14ac:dyDescent="0.25">
       <c r="B17" s="5" t="s">
         <v>56</v>
       </c>
       <c r="D17" s="3"/>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B18" s="5"/>
       <c r="D18" s="3"/>
     </row>
-    <row r="19" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
         <v>13</v>
       </c>
       <c r="B19" s="5"/>
       <c r="D19" s="3"/>
     </row>
-    <row r="20" spans="1:4" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4" ht="27.6" x14ac:dyDescent="0.25">
       <c r="B20" s="5" t="s">
         <v>14</v>
       </c>
       <c r="D20" s="3"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B21" s="5"/>
       <c r="D21" s="3"/>
     </row>
-    <row r="22" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
         <v>27</v>
       </c>
       <c r="B22" s="5"/>
       <c r="D22" s="3"/>
     </row>
-    <row r="23" spans="1:4" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4" ht="41.4" x14ac:dyDescent="0.25">
       <c r="B23" s="5" t="s">
         <v>28</v>
       </c>
       <c r="D23" s="3"/>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B24" s="5"/>
       <c r="D24" s="3"/>
     </row>
-    <row r="25" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
         <v>50</v>
       </c>
       <c r="B25" s="5"/>
       <c r="D25" s="3"/>
     </row>
-    <row r="26" spans="1:4" ht="57" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:4" ht="55.2" x14ac:dyDescent="0.25">
       <c r="B26" s="5" t="s">
         <v>51</v>
       </c>
       <c r="D26" s="3"/>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B27" s="5"/>
       <c r="D27" s="3"/>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B28" s="5" t="s">
         <v>54</v>
       </c>
       <c r="D28" s="3"/>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B29" s="5"/>
       <c r="D29" s="3"/>
     </row>
-    <row r="30" spans="1:4" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:4" ht="27.6" x14ac:dyDescent="0.25">
       <c r="B30" s="5" t="s">
         <v>52</v>
       </c>
       <c r="D30" s="3"/>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B31" s="5"/>
       <c r="D31" s="3"/>
     </row>
-    <row r="32" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
         <v>29</v>
       </c>
       <c r="B32" s="5"/>
       <c r="D32" s="3"/>
     </row>
-    <row r="33" spans="1:4" ht="57" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:4" ht="55.2" x14ac:dyDescent="0.25">
       <c r="B33" s="5" t="s">
         <v>30</v>
       </c>
       <c r="D33" s="3"/>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B34" s="5"/>
       <c r="D34" s="3"/>
     </row>
-    <row r="35" spans="1:4" ht="57" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:4" ht="55.2" x14ac:dyDescent="0.25">
       <c r="B35" s="5" t="s">
         <v>31</v>
       </c>
       <c r="D35" s="3"/>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B36" s="5"/>
       <c r="D36" s="3"/>
     </row>
-    <row r="37" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
         <v>2</v>
       </c>
       <c r="B37" s="3"/>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B38" s="5" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B39" s="6" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B40" s="3"/>
     </row>
-    <row r="41" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B41" s="5"/>
     </row>
-    <row r="42" spans="1:4" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:4" ht="27.6" x14ac:dyDescent="0.25">
       <c r="B42" s="5" t="s">
         <v>6</v>
       </c>
@@ -6794,167 +6797,167 @@
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.625" style="43" customWidth="1"/>
-    <col min="2" max="2" width="67.625" style="43" customWidth="1"/>
-    <col min="3" max="3" width="2.875" customWidth="1"/>
+    <col min="1" max="1" width="2.59765625" style="43" customWidth="1"/>
+    <col min="2" max="2" width="67.59765625" style="43" customWidth="1"/>
+    <col min="3" max="3" width="2.8984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="53"/>
       <c r="B1" s="53" t="s">
         <v>33</v>
       </c>
       <c r="C1" s="53"/>
     </row>
-    <row r="2" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="51"/>
       <c r="B2" s="37"/>
       <c r="C2" s="52"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="35"/>
       <c r="B3" s="38" t="s">
         <v>35</v>
       </c>
       <c r="C3" s="36"/>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="35"/>
       <c r="B4" s="44" t="s">
         <v>34</v>
       </c>
       <c r="C4" s="36"/>
     </row>
-    <row r="5" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" s="35"/>
       <c r="B5" s="39"/>
       <c r="C5" s="36"/>
     </row>
-    <row r="6" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A6" s="35"/>
       <c r="B6" s="40" t="s">
         <v>7</v>
       </c>
       <c r="C6" s="36"/>
     </row>
-    <row r="7" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="35"/>
       <c r="B7" s="39"/>
       <c r="C7" s="36"/>
     </row>
-    <row r="8" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="35"/>
       <c r="B8" s="39" t="s">
         <v>3</v>
       </c>
       <c r="C8" s="36"/>
     </row>
-    <row r="9" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" s="35"/>
       <c r="B9" s="39"/>
       <c r="C9" s="36"/>
     </row>
-    <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="35"/>
       <c r="B10" s="39" t="s">
         <v>36</v>
       </c>
       <c r="C10" s="36"/>
     </row>
-    <row r="11" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" s="35"/>
       <c r="B11" s="39"/>
       <c r="C11" s="36"/>
     </row>
-    <row r="12" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="35"/>
       <c r="B12" s="39" t="s">
         <v>37</v>
       </c>
       <c r="C12" s="36"/>
     </row>
-    <row r="13" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" s="35"/>
       <c r="B13" s="39"/>
       <c r="C13" s="36"/>
     </row>
-    <row r="14" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A14" s="35"/>
       <c r="B14" s="41" t="s">
         <v>4</v>
       </c>
       <c r="C14" s="36"/>
     </row>
-    <row r="15" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A15" s="35"/>
       <c r="B15" s="42"/>
       <c r="C15" s="36"/>
     </row>
-    <row r="16" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A16" s="35"/>
       <c r="B16" s="45" t="s">
         <v>38</v>
       </c>
       <c r="C16" s="36"/>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="35"/>
       <c r="B17" s="35"/>
       <c r="C17" s="36"/>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="35"/>
       <c r="B18" s="35"/>
       <c r="C18" s="36"/>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="35"/>
       <c r="B19" s="35"/>
       <c r="C19" s="36"/>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="35"/>
       <c r="B20" s="35"/>
       <c r="C20" s="36"/>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="35"/>
       <c r="B21" s="35"/>
       <c r="C21" s="36"/>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="35"/>
       <c r="B22" s="35"/>
       <c r="C22" s="36"/>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="35"/>
       <c r="B23" s="35"/>
       <c r="C23" s="36"/>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="35"/>
       <c r="B24" s="35"/>
       <c r="C24" s="36"/>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="35"/>
       <c r="B25" s="35"/>
       <c r="C25" s="36"/>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="35"/>
       <c r="B26" s="35"/>
       <c r="C26" s="36"/>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="35"/>
       <c r="B27" s="35"/>
       <c r="C27" s="36"/>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="35"/>
       <c r="B28" s="35"/>
       <c r="C28" s="36"/>

</xml_diff>

<commit_message>
Update Tasks of week 3 Developement and Testing
Update Tasks of week 3 Developement and Testing
</commit_message>
<xml_diff>
--- a/PM/Project schedule.xlsx
+++ b/PM/Project schedule.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="122">
   <si>
     <t>HELP</t>
   </si>
@@ -219,9 +219,6 @@
   </si>
   <si>
     <t>PM</t>
-  </si>
-  <si>
-    <t>Development</t>
   </si>
   <si>
     <t>Testing</t>
@@ -343,6 +340,72 @@
 Sondos
 Khadija
 Ahmed</t>
+  </si>
+  <si>
+    <t>Create Data Base and tables</t>
+  </si>
+  <si>
+    <t>Salsabeel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dev.Register Page. Front end </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dev.Register Page. Back end </t>
+  </si>
+  <si>
+    <t>Hassan _Alaa</t>
+  </si>
+  <si>
+    <t>Salsabeel_Ahmed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dev.Log in Page. Front end </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dev.Log in Page. Back end </t>
+  </si>
+  <si>
+    <t>Design.TC.log in page</t>
+  </si>
+  <si>
+    <t>Sondos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Update SRS and SIQ </t>
+  </si>
+  <si>
+    <t>Khadeja</t>
+  </si>
+  <si>
+    <t>Design.TC.Admin page</t>
+  </si>
+  <si>
+    <t>Design.TC.Registation page</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dev.User Main Page. Front end </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dev.User Main Page. Back end </t>
+  </si>
+  <si>
+    <t>Design.TC.Account Main page.Front</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dev.Accounts Page. Front end </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dev.Accounts Page. Back end </t>
+  </si>
+  <si>
+    <t>Development and Testing</t>
+  </si>
+  <si>
+    <t>Design.TC.Transfere Page.Front</t>
+  </si>
+  <si>
+    <t>Design.TC.Previous TR Page.Front</t>
   </si>
 </sst>
 </file>
@@ -537,7 +600,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -572,6 +635,12 @@
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.39997558519241921"/>
         <bgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -781,7 +850,7 @@
     </xf>
     <xf numFmtId="9" fontId="25" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="70">
+  <cellXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -968,6 +1037,9 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" customBuiltin="1"/>
@@ -1148,9 +1220,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:f>ProjectTimeline!$A$32:$B$102</c:f>
+              <c:f>ProjectTimeline!$A$32:$B$133</c:f>
               <c:multiLvlStrCache>
-                <c:ptCount val="66"/>
+                <c:ptCount val="97"/>
                 <c:lvl>
                   <c:pt idx="5">
                     <c:v>Responsibility Assignment Matrix</c:v>
@@ -1214,6 +1286,63 @@
                   </c:pt>
                   <c:pt idx="49">
                     <c:v>Software Peer Review Sheet </c:v>
+                  </c:pt>
+                  <c:pt idx="52">
+                    <c:v>Create Data Base and tables</c:v>
+                  </c:pt>
+                  <c:pt idx="54">
+                    <c:v>Dev.Register Page. Front end </c:v>
+                  </c:pt>
+                  <c:pt idx="56">
+                    <c:v>Dev.Register Page. Back end </c:v>
+                  </c:pt>
+                  <c:pt idx="58">
+                    <c:v>Design.TC.log in page</c:v>
+                  </c:pt>
+                  <c:pt idx="60">
+                    <c:v>Dev.Log in Page. Front end </c:v>
+                  </c:pt>
+                  <c:pt idx="62">
+                    <c:v>Dev.Log in Page. Back end </c:v>
+                  </c:pt>
+                  <c:pt idx="64">
+                    <c:v>Update SRS and SIQ </c:v>
+                  </c:pt>
+                  <c:pt idx="66">
+                    <c:v>Design.TC.Admin page</c:v>
+                  </c:pt>
+                  <c:pt idx="68">
+                    <c:v>Design.TC.Registation page</c:v>
+                  </c:pt>
+                  <c:pt idx="70">
+                    <c:v>Dev.User Main Page. Front end </c:v>
+                  </c:pt>
+                  <c:pt idx="72">
+                    <c:v>Dev.User Main Page. Back end </c:v>
+                  </c:pt>
+                  <c:pt idx="74">
+                    <c:v>Design.TC.Account Main page.Front</c:v>
+                  </c:pt>
+                  <c:pt idx="76">
+                    <c:v>Design.TC.Account Main page.Front</c:v>
+                  </c:pt>
+                  <c:pt idx="78">
+                    <c:v>Dev.Accounts Page. Front end </c:v>
+                  </c:pt>
+                  <c:pt idx="80">
+                    <c:v>Dev.Accounts Page. Back end </c:v>
+                  </c:pt>
+                  <c:pt idx="82">
+                    <c:v>Update Schedule</c:v>
+                  </c:pt>
+                  <c:pt idx="84">
+                    <c:v>Update RTM</c:v>
+                  </c:pt>
+                  <c:pt idx="86">
+                    <c:v>Design.TC.Transfere Page.Front</c:v>
+                  </c:pt>
+                  <c:pt idx="88">
+                    <c:v>Design.TC.Previous TR Page.Front</c:v>
                   </c:pt>
                 </c:lvl>
                 <c:lvl>
@@ -1227,12 +1356,12 @@
                     <c:v>Design</c:v>
                   </c:pt>
                   <c:pt idx="51">
-                    <c:v>Development</c:v>
-                  </c:pt>
-                  <c:pt idx="60">
+                    <c:v>Development and Testing</c:v>
+                  </c:pt>
+                  <c:pt idx="91">
                     <c:v>Testing</c:v>
                   </c:pt>
-                  <c:pt idx="65">
+                  <c:pt idx="96">
                     <c:v>Delivery</c:v>
                   </c:pt>
                 </c:lvl>
@@ -1241,10 +1370,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>ProjectTimeline!$F$32:$F$102</c:f>
+              <c:f>ProjectTimeline!$F$32:$F$133</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="71"/>
+                <c:ptCount val="102"/>
                 <c:pt idx="5" formatCode="m/d/yy;@">
                   <c:v>43582</c:v>
                 </c:pt>
@@ -1312,30 +1441,78 @@
                   <c:v>43596</c:v>
                 </c:pt>
                 <c:pt idx="52" formatCode="m/d/yy;@">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="53" formatCode="m/d/yy;@">
-                  <c:v>0</c:v>
+                  <c:v>43597</c:v>
+                </c:pt>
+                <c:pt idx="54" formatCode="m/d/yy;@">
+                  <c:v>43597</c:v>
+                </c:pt>
+                <c:pt idx="56" formatCode="m/d/yy;@">
+                  <c:v>43597</c:v>
                 </c:pt>
                 <c:pt idx="58" formatCode="m/d/yy;@">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="59" formatCode="m/d/yy;@">
-                  <c:v>0</c:v>
+                  <c:v>43597</c:v>
                 </c:pt>
                 <c:pt idx="60" formatCode="m/d/yy;@">
+                  <c:v>43598</c:v>
+                </c:pt>
+                <c:pt idx="62" formatCode="m/d/yy;@">
+                  <c:v>43598</c:v>
+                </c:pt>
+                <c:pt idx="64" formatCode="m/d/yy;@">
+                  <c:v>43598</c:v>
+                </c:pt>
+                <c:pt idx="66" formatCode="m/d/yy;@">
+                  <c:v>43598</c:v>
+                </c:pt>
+                <c:pt idx="68" formatCode="m/d/yy;@">
+                  <c:v>43599</c:v>
+                </c:pt>
+                <c:pt idx="70" formatCode="m/d/yy;@">
+                  <c:v>43599</c:v>
+                </c:pt>
+                <c:pt idx="72" formatCode="m/d/yy;@">
+                  <c:v>43599</c:v>
+                </c:pt>
+                <c:pt idx="74" formatCode="m/d/yy;@">
+                  <c:v>43600</c:v>
+                </c:pt>
+                <c:pt idx="76" formatCode="m/d/yy;@">
+                  <c:v>43600</c:v>
+                </c:pt>
+                <c:pt idx="78" formatCode="m/d/yy;@">
+                  <c:v>43599</c:v>
+                </c:pt>
+                <c:pt idx="80" formatCode="m/d/yy;@">
+                  <c:v>43599</c:v>
+                </c:pt>
+                <c:pt idx="82" formatCode="m/d/yy;@">
+                  <c:v>43600</c:v>
+                </c:pt>
+                <c:pt idx="84" formatCode="m/d/yy;@">
+                  <c:v>43600</c:v>
+                </c:pt>
+                <c:pt idx="86" formatCode="m/d/yy;@">
+                  <c:v>43600</c:v>
+                </c:pt>
+                <c:pt idx="88" formatCode="m/d/yy;@">
+                  <c:v>43601</c:v>
+                </c:pt>
+                <c:pt idx="90" formatCode="m/d/yy;@">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="91" formatCode="m/d/yy;@">
                   <c:v>43603</c:v>
                 </c:pt>
-                <c:pt idx="61" formatCode="m/d/yy;@">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="62" formatCode="m/d/yy;@">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="65" formatCode="m/d/yy;@">
+                <c:pt idx="92" formatCode="m/d/yy;@">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="93" formatCode="m/d/yy;@">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="96" formatCode="m/d/yy;@">
                   <c:v>43610</c:v>
                 </c:pt>
-                <c:pt idx="69" formatCode="m/d/yy;@">
+                <c:pt idx="100" formatCode="m/d/yy;@">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -1373,9 +1550,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:f>ProjectTimeline!$A$32:$B$102</c:f>
+              <c:f>ProjectTimeline!$A$32:$B$133</c:f>
               <c:multiLvlStrCache>
-                <c:ptCount val="66"/>
+                <c:ptCount val="97"/>
                 <c:lvl>
                   <c:pt idx="5">
                     <c:v>Responsibility Assignment Matrix</c:v>
@@ -1439,6 +1616,63 @@
                   </c:pt>
                   <c:pt idx="49">
                     <c:v>Software Peer Review Sheet </c:v>
+                  </c:pt>
+                  <c:pt idx="52">
+                    <c:v>Create Data Base and tables</c:v>
+                  </c:pt>
+                  <c:pt idx="54">
+                    <c:v>Dev.Register Page. Front end </c:v>
+                  </c:pt>
+                  <c:pt idx="56">
+                    <c:v>Dev.Register Page. Back end </c:v>
+                  </c:pt>
+                  <c:pt idx="58">
+                    <c:v>Design.TC.log in page</c:v>
+                  </c:pt>
+                  <c:pt idx="60">
+                    <c:v>Dev.Log in Page. Front end </c:v>
+                  </c:pt>
+                  <c:pt idx="62">
+                    <c:v>Dev.Log in Page. Back end </c:v>
+                  </c:pt>
+                  <c:pt idx="64">
+                    <c:v>Update SRS and SIQ </c:v>
+                  </c:pt>
+                  <c:pt idx="66">
+                    <c:v>Design.TC.Admin page</c:v>
+                  </c:pt>
+                  <c:pt idx="68">
+                    <c:v>Design.TC.Registation page</c:v>
+                  </c:pt>
+                  <c:pt idx="70">
+                    <c:v>Dev.User Main Page. Front end </c:v>
+                  </c:pt>
+                  <c:pt idx="72">
+                    <c:v>Dev.User Main Page. Back end </c:v>
+                  </c:pt>
+                  <c:pt idx="74">
+                    <c:v>Design.TC.Account Main page.Front</c:v>
+                  </c:pt>
+                  <c:pt idx="76">
+                    <c:v>Design.TC.Account Main page.Front</c:v>
+                  </c:pt>
+                  <c:pt idx="78">
+                    <c:v>Dev.Accounts Page. Front end </c:v>
+                  </c:pt>
+                  <c:pt idx="80">
+                    <c:v>Dev.Accounts Page. Back end </c:v>
+                  </c:pt>
+                  <c:pt idx="82">
+                    <c:v>Update Schedule</c:v>
+                  </c:pt>
+                  <c:pt idx="84">
+                    <c:v>Update RTM</c:v>
+                  </c:pt>
+                  <c:pt idx="86">
+                    <c:v>Design.TC.Transfere Page.Front</c:v>
+                  </c:pt>
+                  <c:pt idx="88">
+                    <c:v>Design.TC.Previous TR Page.Front</c:v>
                   </c:pt>
                 </c:lvl>
                 <c:lvl>
@@ -1452,12 +1686,12 @@
                     <c:v>Design</c:v>
                   </c:pt>
                   <c:pt idx="51">
-                    <c:v>Development</c:v>
-                  </c:pt>
-                  <c:pt idx="60">
+                    <c:v>Development and Testing</c:v>
+                  </c:pt>
+                  <c:pt idx="91">
                     <c:v>Testing</c:v>
                   </c:pt>
-                  <c:pt idx="65">
+                  <c:pt idx="96">
                     <c:v>Delivery</c:v>
                   </c:pt>
                 </c:lvl>
@@ -1466,10 +1700,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>ProjectTimeline!$G$32:$G$102</c:f>
+              <c:f>ProjectTimeline!$G$32:$G$133</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="71"/>
+                <c:ptCount val="102"/>
                 <c:pt idx="5">
                   <c:v>5</c:v>
                 </c:pt>
@@ -1539,28 +1773,76 @@
                 <c:pt idx="52">
                   <c:v>0</c:v>
                 </c:pt>
-                <c:pt idx="53">
+                <c:pt idx="54">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="56">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="58">
                   <c:v>0</c:v>
                 </c:pt>
-                <c:pt idx="59">
-                  <c:v>0</c:v>
-                </c:pt>
                 <c:pt idx="60">
                   <c:v>0</c:v>
                 </c:pt>
-                <c:pt idx="61">
-                  <c:v>0</c:v>
-                </c:pt>
                 <c:pt idx="62">
                   <c:v>0</c:v>
                 </c:pt>
-                <c:pt idx="65">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="69">
+                <c:pt idx="64">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="100">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -1598,9 +1880,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:f>ProjectTimeline!$A$32:$B$102</c:f>
+              <c:f>ProjectTimeline!$A$32:$B$133</c:f>
               <c:multiLvlStrCache>
-                <c:ptCount val="66"/>
+                <c:ptCount val="97"/>
                 <c:lvl>
                   <c:pt idx="5">
                     <c:v>Responsibility Assignment Matrix</c:v>
@@ -1664,6 +1946,63 @@
                   </c:pt>
                   <c:pt idx="49">
                     <c:v>Software Peer Review Sheet </c:v>
+                  </c:pt>
+                  <c:pt idx="52">
+                    <c:v>Create Data Base and tables</c:v>
+                  </c:pt>
+                  <c:pt idx="54">
+                    <c:v>Dev.Register Page. Front end </c:v>
+                  </c:pt>
+                  <c:pt idx="56">
+                    <c:v>Dev.Register Page. Back end </c:v>
+                  </c:pt>
+                  <c:pt idx="58">
+                    <c:v>Design.TC.log in page</c:v>
+                  </c:pt>
+                  <c:pt idx="60">
+                    <c:v>Dev.Log in Page. Front end </c:v>
+                  </c:pt>
+                  <c:pt idx="62">
+                    <c:v>Dev.Log in Page. Back end </c:v>
+                  </c:pt>
+                  <c:pt idx="64">
+                    <c:v>Update SRS and SIQ </c:v>
+                  </c:pt>
+                  <c:pt idx="66">
+                    <c:v>Design.TC.Admin page</c:v>
+                  </c:pt>
+                  <c:pt idx="68">
+                    <c:v>Design.TC.Registation page</c:v>
+                  </c:pt>
+                  <c:pt idx="70">
+                    <c:v>Dev.User Main Page. Front end </c:v>
+                  </c:pt>
+                  <c:pt idx="72">
+                    <c:v>Dev.User Main Page. Back end </c:v>
+                  </c:pt>
+                  <c:pt idx="74">
+                    <c:v>Design.TC.Account Main page.Front</c:v>
+                  </c:pt>
+                  <c:pt idx="76">
+                    <c:v>Design.TC.Account Main page.Front</c:v>
+                  </c:pt>
+                  <c:pt idx="78">
+                    <c:v>Dev.Accounts Page. Front end </c:v>
+                  </c:pt>
+                  <c:pt idx="80">
+                    <c:v>Dev.Accounts Page. Back end </c:v>
+                  </c:pt>
+                  <c:pt idx="82">
+                    <c:v>Update Schedule</c:v>
+                  </c:pt>
+                  <c:pt idx="84">
+                    <c:v>Update RTM</c:v>
+                  </c:pt>
+                  <c:pt idx="86">
+                    <c:v>Design.TC.Transfere Page.Front</c:v>
+                  </c:pt>
+                  <c:pt idx="88">
+                    <c:v>Design.TC.Previous TR Page.Front</c:v>
                   </c:pt>
                 </c:lvl>
                 <c:lvl>
@@ -1677,12 +2016,12 @@
                     <c:v>Design</c:v>
                   </c:pt>
                   <c:pt idx="51">
-                    <c:v>Development</c:v>
-                  </c:pt>
-                  <c:pt idx="60">
+                    <c:v>Development and Testing</c:v>
+                  </c:pt>
+                  <c:pt idx="91">
                     <c:v>Testing</c:v>
                   </c:pt>
-                  <c:pt idx="65">
+                  <c:pt idx="96">
                     <c:v>Delivery</c:v>
                   </c:pt>
                 </c:lvl>
@@ -1691,10 +2030,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>ProjectTimeline!$H$32:$H$102</c:f>
+              <c:f>ProjectTimeline!$H$32:$H$133</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="71"/>
+                <c:ptCount val="102"/>
                 <c:pt idx="5">
                   <c:v>0</c:v>
                 </c:pt>
@@ -1764,28 +2103,76 @@
                 <c:pt idx="52">
                   <c:v>0</c:v>
                 </c:pt>
-                <c:pt idx="53">
+                <c:pt idx="54">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="56">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="58">
                   <c:v>0</c:v>
                 </c:pt>
-                <c:pt idx="59">
-                  <c:v>0</c:v>
-                </c:pt>
                 <c:pt idx="60">
                   <c:v>0</c:v>
                 </c:pt>
-                <c:pt idx="61">
-                  <c:v>0</c:v>
-                </c:pt>
                 <c:pt idx="62">
                   <c:v>0</c:v>
                 </c:pt>
-                <c:pt idx="65">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="69">
+                <c:pt idx="64">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="100">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -1823,9 +2210,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:f>ProjectTimeline!$A$32:$B$102</c:f>
+              <c:f>ProjectTimeline!$A$32:$B$133</c:f>
               <c:multiLvlStrCache>
-                <c:ptCount val="66"/>
+                <c:ptCount val="97"/>
                 <c:lvl>
                   <c:pt idx="5">
                     <c:v>Responsibility Assignment Matrix</c:v>
@@ -1889,6 +2276,63 @@
                   </c:pt>
                   <c:pt idx="49">
                     <c:v>Software Peer Review Sheet </c:v>
+                  </c:pt>
+                  <c:pt idx="52">
+                    <c:v>Create Data Base and tables</c:v>
+                  </c:pt>
+                  <c:pt idx="54">
+                    <c:v>Dev.Register Page. Front end </c:v>
+                  </c:pt>
+                  <c:pt idx="56">
+                    <c:v>Dev.Register Page. Back end </c:v>
+                  </c:pt>
+                  <c:pt idx="58">
+                    <c:v>Design.TC.log in page</c:v>
+                  </c:pt>
+                  <c:pt idx="60">
+                    <c:v>Dev.Log in Page. Front end </c:v>
+                  </c:pt>
+                  <c:pt idx="62">
+                    <c:v>Dev.Log in Page. Back end </c:v>
+                  </c:pt>
+                  <c:pt idx="64">
+                    <c:v>Update SRS and SIQ </c:v>
+                  </c:pt>
+                  <c:pt idx="66">
+                    <c:v>Design.TC.Admin page</c:v>
+                  </c:pt>
+                  <c:pt idx="68">
+                    <c:v>Design.TC.Registation page</c:v>
+                  </c:pt>
+                  <c:pt idx="70">
+                    <c:v>Dev.User Main Page. Front end </c:v>
+                  </c:pt>
+                  <c:pt idx="72">
+                    <c:v>Dev.User Main Page. Back end </c:v>
+                  </c:pt>
+                  <c:pt idx="74">
+                    <c:v>Design.TC.Account Main page.Front</c:v>
+                  </c:pt>
+                  <c:pt idx="76">
+                    <c:v>Design.TC.Account Main page.Front</c:v>
+                  </c:pt>
+                  <c:pt idx="78">
+                    <c:v>Dev.Accounts Page. Front end </c:v>
+                  </c:pt>
+                  <c:pt idx="80">
+                    <c:v>Dev.Accounts Page. Back end </c:v>
+                  </c:pt>
+                  <c:pt idx="82">
+                    <c:v>Update Schedule</c:v>
+                  </c:pt>
+                  <c:pt idx="84">
+                    <c:v>Update RTM</c:v>
+                  </c:pt>
+                  <c:pt idx="86">
+                    <c:v>Design.TC.Transfere Page.Front</c:v>
+                  </c:pt>
+                  <c:pt idx="88">
+                    <c:v>Design.TC.Previous TR Page.Front</c:v>
                   </c:pt>
                 </c:lvl>
                 <c:lvl>
@@ -1902,12 +2346,12 @@
                     <c:v>Design</c:v>
                   </c:pt>
                   <c:pt idx="51">
-                    <c:v>Development</c:v>
-                  </c:pt>
-                  <c:pt idx="60">
+                    <c:v>Development and Testing</c:v>
+                  </c:pt>
+                  <c:pt idx="91">
                     <c:v>Testing</c:v>
                   </c:pt>
-                  <c:pt idx="65">
+                  <c:pt idx="96">
                     <c:v>Delivery</c:v>
                   </c:pt>
                 </c:lvl>
@@ -1916,10 +2360,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>ProjectTimeline!$I$32:$I$102</c:f>
+              <c:f>ProjectTimeline!$I$32:$I$133</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="71"/>
+                <c:ptCount val="102"/>
                 <c:pt idx="5">
                   <c:v>0</c:v>
                 </c:pt>
@@ -1989,28 +2433,76 @@
                 <c:pt idx="52">
                   <c:v>0</c:v>
                 </c:pt>
-                <c:pt idx="53">
+                <c:pt idx="54">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="56">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="58">
                   <c:v>0</c:v>
                 </c:pt>
-                <c:pt idx="59">
-                  <c:v>0</c:v>
-                </c:pt>
                 <c:pt idx="60">
                   <c:v>0</c:v>
                 </c:pt>
-                <c:pt idx="61">
-                  <c:v>0</c:v>
-                </c:pt>
                 <c:pt idx="62">
                   <c:v>0</c:v>
                 </c:pt>
-                <c:pt idx="65">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="69">
+                <c:pt idx="64">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="100">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -2048,9 +2540,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:f>ProjectTimeline!$A$32:$B$102</c:f>
+              <c:f>ProjectTimeline!$A$32:$B$133</c:f>
               <c:multiLvlStrCache>
-                <c:ptCount val="66"/>
+                <c:ptCount val="97"/>
                 <c:lvl>
                   <c:pt idx="5">
                     <c:v>Responsibility Assignment Matrix</c:v>
@@ -2114,6 +2606,63 @@
                   </c:pt>
                   <c:pt idx="49">
                     <c:v>Software Peer Review Sheet </c:v>
+                  </c:pt>
+                  <c:pt idx="52">
+                    <c:v>Create Data Base and tables</c:v>
+                  </c:pt>
+                  <c:pt idx="54">
+                    <c:v>Dev.Register Page. Front end </c:v>
+                  </c:pt>
+                  <c:pt idx="56">
+                    <c:v>Dev.Register Page. Back end </c:v>
+                  </c:pt>
+                  <c:pt idx="58">
+                    <c:v>Design.TC.log in page</c:v>
+                  </c:pt>
+                  <c:pt idx="60">
+                    <c:v>Dev.Log in Page. Front end </c:v>
+                  </c:pt>
+                  <c:pt idx="62">
+                    <c:v>Dev.Log in Page. Back end </c:v>
+                  </c:pt>
+                  <c:pt idx="64">
+                    <c:v>Update SRS and SIQ </c:v>
+                  </c:pt>
+                  <c:pt idx="66">
+                    <c:v>Design.TC.Admin page</c:v>
+                  </c:pt>
+                  <c:pt idx="68">
+                    <c:v>Design.TC.Registation page</c:v>
+                  </c:pt>
+                  <c:pt idx="70">
+                    <c:v>Dev.User Main Page. Front end </c:v>
+                  </c:pt>
+                  <c:pt idx="72">
+                    <c:v>Dev.User Main Page. Back end </c:v>
+                  </c:pt>
+                  <c:pt idx="74">
+                    <c:v>Design.TC.Account Main page.Front</c:v>
+                  </c:pt>
+                  <c:pt idx="76">
+                    <c:v>Design.TC.Account Main page.Front</c:v>
+                  </c:pt>
+                  <c:pt idx="78">
+                    <c:v>Dev.Accounts Page. Front end </c:v>
+                  </c:pt>
+                  <c:pt idx="80">
+                    <c:v>Dev.Accounts Page. Back end </c:v>
+                  </c:pt>
+                  <c:pt idx="82">
+                    <c:v>Update Schedule</c:v>
+                  </c:pt>
+                  <c:pt idx="84">
+                    <c:v>Update RTM</c:v>
+                  </c:pt>
+                  <c:pt idx="86">
+                    <c:v>Design.TC.Transfere Page.Front</c:v>
+                  </c:pt>
+                  <c:pt idx="88">
+                    <c:v>Design.TC.Previous TR Page.Front</c:v>
                   </c:pt>
                 </c:lvl>
                 <c:lvl>
@@ -2127,12 +2676,12 @@
                     <c:v>Design</c:v>
                   </c:pt>
                   <c:pt idx="51">
-                    <c:v>Development</c:v>
-                  </c:pt>
-                  <c:pt idx="60">
+                    <c:v>Development and Testing</c:v>
+                  </c:pt>
+                  <c:pt idx="91">
                     <c:v>Testing</c:v>
                   </c:pt>
-                  <c:pt idx="65">
+                  <c:pt idx="96">
                     <c:v>Delivery</c:v>
                   </c:pt>
                 </c:lvl>
@@ -2141,10 +2690,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>ProjectTimeline!$J$32:$J$102</c:f>
+              <c:f>ProjectTimeline!$J$32:$J$133</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="71"/>
+                <c:ptCount val="102"/>
                 <c:pt idx="5">
                   <c:v>0</c:v>
                 </c:pt>
@@ -2209,33 +2758,81 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>10</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="53">
-                  <c:v>0</c:v>
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="59">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="61">
-                  <c:v>0</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="65">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="69">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="100">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -2273,9 +2870,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:f>ProjectTimeline!$A$32:$B$102</c:f>
+              <c:f>ProjectTimeline!$A$32:$B$133</c:f>
               <c:multiLvlStrCache>
-                <c:ptCount val="66"/>
+                <c:ptCount val="97"/>
                 <c:lvl>
                   <c:pt idx="5">
                     <c:v>Responsibility Assignment Matrix</c:v>
@@ -2339,6 +2936,63 @@
                   </c:pt>
                   <c:pt idx="49">
                     <c:v>Software Peer Review Sheet </c:v>
+                  </c:pt>
+                  <c:pt idx="52">
+                    <c:v>Create Data Base and tables</c:v>
+                  </c:pt>
+                  <c:pt idx="54">
+                    <c:v>Dev.Register Page. Front end </c:v>
+                  </c:pt>
+                  <c:pt idx="56">
+                    <c:v>Dev.Register Page. Back end </c:v>
+                  </c:pt>
+                  <c:pt idx="58">
+                    <c:v>Design.TC.log in page</c:v>
+                  </c:pt>
+                  <c:pt idx="60">
+                    <c:v>Dev.Log in Page. Front end </c:v>
+                  </c:pt>
+                  <c:pt idx="62">
+                    <c:v>Dev.Log in Page. Back end </c:v>
+                  </c:pt>
+                  <c:pt idx="64">
+                    <c:v>Update SRS and SIQ </c:v>
+                  </c:pt>
+                  <c:pt idx="66">
+                    <c:v>Design.TC.Admin page</c:v>
+                  </c:pt>
+                  <c:pt idx="68">
+                    <c:v>Design.TC.Registation page</c:v>
+                  </c:pt>
+                  <c:pt idx="70">
+                    <c:v>Dev.User Main Page. Front end </c:v>
+                  </c:pt>
+                  <c:pt idx="72">
+                    <c:v>Dev.User Main Page. Back end </c:v>
+                  </c:pt>
+                  <c:pt idx="74">
+                    <c:v>Design.TC.Account Main page.Front</c:v>
+                  </c:pt>
+                  <c:pt idx="76">
+                    <c:v>Design.TC.Account Main page.Front</c:v>
+                  </c:pt>
+                  <c:pt idx="78">
+                    <c:v>Dev.Accounts Page. Front end </c:v>
+                  </c:pt>
+                  <c:pt idx="80">
+                    <c:v>Dev.Accounts Page. Back end </c:v>
+                  </c:pt>
+                  <c:pt idx="82">
+                    <c:v>Update Schedule</c:v>
+                  </c:pt>
+                  <c:pt idx="84">
+                    <c:v>Update RTM</c:v>
+                  </c:pt>
+                  <c:pt idx="86">
+                    <c:v>Design.TC.Transfere Page.Front</c:v>
+                  </c:pt>
+                  <c:pt idx="88">
+                    <c:v>Design.TC.Previous TR Page.Front</c:v>
                   </c:pt>
                 </c:lvl>
                 <c:lvl>
@@ -2352,12 +3006,12 @@
                     <c:v>Design</c:v>
                   </c:pt>
                   <c:pt idx="51">
-                    <c:v>Development</c:v>
-                  </c:pt>
-                  <c:pt idx="60">
+                    <c:v>Development and Testing</c:v>
+                  </c:pt>
+                  <c:pt idx="91">
                     <c:v>Testing</c:v>
                   </c:pt>
-                  <c:pt idx="65">
+                  <c:pt idx="96">
                     <c:v>Delivery</c:v>
                   </c:pt>
                 </c:lvl>
@@ -2366,10 +3020,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>ProjectTimeline!$K$32:$K$102</c:f>
+              <c:f>ProjectTimeline!$K$32:$K$133</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="71"/>
+                <c:ptCount val="102"/>
                 <c:pt idx="5">
                   <c:v>0</c:v>
                 </c:pt>
@@ -2439,28 +3093,76 @@
                 <c:pt idx="52">
                   <c:v>0</c:v>
                 </c:pt>
-                <c:pt idx="53">
+                <c:pt idx="54">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="56">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="58">
                   <c:v>0</c:v>
                 </c:pt>
-                <c:pt idx="59">
-                  <c:v>0</c:v>
-                </c:pt>
                 <c:pt idx="60">
                   <c:v>0</c:v>
                 </c:pt>
-                <c:pt idx="61">
-                  <c:v>0</c:v>
-                </c:pt>
                 <c:pt idx="62">
                   <c:v>0</c:v>
                 </c:pt>
-                <c:pt idx="65">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="69">
+                <c:pt idx="64">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="100">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -2498,9 +3200,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:f>ProjectTimeline!$A$32:$B$102</c:f>
+              <c:f>ProjectTimeline!$A$32:$B$133</c:f>
               <c:multiLvlStrCache>
-                <c:ptCount val="66"/>
+                <c:ptCount val="97"/>
                 <c:lvl>
                   <c:pt idx="5">
                     <c:v>Responsibility Assignment Matrix</c:v>
@@ -2564,6 +3266,63 @@
                   </c:pt>
                   <c:pt idx="49">
                     <c:v>Software Peer Review Sheet </c:v>
+                  </c:pt>
+                  <c:pt idx="52">
+                    <c:v>Create Data Base and tables</c:v>
+                  </c:pt>
+                  <c:pt idx="54">
+                    <c:v>Dev.Register Page. Front end </c:v>
+                  </c:pt>
+                  <c:pt idx="56">
+                    <c:v>Dev.Register Page. Back end </c:v>
+                  </c:pt>
+                  <c:pt idx="58">
+                    <c:v>Design.TC.log in page</c:v>
+                  </c:pt>
+                  <c:pt idx="60">
+                    <c:v>Dev.Log in Page. Front end </c:v>
+                  </c:pt>
+                  <c:pt idx="62">
+                    <c:v>Dev.Log in Page. Back end </c:v>
+                  </c:pt>
+                  <c:pt idx="64">
+                    <c:v>Update SRS and SIQ </c:v>
+                  </c:pt>
+                  <c:pt idx="66">
+                    <c:v>Design.TC.Admin page</c:v>
+                  </c:pt>
+                  <c:pt idx="68">
+                    <c:v>Design.TC.Registation page</c:v>
+                  </c:pt>
+                  <c:pt idx="70">
+                    <c:v>Dev.User Main Page. Front end </c:v>
+                  </c:pt>
+                  <c:pt idx="72">
+                    <c:v>Dev.User Main Page. Back end </c:v>
+                  </c:pt>
+                  <c:pt idx="74">
+                    <c:v>Design.TC.Account Main page.Front</c:v>
+                  </c:pt>
+                  <c:pt idx="76">
+                    <c:v>Design.TC.Account Main page.Front</c:v>
+                  </c:pt>
+                  <c:pt idx="78">
+                    <c:v>Dev.Accounts Page. Front end </c:v>
+                  </c:pt>
+                  <c:pt idx="80">
+                    <c:v>Dev.Accounts Page. Back end </c:v>
+                  </c:pt>
+                  <c:pt idx="82">
+                    <c:v>Update Schedule</c:v>
+                  </c:pt>
+                  <c:pt idx="84">
+                    <c:v>Update RTM</c:v>
+                  </c:pt>
+                  <c:pt idx="86">
+                    <c:v>Design.TC.Transfere Page.Front</c:v>
+                  </c:pt>
+                  <c:pt idx="88">
+                    <c:v>Design.TC.Previous TR Page.Front</c:v>
                   </c:pt>
                 </c:lvl>
                 <c:lvl>
@@ -2577,12 +3336,12 @@
                     <c:v>Design</c:v>
                   </c:pt>
                   <c:pt idx="51">
-                    <c:v>Development</c:v>
-                  </c:pt>
-                  <c:pt idx="60">
+                    <c:v>Development and Testing</c:v>
+                  </c:pt>
+                  <c:pt idx="91">
                     <c:v>Testing</c:v>
                   </c:pt>
-                  <c:pt idx="65">
+                  <c:pt idx="96">
                     <c:v>Delivery</c:v>
                   </c:pt>
                 </c:lvl>
@@ -2591,10 +3350,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>ProjectTimeline!$L$32:$L$102</c:f>
+              <c:f>ProjectTimeline!$L$32:$L$133</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="71"/>
+                <c:ptCount val="102"/>
                 <c:pt idx="5">
                   <c:v>0</c:v>
                 </c:pt>
@@ -2664,28 +3423,76 @@
                 <c:pt idx="52">
                   <c:v>0</c:v>
                 </c:pt>
-                <c:pt idx="53">
+                <c:pt idx="54">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="56">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="58">
                   <c:v>0</c:v>
                 </c:pt>
-                <c:pt idx="59">
-                  <c:v>0</c:v>
-                </c:pt>
                 <c:pt idx="60">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="91">
                   <c:v>11</c:v>
                 </c:pt>
-                <c:pt idx="61">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="62">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="65">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="69">
+                <c:pt idx="92">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="100">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -2707,8 +3514,8 @@
         </c:dLbls>
         <c:gapWidth val="20"/>
         <c:overlap val="100"/>
-        <c:axId val="-1643671296"/>
-        <c:axId val="-1292824464"/>
+        <c:axId val="1824398448"/>
+        <c:axId val="1824394096"/>
       </c:barChart>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
@@ -2718,7 +3525,7 @@
           <c:order val="7"/>
           <c:tx>
             <c:strRef>
-              <c:f>ProjectTimeline!$B$107</c:f>
+              <c:f>ProjectTimeline!$B$138</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2809,7 +3616,7 @@
           </c:dLbls>
           <c:xVal>
             <c:numRef>
-              <c:f>(ProjectTimeline!$C$107,ProjectTimeline!$C$107)</c:f>
+              <c:f>(ProjectTimeline!$C$138,ProjectTimeline!$C$138)</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy;@</c:formatCode>
                 <c:ptCount val="2"/>
@@ -2824,7 +3631,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>ProjectTimeline!$D$107:$E$107</c:f>
+              <c:f>ProjectTimeline!$D$138:$E$138</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="2"/>
@@ -2849,7 +3656,7 @@
           <c:order val="8"/>
           <c:tx>
             <c:strRef>
-              <c:f>ProjectTimeline!$B$108</c:f>
+              <c:f>ProjectTimeline!$B$139</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2964,7 +3771,7 @@
           </c:dLbls>
           <c:xVal>
             <c:numRef>
-              <c:f>(ProjectTimeline!$C$108,ProjectTimeline!$C$108)</c:f>
+              <c:f>(ProjectTimeline!$C$139,ProjectTimeline!$C$139)</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy;@</c:formatCode>
                 <c:ptCount val="2"/>
@@ -2979,7 +3786,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>ProjectTimeline!$D$108:$E$108</c:f>
+              <c:f>ProjectTimeline!$D$139:$E$139</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="2"/>
@@ -3004,7 +3811,7 @@
           <c:order val="9"/>
           <c:tx>
             <c:strRef>
-              <c:f>ProjectTimeline!$B$109</c:f>
+              <c:f>ProjectTimeline!$B$140</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3095,7 +3902,7 @@
           </c:dLbls>
           <c:xVal>
             <c:numRef>
-              <c:f>(ProjectTimeline!$C$109,ProjectTimeline!$C$109)</c:f>
+              <c:f>(ProjectTimeline!$C$140,ProjectTimeline!$C$140)</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy;@</c:formatCode>
                 <c:ptCount val="2"/>
@@ -3110,7 +3917,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>ProjectTimeline!$D$109:$E$109</c:f>
+              <c:f>ProjectTimeline!$D$140:$E$140</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="2"/>
@@ -3135,7 +3942,7 @@
           <c:order val="10"/>
           <c:tx>
             <c:strRef>
-              <c:f>ProjectTimeline!$B$110</c:f>
+              <c:f>ProjectTimeline!$B$141</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3226,7 +4033,7 @@
           </c:dLbls>
           <c:xVal>
             <c:numRef>
-              <c:f>(ProjectTimeline!$C$110,ProjectTimeline!$C$110)</c:f>
+              <c:f>(ProjectTimeline!$C$141,ProjectTimeline!$C$141)</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy;@</c:formatCode>
                 <c:ptCount val="2"/>
@@ -3241,7 +4048,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>ProjectTimeline!$D$110:$E$110</c:f>
+              <c:f>ProjectTimeline!$D$141:$E$141</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="2"/>
@@ -3269,11 +4076,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1292818480"/>
-        <c:axId val="-1292821744"/>
+        <c:axId val="1824404976"/>
+        <c:axId val="1824395184"/>
       </c:scatterChart>
       <c:catAx>
-        <c:axId val="-1643671296"/>
+        <c:axId val="1824398448"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -3330,7 +4137,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1292824464"/>
+        <c:crossAx val="1824394096"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3340,7 +4147,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1292824464"/>
+        <c:axId val="1824394096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="43646"/>
@@ -3399,13 +4206,13 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1643671296"/>
+        <c:crossAx val="1824398448"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="30"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1292821744"/>
+        <c:axId val="1824395184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -3416,13 +4223,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1292818480"/>
+        <c:crossAx val="1824404976"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="1"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1292818480"/>
+        <c:axId val="1824404976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3432,7 +4239,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1292821744"/>
+        <c:crossAx val="1824395184"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4041,7 +4848,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F44686F1-DCE1-4D18-A327-C5E0B87F1EF6}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{F44686F1-DCE1-4D18-A327-C5E0B87F1EF6}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4091,7 +4898,7 @@
         <xdr:cNvPr id="5" name="Chart 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{83273588-A5A1-4D9D-B78C-30406444437C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{83273588-A5A1-4D9D-B78C-30406444437C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4134,7 +4941,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F5E0D6A9-E059-4B8E-90BD-4CA99306D6EF}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{F5E0D6A9-E059-4B8E-90BD-4CA99306D6EF}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4435,10 +5242,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:O110"/>
+  <dimension ref="A1:O141"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A29" zoomScaleNormal="100" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="G47" sqref="G47"/>
+    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A78" zoomScaleNormal="100" zoomScalePageLayoutView="85" workbookViewId="0">
+      <selection activeCell="A94" sqref="A94:XFD94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -4457,7 +5264,7 @@
   <sheetData>
     <row r="1" spans="1:15" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B1" s="67"/>
       <c r="C1" s="8"/>
@@ -4482,15 +5289,18 @@
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="O3" s="11" t="s">
-        <v>65</v>
-      </c>
-    </row>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" ht="50.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="15" spans="1:15" ht="144" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="24" spans="1:13" ht="141" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="30" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B30" s="59" t="s">
         <v>10</v>
       </c>
       <c r="C30" s="34" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F30" s="61" t="s">
         <v>25</v>
@@ -4540,7 +5350,7 @@
         <v>22</v>
       </c>
       <c r="M31" s="68" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="32" spans="1:13" s="7" customFormat="1" ht="15" hidden="1" x14ac:dyDescent="0.2">
@@ -4618,7 +5428,7 @@
     </row>
     <row r="37" spans="1:13" s="7" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B37" s="31" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C37" s="32">
         <v>43582</v>
@@ -4630,11 +5440,11 @@
         <v>21</v>
       </c>
       <c r="F37" s="64">
-        <f t="shared" ref="F37:F94" si="0">IF(ISBLANK(C37),0,C37)</f>
+        <f t="shared" ref="F37:F125" si="0">IF(ISBLANK(C37),0,C37)</f>
         <v>43582</v>
       </c>
       <c r="G37" s="65">
-        <f t="shared" ref="G37:L101" si="1">IF(ISBLANK($D37),0,IF($E37=G$31,$D37-$C37+1,0))</f>
+        <f t="shared" ref="G37:L132" si="1">IF(ISBLANK($D37),0,IF($E37=G$31,$D37-$C37+1,0))</f>
         <v>5</v>
       </c>
       <c r="H37" s="65">
@@ -4658,10 +5468,10 @@
         <v>0</v>
       </c>
       <c r="M37" s="66" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="38" spans="1:13" s="7" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" s="7" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="30"/>
       <c r="B38" s="31"/>
       <c r="C38" s="32"/>
@@ -4679,7 +5489,7 @@
     <row r="39" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A39" s="30"/>
       <c r="B39" s="31" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C39" s="32">
         <v>43583</v>
@@ -4713,7 +5523,7 @@
         <v>0</v>
       </c>
       <c r="M39" s="66" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="40" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
@@ -4734,7 +5544,7 @@
     <row r="41" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A41" s="30"/>
       <c r="B41" s="31" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C41" s="32">
         <v>43583</v>
@@ -4773,7 +5583,7 @@
         <v>0</v>
       </c>
       <c r="M41" s="66" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="42" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
@@ -4794,7 +5604,7 @@
     <row r="43" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A43" s="30"/>
       <c r="B43" s="31" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C43" s="32">
         <v>43584</v>
@@ -4833,7 +5643,7 @@
         <v>0</v>
       </c>
       <c r="M43" s="66" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="44" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
@@ -4854,7 +5664,7 @@
     <row r="45" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A45" s="30"/>
       <c r="B45" s="31" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C45" s="32">
         <v>43584</v>
@@ -4863,7 +5673,7 @@
         <v>43585</v>
       </c>
       <c r="E45" s="12" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F45" s="64">
         <v>43584</v>
@@ -4887,7 +5697,7 @@
         <v>0</v>
       </c>
       <c r="M45" s="66" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="46" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
@@ -4908,7 +5718,7 @@
     <row r="47" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A47" s="30"/>
       <c r="B47" s="31" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C47" s="32">
         <v>43585</v>
@@ -4946,7 +5756,7 @@
         <v>0</v>
       </c>
       <c r="M47" s="66" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="48" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
@@ -4984,7 +5794,7 @@
     <row r="50" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A50" s="30"/>
       <c r="B50" s="31" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C50" s="32">
         <v>43583</v>
@@ -5024,7 +5834,7 @@
         <v>0</v>
       </c>
       <c r="M50" s="66" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="51" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
@@ -5045,7 +5855,7 @@
     <row r="52" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A52" s="30"/>
       <c r="B52" s="31" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C52" s="32">
         <v>43584</v>
@@ -5085,7 +5895,7 @@
         <v>0</v>
       </c>
       <c r="M52" s="66" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="53" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
@@ -5106,7 +5916,7 @@
     <row r="54" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A54" s="30"/>
       <c r="B54" s="31" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C54" s="32">
         <v>43585</v>
@@ -5146,7 +5956,7 @@
         <v>0</v>
       </c>
       <c r="M54" s="66" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="55" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
@@ -5167,7 +5977,7 @@
     <row r="56" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A56" s="30"/>
       <c r="B56" s="31" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C56" s="32">
         <v>43586</v>
@@ -5207,7 +6017,7 @@
         <v>0</v>
       </c>
       <c r="M56" s="66" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="57" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
@@ -5228,7 +6038,7 @@
     <row r="58" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A58" s="30"/>
       <c r="B58" s="31" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C58" s="32">
         <v>43586</v>
@@ -5268,7 +6078,7 @@
         <v>0</v>
       </c>
       <c r="M58" s="66" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="59" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
@@ -5336,7 +6146,7 @@
     <row r="63" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A63" s="30"/>
       <c r="B63" s="31" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C63" s="32">
         <v>43590</v>
@@ -5375,7 +6185,7 @@
         <v>0</v>
       </c>
       <c r="M63" s="66" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="64" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
@@ -5396,7 +6206,7 @@
     <row r="65" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A65" s="30"/>
       <c r="B65" s="31" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C65" s="32">
         <v>43590</v>
@@ -5429,7 +6239,7 @@
         <v>0</v>
       </c>
       <c r="M65" s="66" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="66" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
@@ -5450,7 +6260,7 @@
     <row r="67" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A67" s="30"/>
       <c r="B67" s="31" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C67" s="32">
         <v>43590</v>
@@ -5489,7 +6299,7 @@
         <v>0</v>
       </c>
       <c r="M67" s="66" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="68" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
@@ -5510,7 +6320,7 @@
     <row r="69" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A69" s="30"/>
       <c r="B69" s="31" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C69" s="32">
         <v>43591</v>
@@ -5543,7 +6353,7 @@
         <v>0</v>
       </c>
       <c r="M69" s="66" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="70" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
@@ -5564,7 +6374,7 @@
     <row r="71" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A71" s="30"/>
       <c r="B71" s="31" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C71" s="32">
         <v>43591</v>
@@ -5597,7 +6407,7 @@
         <v>0</v>
       </c>
       <c r="M71" s="66" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="72" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
@@ -5618,7 +6428,7 @@
     <row r="73" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A73" s="30"/>
       <c r="B73" s="31" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C73" s="32">
         <v>43592</v>
@@ -5651,7 +6461,7 @@
         <v>0</v>
       </c>
       <c r="M73" s="66" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="74" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
@@ -5672,7 +6482,7 @@
     <row r="75" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A75" s="30"/>
       <c r="B75" s="31" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C75" s="32">
         <v>43594</v>
@@ -5711,7 +6521,7 @@
         <v>0</v>
       </c>
       <c r="M75" s="66" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="76" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
@@ -5732,7 +6542,7 @@
     <row r="77" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A77" s="30"/>
       <c r="B77" s="31" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C77" s="32">
         <v>43594</v>
@@ -5765,7 +6575,7 @@
         <v>0</v>
       </c>
       <c r="M77" s="66" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="78" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
@@ -5786,7 +6596,7 @@
     <row r="79" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A79" s="30"/>
       <c r="B79" s="31" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C79" s="32">
         <v>43594</v>
@@ -5819,7 +6629,7 @@
         <v>0</v>
       </c>
       <c r="M79" s="66" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="80" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
@@ -5840,7 +6650,7 @@
     <row r="81" spans="1:13" s="7" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A81" s="30"/>
       <c r="B81" s="31" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C81" s="32">
         <v>43594</v>
@@ -5873,7 +6683,7 @@
         <v>0</v>
       </c>
       <c r="M81" s="69" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="82" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
@@ -5891,9 +6701,9 @@
       <c r="L82" s="66"/>
       <c r="M82" s="66"/>
     </row>
-    <row r="83" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:13" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A83" s="30" t="s">
-        <v>61</v>
+        <v>119</v>
       </c>
       <c r="B83" s="31"/>
       <c r="C83" s="32">
@@ -5922,8 +6732,7 @@
         <v>0</v>
       </c>
       <c r="J83" s="65">
-        <f t="shared" si="1"/>
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="K83" s="65">
         <f t="shared" si="1"/>
@@ -5936,16 +6745,22 @@
       <c r="M83" s="66"/>
     </row>
     <row r="84" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A84" s="30"/>
-      <c r="B84" s="31"/>
-      <c r="C84" s="32"/>
-      <c r="D84" s="33"/>
+      <c r="A84" s="70"/>
+      <c r="B84" s="31" t="s">
+        <v>100</v>
+      </c>
+      <c r="C84" s="32">
+        <v>43597</v>
+      </c>
+      <c r="D84" s="33">
+        <v>43599</v>
+      </c>
       <c r="E84" s="12" t="s">
         <v>24</v>
       </c>
       <c r="F84" s="64">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>43597</v>
       </c>
       <c r="G84" s="65">
         <f t="shared" si="1"/>
@@ -5961,7 +6776,7 @@
       </c>
       <c r="J84" s="65">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="K84" s="65">
         <f t="shared" si="1"/>
@@ -5971,60 +6786,70 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="M84" s="66"/>
+      <c r="M84" s="66" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="85" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A85" s="30"/>
+      <c r="A85" s="70"/>
       <c r="B85" s="31"/>
       <c r="C85" s="32"/>
       <c r="D85" s="33"/>
-      <c r="E85" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="F85" s="64">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G85" s="65">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="H85" s="65">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="I85" s="65">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J85" s="65">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="K85" s="65">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="L85" s="66">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
+      <c r="E85" s="12"/>
+      <c r="F85" s="64"/>
+      <c r="G85" s="65"/>
+      <c r="H85" s="65"/>
+      <c r="I85" s="65"/>
+      <c r="J85" s="65"/>
+      <c r="K85" s="65"/>
+      <c r="L85" s="66"/>
       <c r="M85" s="66"/>
     </row>
     <row r="86" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A86" s="30"/>
-      <c r="B86" s="31"/>
-      <c r="C86" s="32"/>
-      <c r="D86" s="33"/>
-      <c r="E86" s="12"/>
-      <c r="F86" s="64"/>
-      <c r="G86" s="65"/>
-      <c r="H86" s="65"/>
-      <c r="I86" s="65"/>
-      <c r="J86" s="65"/>
-      <c r="K86" s="65"/>
-      <c r="L86" s="66"/>
-      <c r="M86" s="66"/>
+      <c r="B86" s="31" t="s">
+        <v>102</v>
+      </c>
+      <c r="C86" s="32">
+        <v>43597</v>
+      </c>
+      <c r="D86" s="33">
+        <v>43600</v>
+      </c>
+      <c r="E86" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="F86" s="64">
+        <f t="shared" si="0"/>
+        <v>43597</v>
+      </c>
+      <c r="G86" s="65">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H86" s="65">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I86" s="65">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J86" s="65">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="K86" s="65">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L86" s="66">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M86" s="66" t="s">
+        <v>104</v>
+      </c>
     </row>
     <row r="87" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A87" s="30"/>
@@ -6039,22 +6864,52 @@
       <c r="J87" s="65"/>
       <c r="K87" s="65"/>
       <c r="L87" s="66"/>
-      <c r="M87" s="66"/>
     </row>
     <row r="88" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A88" s="30"/>
-      <c r="B88" s="31"/>
-      <c r="C88" s="32"/>
-      <c r="D88" s="33"/>
-      <c r="E88" s="12"/>
-      <c r="F88" s="64"/>
-      <c r="G88" s="65"/>
-      <c r="H88" s="65"/>
-      <c r="I88" s="65"/>
-      <c r="J88" s="65"/>
-      <c r="K88" s="65"/>
-      <c r="L88" s="66"/>
-      <c r="M88" s="66"/>
+      <c r="B88" s="31" t="s">
+        <v>103</v>
+      </c>
+      <c r="C88" s="32">
+        <v>43597</v>
+      </c>
+      <c r="D88" s="33">
+        <v>43600</v>
+      </c>
+      <c r="E88" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="F88" s="64">
+        <f t="shared" ref="F88" si="3">IF(ISBLANK(C88),0,C88)</f>
+        <v>43597</v>
+      </c>
+      <c r="G88" s="65">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H88" s="65">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I88" s="65">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J88" s="65">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="K88" s="65">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L88" s="66">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M88" s="66" t="s">
+        <v>105</v>
+      </c>
     </row>
     <row r="89" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A89" s="30"/>
@@ -6073,206 +6928,156 @@
     </row>
     <row r="90" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A90" s="30"/>
-      <c r="B90" s="31"/>
-      <c r="C90" s="32"/>
-      <c r="D90" s="33"/>
+      <c r="B90" s="31" t="s">
+        <v>108</v>
+      </c>
+      <c r="C90" s="32">
+        <v>43597</v>
+      </c>
+      <c r="D90" s="33">
+        <v>43598</v>
+      </c>
       <c r="E90" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="F90" s="64">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <v>24</v>
+      </c>
+      <c r="F90" s="32">
+        <v>43597</v>
       </c>
       <c r="G90" s="65">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H90" s="65">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="I90" s="65">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="J90" s="65">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K90" s="65">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="L90" s="66">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="M90" s="66"/>
+        <v>0</v>
+      </c>
+      <c r="M90" s="66" t="s">
+        <v>109</v>
+      </c>
     </row>
     <row r="91" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A91" s="30"/>
       <c r="B91" s="31"/>
       <c r="C91" s="32"/>
       <c r="D91" s="33"/>
-      <c r="E91" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="F91" s="64">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G91" s="65">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="H91" s="65">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="I91" s="65">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J91" s="65">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="K91" s="65">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="L91" s="66">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
+      <c r="E91" s="12"/>
+      <c r="F91" s="64"/>
+      <c r="G91" s="65"/>
+      <c r="H91" s="65"/>
+      <c r="I91" s="65"/>
+      <c r="J91" s="65"/>
+      <c r="K91" s="65"/>
+      <c r="L91" s="66"/>
       <c r="M91" s="66"/>
     </row>
     <row r="92" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A92" s="30" t="s">
-        <v>62</v>
-      </c>
-      <c r="B92" s="31"/>
+      <c r="A92" s="30"/>
+      <c r="B92" s="31" t="s">
+        <v>106</v>
+      </c>
       <c r="C92" s="32">
-        <v>43603</v>
+        <v>43598</v>
       </c>
       <c r="D92" s="33">
-        <v>43613</v>
+        <v>43601</v>
       </c>
       <c r="E92" s="12" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="F92" s="64">
-        <f>IF(ISBLANK(C92),0,C92)</f>
-        <v>43603</v>
+        <v>43598</v>
       </c>
       <c r="G92" s="65">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H92" s="65">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="I92" s="65">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="J92" s="65">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="K92" s="65">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="L92" s="66">
-        <f t="shared" si="1"/>
-        <v>11</v>
-      </c>
-      <c r="M92" s="66"/>
+        <v>0</v>
+      </c>
+      <c r="M92" s="66" t="s">
+        <v>104</v>
+      </c>
     </row>
     <row r="93" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A93" s="30"/>
       <c r="B93" s="31"/>
       <c r="C93" s="32"/>
       <c r="D93" s="33"/>
-      <c r="E93" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="F93" s="64">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G93" s="65">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="H93" s="65">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="I93" s="65">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J93" s="65">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="K93" s="65">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="L93" s="66">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="M93" s="66"/>
+      <c r="E93" s="12"/>
+      <c r="F93" s="64"/>
+      <c r="G93" s="65"/>
+      <c r="H93" s="65"/>
+      <c r="I93" s="65"/>
+      <c r="J93" s="65"/>
+      <c r="K93" s="65"/>
+      <c r="L93" s="66"/>
     </row>
     <row r="94" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A94" s="30"/>
-      <c r="B94" s="31"/>
-      <c r="C94" s="32"/>
-      <c r="D94" s="33"/>
-      <c r="E94" s="12" t="s">
-        <v>22</v>
+      <c r="B94" s="31" t="s">
+        <v>107</v>
+      </c>
+      <c r="C94" s="32">
+        <v>43598</v>
+      </c>
+      <c r="D94" s="33">
+        <v>43601</v>
+      </c>
+      <c r="E94" t="s">
+        <v>24</v>
       </c>
       <c r="F94" s="64">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <v>43598</v>
       </c>
       <c r="G94" s="65">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H94" s="65">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="I94" s="65">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="J94" s="65">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="K94" s="65">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="L94" s="66">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="M94" s="66"/>
+        <v>0</v>
+      </c>
+      <c r="M94" s="66" t="s">
+        <v>105</v>
+      </c>
     </row>
     <row r="95" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A95" s="30"/>
       <c r="B95" s="31"/>
       <c r="C95" s="32"/>
       <c r="D95" s="33"/>
-      <c r="E95" s="12"/>
+      <c r="E95"/>
       <c r="F95" s="64"/>
       <c r="G95" s="65"/>
       <c r="H95" s="65"/>
@@ -6284,90 +7089,103 @@
     </row>
     <row r="96" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A96" s="30"/>
-      <c r="B96" s="31"/>
-      <c r="C96" s="32"/>
-      <c r="D96" s="33"/>
+      <c r="B96" s="31" t="s">
+        <v>110</v>
+      </c>
+      <c r="C96" s="32">
+        <v>43598</v>
+      </c>
+      <c r="D96" s="33">
+        <v>43599</v>
+      </c>
       <c r="E96" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="F96" s="64"/>
-      <c r="G96" s="65"/>
-      <c r="H96" s="65"/>
-      <c r="I96" s="65"/>
-      <c r="J96" s="65"/>
-      <c r="K96" s="65"/>
-      <c r="L96" s="66"/>
-      <c r="M96" s="66"/>
+        <v>24</v>
+      </c>
+      <c r="F96" s="32">
+        <v>43598</v>
+      </c>
+      <c r="G96" s="65">
+        <v>0</v>
+      </c>
+      <c r="H96" s="65">
+        <v>0</v>
+      </c>
+      <c r="I96" s="65">
+        <v>0</v>
+      </c>
+      <c r="J96" s="65">
+        <v>2</v>
+      </c>
+      <c r="K96" s="65">
+        <v>0</v>
+      </c>
+      <c r="L96" s="66">
+        <v>0</v>
+      </c>
+      <c r="M96" s="66" t="s">
+        <v>111</v>
+      </c>
     </row>
     <row r="97" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A97" s="30" t="s">
-        <v>84</v>
-      </c>
+      <c r="A97" s="30"/>
       <c r="B97" s="31"/>
-      <c r="C97" s="32">
-        <v>43610</v>
-      </c>
-      <c r="D97" s="33">
-        <v>43613</v>
-      </c>
-      <c r="E97" s="12" t="s">
-        <v>83</v>
-      </c>
-      <c r="F97" s="64">
-        <f t="shared" ref="F97" si="3">IF(ISBLANK(C97),0,C97)</f>
-        <v>43610</v>
-      </c>
-      <c r="G97" s="65">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="H97" s="65">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="I97" s="65">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J97" s="65">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="K97" s="65">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="L97" s="66">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
+      <c r="C97" s="32"/>
+      <c r="D97" s="33"/>
+      <c r="E97" s="12"/>
+      <c r="F97" s="64"/>
+      <c r="G97" s="65"/>
+      <c r="H97" s="65"/>
+      <c r="I97" s="65"/>
+      <c r="J97" s="65"/>
+      <c r="K97" s="65"/>
+      <c r="L97" s="66"/>
       <c r="M97" s="66"/>
     </row>
     <row r="98" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A98" s="30"/>
-      <c r="B98" s="31"/>
-      <c r="C98" s="32"/>
-      <c r="D98" s="33"/>
+      <c r="B98" s="31" t="s">
+        <v>112</v>
+      </c>
+      <c r="C98" s="32">
+        <v>43598</v>
+      </c>
+      <c r="D98" s="33">
+        <v>43599</v>
+      </c>
       <c r="E98" s="12" t="s">
-        <v>83</v>
-      </c>
-      <c r="F98" s="64"/>
-      <c r="G98" s="65"/>
-      <c r="H98" s="65"/>
-      <c r="I98" s="65"/>
-      <c r="J98" s="65"/>
-      <c r="K98" s="65"/>
-      <c r="L98" s="66"/>
-      <c r="M98" s="66"/>
+        <v>24</v>
+      </c>
+      <c r="F98" s="32">
+        <v>43598</v>
+      </c>
+      <c r="G98" s="65">
+        <v>0</v>
+      </c>
+      <c r="H98" s="65">
+        <v>0</v>
+      </c>
+      <c r="I98" s="65">
+        <v>0</v>
+      </c>
+      <c r="J98" s="65">
+        <v>2</v>
+      </c>
+      <c r="K98" s="65">
+        <v>0</v>
+      </c>
+      <c r="L98" s="66">
+        <v>0</v>
+      </c>
+      <c r="M98" s="66" t="s">
+        <v>109</v>
+      </c>
     </row>
     <row r="99" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A99" s="30"/>
       <c r="B99" s="31"/>
       <c r="C99" s="32"/>
       <c r="D99" s="33"/>
-      <c r="E99" s="12" t="s">
-        <v>83</v>
-      </c>
+      <c r="E99" s="12"/>
       <c r="F99" s="64"/>
       <c r="G99" s="65"/>
       <c r="H99" s="65"/>
@@ -6379,149 +7197,1009 @@
     </row>
     <row r="100" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A100" s="30"/>
-      <c r="B100" s="31"/>
-      <c r="C100" s="32"/>
-      <c r="D100" s="33"/>
+      <c r="B100" s="31" t="s">
+        <v>113</v>
+      </c>
+      <c r="C100" s="32">
+        <v>43599</v>
+      </c>
+      <c r="D100" s="33">
+        <v>43600</v>
+      </c>
       <c r="E100" s="12" t="s">
-        <v>83</v>
-      </c>
-      <c r="F100" s="64"/>
-      <c r="G100" s="65"/>
-      <c r="H100" s="65"/>
-      <c r="I100" s="65"/>
-      <c r="J100" s="65"/>
-      <c r="K100" s="65"/>
-      <c r="L100" s="66"/>
-      <c r="M100" s="66"/>
+        <v>24</v>
+      </c>
+      <c r="F100" s="32">
+        <v>43599</v>
+      </c>
+      <c r="G100" s="65">
+        <v>0</v>
+      </c>
+      <c r="H100" s="65">
+        <v>0</v>
+      </c>
+      <c r="I100" s="65">
+        <v>0</v>
+      </c>
+      <c r="J100" s="65">
+        <v>2</v>
+      </c>
+      <c r="K100" s="65">
+        <v>0</v>
+      </c>
+      <c r="L100" s="66">
+        <v>0</v>
+      </c>
+      <c r="M100" s="66" t="s">
+        <v>109</v>
+      </c>
     </row>
     <row r="101" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A101" s="30"/>
       <c r="B101" s="31"/>
       <c r="C101" s="32"/>
       <c r="D101" s="33"/>
-      <c r="E101" s="12" t="s">
+      <c r="E101" s="12"/>
+      <c r="F101" s="64"/>
+      <c r="G101" s="65"/>
+      <c r="H101" s="65"/>
+      <c r="I101" s="65"/>
+      <c r="J101" s="65"/>
+      <c r="K101" s="65"/>
+      <c r="L101" s="66"/>
+      <c r="M101" s="66"/>
+    </row>
+    <row r="102" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A102" s="30"/>
+      <c r="B102" s="31" t="s">
+        <v>114</v>
+      </c>
+      <c r="C102" s="32">
+        <v>43599</v>
+      </c>
+      <c r="D102" s="33">
+        <v>43601</v>
+      </c>
+      <c r="E102" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="F102" s="64">
+        <v>43599</v>
+      </c>
+      <c r="G102" s="65">
+        <v>0</v>
+      </c>
+      <c r="H102" s="65">
+        <v>0</v>
+      </c>
+      <c r="I102" s="65">
+        <v>0</v>
+      </c>
+      <c r="J102" s="65">
+        <v>3</v>
+      </c>
+      <c r="K102" s="65">
+        <v>0</v>
+      </c>
+      <c r="L102" s="66">
+        <v>0</v>
+      </c>
+      <c r="M102" s="66" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="103" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A103" s="30"/>
+      <c r="B103" s="31"/>
+      <c r="C103" s="32"/>
+      <c r="D103" s="33"/>
+      <c r="E103" s="12"/>
+      <c r="F103" s="64"/>
+      <c r="G103" s="65"/>
+      <c r="H103" s="65"/>
+      <c r="I103" s="65"/>
+      <c r="J103" s="65"/>
+      <c r="K103" s="65"/>
+      <c r="L103" s="66"/>
+    </row>
+    <row r="104" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A104" s="30"/>
+      <c r="B104" s="31" t="s">
+        <v>115</v>
+      </c>
+      <c r="C104" s="32">
+        <v>43599</v>
+      </c>
+      <c r="D104" s="33">
+        <v>43601</v>
+      </c>
+      <c r="E104" t="s">
+        <v>24</v>
+      </c>
+      <c r="F104" s="64">
+        <v>43599</v>
+      </c>
+      <c r="G104" s="65">
+        <v>0</v>
+      </c>
+      <c r="H104" s="65">
+        <v>0</v>
+      </c>
+      <c r="I104" s="65">
+        <v>0</v>
+      </c>
+      <c r="J104" s="65">
+        <v>3</v>
+      </c>
+      <c r="K104" s="65">
+        <v>0</v>
+      </c>
+      <c r="L104" s="66">
+        <v>0</v>
+      </c>
+      <c r="M104" s="66" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="105" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A105" s="30"/>
+      <c r="B105" s="31"/>
+      <c r="C105" s="32"/>
+      <c r="D105" s="33"/>
+      <c r="E105"/>
+      <c r="F105" s="64"/>
+      <c r="G105" s="65"/>
+      <c r="H105" s="65"/>
+      <c r="I105" s="65"/>
+      <c r="J105" s="65"/>
+      <c r="K105" s="65"/>
+      <c r="L105" s="66"/>
+      <c r="M105" s="66"/>
+    </row>
+    <row r="106" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A106" s="30"/>
+      <c r="B106" s="31" t="s">
+        <v>116</v>
+      </c>
+      <c r="C106" s="32">
+        <v>43600</v>
+      </c>
+      <c r="D106" s="33">
+        <v>43601</v>
+      </c>
+      <c r="E106" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="F106" s="32">
+        <v>43600</v>
+      </c>
+      <c r="G106" s="65">
+        <v>0</v>
+      </c>
+      <c r="H106" s="65">
+        <v>0</v>
+      </c>
+      <c r="I106" s="65">
+        <v>0</v>
+      </c>
+      <c r="J106" s="65">
+        <v>2</v>
+      </c>
+      <c r="K106" s="65">
+        <v>0</v>
+      </c>
+      <c r="L106" s="66">
+        <v>0</v>
+      </c>
+      <c r="M106" s="66" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="107" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A107" s="30"/>
+      <c r="B107" s="31"/>
+      <c r="C107" s="32"/>
+      <c r="D107" s="33"/>
+      <c r="E107"/>
+      <c r="F107" s="64"/>
+      <c r="G107" s="65"/>
+      <c r="H107" s="65"/>
+      <c r="I107" s="65"/>
+      <c r="J107" s="65"/>
+      <c r="K107" s="65"/>
+      <c r="L107" s="66"/>
+      <c r="M107" s="66"/>
+    </row>
+    <row r="108" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A108" s="30"/>
+      <c r="B108" s="31" t="s">
+        <v>116</v>
+      </c>
+      <c r="C108" s="32">
+        <v>43600</v>
+      </c>
+      <c r="D108" s="33">
+        <v>43601</v>
+      </c>
+      <c r="E108" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="F108" s="32">
+        <v>43600</v>
+      </c>
+      <c r="G108" s="65">
+        <v>0</v>
+      </c>
+      <c r="H108" s="65">
+        <v>0</v>
+      </c>
+      <c r="I108" s="65">
+        <v>0</v>
+      </c>
+      <c r="J108" s="65">
+        <v>2</v>
+      </c>
+      <c r="K108" s="65">
+        <v>0</v>
+      </c>
+      <c r="L108" s="66">
+        <v>0</v>
+      </c>
+      <c r="M108" s="66" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="109" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A109" s="30"/>
+      <c r="B109" s="31"/>
+      <c r="C109" s="32"/>
+      <c r="D109" s="33"/>
+      <c r="E109"/>
+      <c r="F109" s="64"/>
+      <c r="G109" s="65"/>
+      <c r="H109" s="65"/>
+      <c r="I109" s="65"/>
+      <c r="J109" s="65"/>
+      <c r="K109" s="65"/>
+      <c r="L109" s="66"/>
+      <c r="M109" s="66"/>
+    </row>
+    <row r="110" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A110" s="30"/>
+      <c r="B110" s="31" t="s">
+        <v>117</v>
+      </c>
+      <c r="C110" s="32">
+        <v>43600</v>
+      </c>
+      <c r="D110" s="33">
+        <v>43601</v>
+      </c>
+      <c r="E110" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="F110" s="64">
+        <v>43599</v>
+      </c>
+      <c r="G110" s="65">
+        <v>0</v>
+      </c>
+      <c r="H110" s="65">
+        <v>0</v>
+      </c>
+      <c r="I110" s="65">
+        <v>0</v>
+      </c>
+      <c r="J110" s="65">
+        <v>3</v>
+      </c>
+      <c r="K110" s="65">
+        <v>0</v>
+      </c>
+      <c r="L110" s="66">
+        <v>0</v>
+      </c>
+      <c r="M110" s="66" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="111" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A111" s="30"/>
+      <c r="B111" s="31"/>
+      <c r="C111" s="32"/>
+      <c r="D111" s="33"/>
+      <c r="E111" s="12"/>
+      <c r="F111" s="64"/>
+      <c r="G111" s="65"/>
+      <c r="H111" s="65"/>
+      <c r="I111" s="65"/>
+      <c r="J111" s="65"/>
+      <c r="K111" s="65"/>
+      <c r="L111" s="66"/>
+    </row>
+    <row r="112" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A112" s="30"/>
+      <c r="B112" s="31" t="s">
+        <v>118</v>
+      </c>
+      <c r="C112" s="32">
+        <v>43600</v>
+      </c>
+      <c r="D112" s="33">
+        <v>43601</v>
+      </c>
+      <c r="E112" t="s">
+        <v>24</v>
+      </c>
+      <c r="F112" s="64">
+        <v>43599</v>
+      </c>
+      <c r="G112" s="65">
+        <v>0</v>
+      </c>
+      <c r="H112" s="65">
+        <v>0</v>
+      </c>
+      <c r="I112" s="65">
+        <v>0</v>
+      </c>
+      <c r="J112" s="65">
+        <v>3</v>
+      </c>
+      <c r="K112" s="65">
+        <v>0</v>
+      </c>
+      <c r="L112" s="66">
+        <v>0</v>
+      </c>
+      <c r="M112" s="66" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="113" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A113" s="30"/>
+      <c r="B113" s="31"/>
+      <c r="C113" s="32"/>
+      <c r="D113" s="33"/>
+      <c r="E113"/>
+      <c r="F113" s="64"/>
+      <c r="G113" s="65"/>
+      <c r="H113" s="65"/>
+      <c r="I113" s="65"/>
+      <c r="J113" s="65"/>
+      <c r="K113" s="65"/>
+      <c r="L113" s="66"/>
+      <c r="M113" s="66"/>
+    </row>
+    <row r="114" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A114" s="30"/>
+      <c r="B114" s="31" t="s">
+        <v>95</v>
+      </c>
+      <c r="C114" s="32">
+        <v>43600</v>
+      </c>
+      <c r="D114" s="32">
+        <v>43600</v>
+      </c>
+      <c r="E114" t="s">
+        <v>24</v>
+      </c>
+      <c r="F114" s="64">
+        <v>43600</v>
+      </c>
+      <c r="G114" s="65">
+        <v>0</v>
+      </c>
+      <c r="H114" s="65">
+        <v>0</v>
+      </c>
+      <c r="I114" s="65">
+        <v>0</v>
+      </c>
+      <c r="J114" s="65">
+        <v>1</v>
+      </c>
+      <c r="K114" s="65">
+        <v>0</v>
+      </c>
+      <c r="L114" s="66">
+        <v>0</v>
+      </c>
+      <c r="M114" s="66" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="115" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A115" s="30"/>
+      <c r="B115" s="31"/>
+      <c r="C115" s="32"/>
+      <c r="D115" s="33"/>
+      <c r="E115"/>
+      <c r="F115" s="64"/>
+      <c r="G115" s="65"/>
+      <c r="H115" s="65"/>
+      <c r="I115" s="65"/>
+      <c r="J115" s="65"/>
+      <c r="K115" s="65"/>
+      <c r="L115" s="66"/>
+      <c r="M115" s="66"/>
+    </row>
+    <row r="116" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A116" s="30"/>
+      <c r="B116" s="31" t="s">
+        <v>96</v>
+      </c>
+      <c r="C116" s="32">
+        <v>43600</v>
+      </c>
+      <c r="D116" s="32">
+        <v>43601</v>
+      </c>
+      <c r="E116" t="s">
+        <v>24</v>
+      </c>
+      <c r="F116" s="64">
+        <v>43600</v>
+      </c>
+      <c r="G116" s="65">
+        <v>0</v>
+      </c>
+      <c r="H116" s="65">
+        <v>0</v>
+      </c>
+      <c r="I116" s="65">
+        <v>0</v>
+      </c>
+      <c r="J116" s="65">
+        <v>2</v>
+      </c>
+      <c r="K116" s="65">
+        <v>0</v>
+      </c>
+      <c r="L116" s="66">
+        <v>0</v>
+      </c>
+      <c r="M116" s="66" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="117" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A117" s="30"/>
+      <c r="B117" s="31"/>
+      <c r="C117" s="32"/>
+      <c r="D117" s="33"/>
+      <c r="E117"/>
+      <c r="F117" s="64"/>
+      <c r="G117" s="65"/>
+      <c r="H117" s="65"/>
+      <c r="I117" s="65"/>
+      <c r="J117" s="65"/>
+      <c r="K117" s="65"/>
+      <c r="L117" s="66"/>
+      <c r="M117" s="66"/>
+    </row>
+    <row r="118" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A118" s="30"/>
+      <c r="B118" s="31" t="s">
+        <v>120</v>
+      </c>
+      <c r="C118" s="32">
+        <v>43600</v>
+      </c>
+      <c r="D118" s="33">
+        <v>43602</v>
+      </c>
+      <c r="E118" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="F118" s="32">
+        <v>43600</v>
+      </c>
+      <c r="G118" s="65">
+        <v>0</v>
+      </c>
+      <c r="H118" s="65">
+        <v>0</v>
+      </c>
+      <c r="I118" s="65">
+        <v>0</v>
+      </c>
+      <c r="J118" s="65">
+        <v>3</v>
+      </c>
+      <c r="K118" s="65">
+        <v>0</v>
+      </c>
+      <c r="L118" s="66">
+        <v>0</v>
+      </c>
+      <c r="M118" s="66" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="119" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A119" s="30"/>
+      <c r="B119" s="31"/>
+      <c r="C119" s="32"/>
+      <c r="D119" s="33"/>
+      <c r="E119"/>
+      <c r="F119" s="64"/>
+      <c r="G119" s="65"/>
+      <c r="H119" s="65"/>
+      <c r="I119" s="65"/>
+      <c r="J119" s="65"/>
+      <c r="K119" s="65"/>
+      <c r="L119" s="66"/>
+      <c r="M119" s="66"/>
+    </row>
+    <row r="120" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A120" s="30"/>
+      <c r="B120" s="31" t="s">
+        <v>121</v>
+      </c>
+      <c r="C120" s="32">
+        <v>43601</v>
+      </c>
+      <c r="D120" s="33">
+        <v>43602</v>
+      </c>
+      <c r="E120" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="F120" s="32">
+        <v>43601</v>
+      </c>
+      <c r="G120" s="65">
+        <v>0</v>
+      </c>
+      <c r="H120" s="65">
+        <v>0</v>
+      </c>
+      <c r="I120" s="65">
+        <v>0</v>
+      </c>
+      <c r="J120" s="65">
+        <v>2</v>
+      </c>
+      <c r="K120" s="65">
+        <v>0</v>
+      </c>
+      <c r="L120" s="66">
+        <v>0</v>
+      </c>
+      <c r="M120" s="66" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="121" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A121" s="30"/>
+      <c r="B121" s="31"/>
+      <c r="C121" s="32"/>
+      <c r="D121" s="33"/>
+      <c r="E121"/>
+      <c r="F121" s="64"/>
+      <c r="G121" s="65"/>
+      <c r="H121" s="65"/>
+      <c r="I121" s="65"/>
+      <c r="J121" s="65"/>
+      <c r="K121" s="65"/>
+      <c r="L121" s="66"/>
+      <c r="M121" s="66"/>
+    </row>
+    <row r="122" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A122" s="30"/>
+      <c r="B122" s="31"/>
+      <c r="C122" s="32"/>
+      <c r="D122" s="33"/>
+      <c r="E122" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="F122" s="64">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G122" s="65">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H122" s="65">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I122" s="65">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J122" s="65">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K122" s="65">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L122" s="66">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M122" s="66"/>
+    </row>
+    <row r="123" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A123" s="30" t="s">
+        <v>61</v>
+      </c>
+      <c r="B123" s="31"/>
+      <c r="C123" s="32">
+        <v>43603</v>
+      </c>
+      <c r="D123" s="33">
+        <v>43613</v>
+      </c>
+      <c r="E123" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="F123" s="64">
+        <f>IF(ISBLANK(C123),0,C123)</f>
+        <v>43603</v>
+      </c>
+      <c r="G123" s="65">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H123" s="65">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I123" s="65">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J123" s="65">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K123" s="65">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L123" s="66">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+      <c r="M123" s="66"/>
+    </row>
+    <row r="124" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A124" s="30"/>
+      <c r="B124" s="31"/>
+      <c r="C124" s="32"/>
+      <c r="D124" s="33"/>
+      <c r="E124" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="F124" s="64">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G124" s="65">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H124" s="65">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I124" s="65">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J124" s="65">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K124" s="65">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L124" s="66">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M124" s="66"/>
+    </row>
+    <row r="125" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A125" s="30"/>
+      <c r="B125" s="31"/>
+      <c r="C125" s="32"/>
+      <c r="D125" s="33"/>
+      <c r="E125" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="F125" s="64">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G125" s="65">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H125" s="65">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I125" s="65">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J125" s="65">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K125" s="65">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L125" s="66">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M125" s="66"/>
+    </row>
+    <row r="126" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A126" s="30"/>
+      <c r="B126" s="31"/>
+      <c r="C126" s="32"/>
+      <c r="D126" s="33"/>
+      <c r="E126" s="12"/>
+      <c r="F126" s="64"/>
+      <c r="G126" s="65"/>
+      <c r="H126" s="65"/>
+      <c r="I126" s="65"/>
+      <c r="J126" s="65"/>
+      <c r="K126" s="65"/>
+      <c r="L126" s="66"/>
+      <c r="M126" s="66"/>
+    </row>
+    <row r="127" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A127" s="30"/>
+      <c r="B127" s="31"/>
+      <c r="C127" s="32"/>
+      <c r="D127" s="33"/>
+      <c r="E127" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="F127" s="64"/>
+      <c r="G127" s="65"/>
+      <c r="H127" s="65"/>
+      <c r="I127" s="65"/>
+      <c r="J127" s="65"/>
+      <c r="K127" s="65"/>
+      <c r="L127" s="66"/>
+      <c r="M127" s="66"/>
+    </row>
+    <row r="128" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A128" s="30" t="s">
         <v>83</v>
       </c>
-      <c r="F101" s="64">
-        <f>IF(ISBLANK(C101),0,C101)</f>
-        <v>0</v>
-      </c>
-      <c r="G101" s="65">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="H101" s="65">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="I101" s="65">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J101" s="65">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="K101" s="65">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="L101" s="66">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="M101" s="66"/>
-    </row>
-    <row r="102" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A102" s="24"/>
-      <c r="B102" s="25"/>
-      <c r="C102" s="26" t="s">
+      <c r="B128" s="31"/>
+      <c r="C128" s="32">
+        <v>43610</v>
+      </c>
+      <c r="D128" s="33">
+        <v>43613</v>
+      </c>
+      <c r="E128" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="F128" s="64">
+        <f t="shared" ref="F128" si="4">IF(ISBLANK(C128),0,C128)</f>
+        <v>43610</v>
+      </c>
+      <c r="G128" s="65">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H128" s="65">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I128" s="65">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J128" s="65">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K128" s="65">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L128" s="66">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M128" s="66"/>
+    </row>
+    <row r="129" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A129" s="30"/>
+      <c r="B129" s="31"/>
+      <c r="C129" s="32"/>
+      <c r="D129" s="33"/>
+      <c r="E129" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="F129" s="64"/>
+      <c r="G129" s="65"/>
+      <c r="H129" s="65"/>
+      <c r="I129" s="65"/>
+      <c r="J129" s="65"/>
+      <c r="K129" s="65"/>
+      <c r="L129" s="66"/>
+      <c r="M129" s="66"/>
+    </row>
+    <row r="130" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A130" s="30"/>
+      <c r="B130" s="31"/>
+      <c r="C130" s="32"/>
+      <c r="D130" s="33"/>
+      <c r="E130" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="F130" s="64"/>
+      <c r="G130" s="65"/>
+      <c r="H130" s="65"/>
+      <c r="I130" s="65"/>
+      <c r="J130" s="65"/>
+      <c r="K130" s="65"/>
+      <c r="L130" s="66"/>
+      <c r="M130" s="66"/>
+    </row>
+    <row r="131" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A131" s="30"/>
+      <c r="B131" s="31"/>
+      <c r="C131" s="32"/>
+      <c r="D131" s="33"/>
+      <c r="E131" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="F131" s="64"/>
+      <c r="G131" s="65"/>
+      <c r="H131" s="65"/>
+      <c r="I131" s="65"/>
+      <c r="J131" s="65"/>
+      <c r="K131" s="65"/>
+      <c r="L131" s="66"/>
+      <c r="M131" s="66"/>
+    </row>
+    <row r="132" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A132" s="30"/>
+      <c r="B132" s="31"/>
+      <c r="C132" s="32"/>
+      <c r="D132" s="33"/>
+      <c r="E132" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="F132" s="64">
+        <f>IF(ISBLANK(C132),0,C132)</f>
+        <v>0</v>
+      </c>
+      <c r="G132" s="65">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H132" s="65">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I132" s="65">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J132" s="65">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K132" s="65">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L132" s="66">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M132" s="66"/>
+    </row>
+    <row r="133" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A133" s="24"/>
+      <c r="B133" s="25"/>
+      <c r="C133" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="D102" s="27"/>
-      <c r="E102" s="27"/>
-      <c r="F102" s="28"/>
-      <c r="G102" s="28"/>
-      <c r="H102" s="28"/>
-      <c r="I102" s="28"/>
-      <c r="J102" s="28"/>
-      <c r="K102" s="28"/>
-      <c r="L102" s="29"/>
-      <c r="M102" s="29"/>
-    </row>
-    <row r="106" spans="1:13" ht="24" x14ac:dyDescent="0.2">
-      <c r="B106" s="19" t="s">
+      <c r="D133" s="27"/>
+      <c r="E133" s="27"/>
+      <c r="F133" s="28"/>
+      <c r="G133" s="28"/>
+      <c r="H133" s="28"/>
+      <c r="I133" s="28"/>
+      <c r="J133" s="28"/>
+      <c r="K133" s="28"/>
+      <c r="L133" s="29"/>
+      <c r="M133" s="29"/>
+    </row>
+    <row r="137" spans="1:13" ht="24" x14ac:dyDescent="0.2">
+      <c r="B137" s="19" t="s">
         <v>46</v>
       </c>
-      <c r="C106" s="19" t="s">
+      <c r="C137" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="D106" s="60" t="s">
+      <c r="D137" s="60" t="s">
         <v>48</v>
       </c>
-      <c r="E106" s="60" t="s">
+      <c r="E137" s="60" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="107" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B107" s="31" t="s">
+    <row r="138" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B138" s="31" t="s">
         <v>42</v>
       </c>
-      <c r="C107" s="57">
+      <c r="C138" s="57">
         <v>43588</v>
       </c>
-      <c r="D107" s="58">
+      <c r="D138" s="58">
         <v>0.5</v>
       </c>
-      <c r="E107" s="58">
+      <c r="E138" s="58">
         <v>0.95</v>
       </c>
     </row>
-    <row r="108" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B108" s="31" t="s">
+    <row r="139" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B139" s="31" t="s">
         <v>43</v>
       </c>
-      <c r="C108" s="57">
+      <c r="C139" s="57">
         <v>43595</v>
       </c>
-      <c r="D108" s="58">
+      <c r="D139" s="58">
         <v>0.25</v>
       </c>
-      <c r="E108" s="58">
+      <c r="E139" s="58">
         <v>0.95</v>
       </c>
     </row>
-    <row r="109" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B109" s="31" t="s">
+    <row r="140" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B140" s="31" t="s">
         <v>44</v>
       </c>
-      <c r="C109" s="57">
+      <c r="C140" s="57">
         <v>43602</v>
       </c>
-      <c r="D109" s="58">
+      <c r="D140" s="58">
         <v>0.1</v>
       </c>
-      <c r="E109" s="58">
+      <c r="E140" s="58">
         <v>0.95</v>
       </c>
     </row>
-    <row r="110" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B110" s="31" t="s">
+    <row r="141" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B141" s="31" t="s">
         <v>45</v>
       </c>
-      <c r="C110" s="57">
+      <c r="C141" s="57">
         <v>43609</v>
       </c>
-      <c r="D110" s="58">
+      <c r="D141" s="58">
         <v>0.3</v>
       </c>
-      <c r="E110" s="58">
+      <c r="E141" s="58">
         <v>0.95</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" sqref="E32:E101">
+    <dataValidation type="list" allowBlank="1" sqref="E32:E132">
       <formula1>$G$31:$L$31</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Added tasks of Khadeja and Sondos
Added tasks of Khadeja and Sondos
</commit_message>
<xml_diff>
--- a/PM/Project schedule.xlsx
+++ b/PM/Project schedule.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="133">
   <si>
     <t>HELP</t>
   </si>
@@ -219,9 +219,6 @@
   </si>
   <si>
     <t>PM</t>
-  </si>
-  <si>
-    <t>Testing</t>
   </si>
   <si>
     <t>27/4/2019</t>
@@ -406,6 +403,42 @@
   </si>
   <si>
     <t>Design.TC.Previous TR Page.Front</t>
+  </si>
+  <si>
+    <t>Complete TC for Reg</t>
+  </si>
+  <si>
+    <t>sondos</t>
+  </si>
+  <si>
+    <t>khadeja</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Complete TC for Accounts </t>
+  </si>
+  <si>
+    <t>Design admin TC</t>
+  </si>
+  <si>
+    <t>Optmize login TC</t>
+  </si>
+  <si>
+    <t>Complete TC for prev Trans</t>
+  </si>
+  <si>
+    <t>Design transfer TC</t>
+  </si>
+  <si>
+    <t>Review on admin TC</t>
+  </si>
+  <si>
+    <t>Review on transfer and login TC</t>
+  </si>
+  <si>
+    <t>Update TC up on review comments</t>
+  </si>
+  <si>
+    <t>Review on Reg-PT-Accounts TC</t>
   </si>
 </sst>
 </file>
@@ -1220,9 +1253,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:f>ProjectTimeline!$A$32:$B$133</c:f>
+              <c:f>ProjectTimeline!$A$32:$B$153</c:f>
               <c:multiLvlStrCache>
-                <c:ptCount val="97"/>
+                <c:ptCount val="117"/>
                 <c:lvl>
                   <c:pt idx="5">
                     <c:v>Responsibility Assignment Matrix</c:v>
@@ -1343,6 +1376,42 @@
                   </c:pt>
                   <c:pt idx="88">
                     <c:v>Design.TC.Previous TR Page.Front</c:v>
+                  </c:pt>
+                  <c:pt idx="92">
+                    <c:v>Optmize login TC</c:v>
+                  </c:pt>
+                  <c:pt idx="94">
+                    <c:v>Complete TC for Reg</c:v>
+                  </c:pt>
+                  <c:pt idx="96">
+                    <c:v>Complete TC for Accounts </c:v>
+                  </c:pt>
+                  <c:pt idx="98">
+                    <c:v>Design admin TC</c:v>
+                  </c:pt>
+                  <c:pt idx="100">
+                    <c:v>Complete TC for prev Trans</c:v>
+                  </c:pt>
+                  <c:pt idx="102">
+                    <c:v>Design transfer TC</c:v>
+                  </c:pt>
+                  <c:pt idx="104">
+                    <c:v>Review on admin TC</c:v>
+                  </c:pt>
+                  <c:pt idx="106">
+                    <c:v>Review on transfer and login TC</c:v>
+                  </c:pt>
+                  <c:pt idx="108">
+                    <c:v>Review on Reg-PT-Accounts TC</c:v>
+                  </c:pt>
+                  <c:pt idx="110">
+                    <c:v>Update TC up on review comments</c:v>
+                  </c:pt>
+                  <c:pt idx="112">
+                    <c:v>Update TC up on review comments</c:v>
+                  </c:pt>
+                  <c:pt idx="114">
+                    <c:v>Update Schedule</c:v>
                   </c:pt>
                 </c:lvl>
                 <c:lvl>
@@ -1359,9 +1428,9 @@
                     <c:v>Development and Testing</c:v>
                   </c:pt>
                   <c:pt idx="91">
-                    <c:v>Testing</c:v>
-                  </c:pt>
-                  <c:pt idx="96">
+                    <c:v>Development and Testing</c:v>
+                  </c:pt>
+                  <c:pt idx="116">
                     <c:v>Delivery</c:v>
                   </c:pt>
                 </c:lvl>
@@ -1370,10 +1439,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>ProjectTimeline!$F$32:$F$133</c:f>
+              <c:f>ProjectTimeline!$F$32:$F$153</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="102"/>
+                <c:ptCount val="122"/>
                 <c:pt idx="5" formatCode="m/d/yy;@">
                   <c:v>43582</c:v>
                 </c:pt>
@@ -1500,19 +1569,46 @@
                 <c:pt idx="90" formatCode="m/d/yy;@">
                   <c:v>0</c:v>
                 </c:pt>
-                <c:pt idx="91" formatCode="m/d/yy;@">
-                  <c:v>43603</c:v>
-                </c:pt>
                 <c:pt idx="92" formatCode="m/d/yy;@">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="93" formatCode="m/d/yy;@">
-                  <c:v>0</c:v>
+                  <c:v>43604</c:v>
+                </c:pt>
+                <c:pt idx="94" formatCode="m/d/yy;@">
+                  <c:v>43604</c:v>
                 </c:pt>
                 <c:pt idx="96" formatCode="m/d/yy;@">
+                  <c:v>43605</c:v>
+                </c:pt>
+                <c:pt idx="98" formatCode="m/d/yy;@">
+                  <c:v>43605</c:v>
+                </c:pt>
+                <c:pt idx="100" formatCode="m/d/yy;@">
+                  <c:v>43606</c:v>
+                </c:pt>
+                <c:pt idx="102" formatCode="m/d/yy;@">
+                  <c:v>43607</c:v>
+                </c:pt>
+                <c:pt idx="104" formatCode="m/d/yy;@">
+                  <c:v>43607</c:v>
+                </c:pt>
+                <c:pt idx="106" formatCode="m/d/yy;@">
+                  <c:v>43608</c:v>
+                </c:pt>
+                <c:pt idx="108" formatCode="m/d/yy;@">
+                  <c:v>43608</c:v>
+                </c:pt>
+                <c:pt idx="110" formatCode="m/d/yy;@">
+                  <c:v>43608</c:v>
+                </c:pt>
+                <c:pt idx="112" formatCode="m/d/yy;@">
+                  <c:v>43609</c:v>
+                </c:pt>
+                <c:pt idx="114" formatCode="m/d/yy;@">
+                  <c:v>43609</c:v>
+                </c:pt>
+                <c:pt idx="116" formatCode="m/d/yy;@">
                   <c:v>43610</c:v>
                 </c:pt>
-                <c:pt idx="100" formatCode="m/d/yy;@">
+                <c:pt idx="120" formatCode="m/d/yy;@">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -1550,9 +1646,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:f>ProjectTimeline!$A$32:$B$133</c:f>
+              <c:f>ProjectTimeline!$A$32:$B$153</c:f>
               <c:multiLvlStrCache>
-                <c:ptCount val="97"/>
+                <c:ptCount val="117"/>
                 <c:lvl>
                   <c:pt idx="5">
                     <c:v>Responsibility Assignment Matrix</c:v>
@@ -1673,6 +1769,42 @@
                   </c:pt>
                   <c:pt idx="88">
                     <c:v>Design.TC.Previous TR Page.Front</c:v>
+                  </c:pt>
+                  <c:pt idx="92">
+                    <c:v>Optmize login TC</c:v>
+                  </c:pt>
+                  <c:pt idx="94">
+                    <c:v>Complete TC for Reg</c:v>
+                  </c:pt>
+                  <c:pt idx="96">
+                    <c:v>Complete TC for Accounts </c:v>
+                  </c:pt>
+                  <c:pt idx="98">
+                    <c:v>Design admin TC</c:v>
+                  </c:pt>
+                  <c:pt idx="100">
+                    <c:v>Complete TC for prev Trans</c:v>
+                  </c:pt>
+                  <c:pt idx="102">
+                    <c:v>Design transfer TC</c:v>
+                  </c:pt>
+                  <c:pt idx="104">
+                    <c:v>Review on admin TC</c:v>
+                  </c:pt>
+                  <c:pt idx="106">
+                    <c:v>Review on transfer and login TC</c:v>
+                  </c:pt>
+                  <c:pt idx="108">
+                    <c:v>Review on Reg-PT-Accounts TC</c:v>
+                  </c:pt>
+                  <c:pt idx="110">
+                    <c:v>Update TC up on review comments</c:v>
+                  </c:pt>
+                  <c:pt idx="112">
+                    <c:v>Update TC up on review comments</c:v>
+                  </c:pt>
+                  <c:pt idx="114">
+                    <c:v>Update Schedule</c:v>
                   </c:pt>
                 </c:lvl>
                 <c:lvl>
@@ -1689,9 +1821,9 @@
                     <c:v>Development and Testing</c:v>
                   </c:pt>
                   <c:pt idx="91">
-                    <c:v>Testing</c:v>
-                  </c:pt>
-                  <c:pt idx="96">
+                    <c:v>Development and Testing</c:v>
+                  </c:pt>
+                  <c:pt idx="116">
                     <c:v>Delivery</c:v>
                   </c:pt>
                 </c:lvl>
@@ -1700,10 +1832,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>ProjectTimeline!$G$32:$G$133</c:f>
+              <c:f>ProjectTimeline!$G$32:$G$153</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="102"/>
+                <c:ptCount val="122"/>
                 <c:pt idx="5">
                   <c:v>5</c:v>
                 </c:pt>
@@ -1836,13 +1968,43 @@
                 <c:pt idx="92">
                   <c:v>0</c:v>
                 </c:pt>
-                <c:pt idx="93">
+                <c:pt idx="94">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="96">
                   <c:v>0</c:v>
                 </c:pt>
+                <c:pt idx="98">
+                  <c:v>0</c:v>
+                </c:pt>
                 <c:pt idx="100">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="108">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="110">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="112">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="114">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="116">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="120">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -1880,9 +2042,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:f>ProjectTimeline!$A$32:$B$133</c:f>
+              <c:f>ProjectTimeline!$A$32:$B$153</c:f>
               <c:multiLvlStrCache>
-                <c:ptCount val="97"/>
+                <c:ptCount val="117"/>
                 <c:lvl>
                   <c:pt idx="5">
                     <c:v>Responsibility Assignment Matrix</c:v>
@@ -2003,6 +2165,42 @@
                   </c:pt>
                   <c:pt idx="88">
                     <c:v>Design.TC.Previous TR Page.Front</c:v>
+                  </c:pt>
+                  <c:pt idx="92">
+                    <c:v>Optmize login TC</c:v>
+                  </c:pt>
+                  <c:pt idx="94">
+                    <c:v>Complete TC for Reg</c:v>
+                  </c:pt>
+                  <c:pt idx="96">
+                    <c:v>Complete TC for Accounts </c:v>
+                  </c:pt>
+                  <c:pt idx="98">
+                    <c:v>Design admin TC</c:v>
+                  </c:pt>
+                  <c:pt idx="100">
+                    <c:v>Complete TC for prev Trans</c:v>
+                  </c:pt>
+                  <c:pt idx="102">
+                    <c:v>Design transfer TC</c:v>
+                  </c:pt>
+                  <c:pt idx="104">
+                    <c:v>Review on admin TC</c:v>
+                  </c:pt>
+                  <c:pt idx="106">
+                    <c:v>Review on transfer and login TC</c:v>
+                  </c:pt>
+                  <c:pt idx="108">
+                    <c:v>Review on Reg-PT-Accounts TC</c:v>
+                  </c:pt>
+                  <c:pt idx="110">
+                    <c:v>Update TC up on review comments</c:v>
+                  </c:pt>
+                  <c:pt idx="112">
+                    <c:v>Update TC up on review comments</c:v>
+                  </c:pt>
+                  <c:pt idx="114">
+                    <c:v>Update Schedule</c:v>
                   </c:pt>
                 </c:lvl>
                 <c:lvl>
@@ -2019,9 +2217,9 @@
                     <c:v>Development and Testing</c:v>
                   </c:pt>
                   <c:pt idx="91">
-                    <c:v>Testing</c:v>
-                  </c:pt>
-                  <c:pt idx="96">
+                    <c:v>Development and Testing</c:v>
+                  </c:pt>
+                  <c:pt idx="116">
                     <c:v>Delivery</c:v>
                   </c:pt>
                 </c:lvl>
@@ -2030,10 +2228,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>ProjectTimeline!$H$32:$H$133</c:f>
+              <c:f>ProjectTimeline!$H$32:$H$153</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="102"/>
+                <c:ptCount val="122"/>
                 <c:pt idx="5">
                   <c:v>0</c:v>
                 </c:pt>
@@ -2166,13 +2364,43 @@
                 <c:pt idx="92">
                   <c:v>0</c:v>
                 </c:pt>
-                <c:pt idx="93">
+                <c:pt idx="94">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="96">
                   <c:v>0</c:v>
                 </c:pt>
+                <c:pt idx="98">
+                  <c:v>0</c:v>
+                </c:pt>
                 <c:pt idx="100">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="108">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="110">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="112">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="114">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="116">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="120">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -2210,9 +2438,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:f>ProjectTimeline!$A$32:$B$133</c:f>
+              <c:f>ProjectTimeline!$A$32:$B$153</c:f>
               <c:multiLvlStrCache>
-                <c:ptCount val="97"/>
+                <c:ptCount val="117"/>
                 <c:lvl>
                   <c:pt idx="5">
                     <c:v>Responsibility Assignment Matrix</c:v>
@@ -2333,6 +2561,42 @@
                   </c:pt>
                   <c:pt idx="88">
                     <c:v>Design.TC.Previous TR Page.Front</c:v>
+                  </c:pt>
+                  <c:pt idx="92">
+                    <c:v>Optmize login TC</c:v>
+                  </c:pt>
+                  <c:pt idx="94">
+                    <c:v>Complete TC for Reg</c:v>
+                  </c:pt>
+                  <c:pt idx="96">
+                    <c:v>Complete TC for Accounts </c:v>
+                  </c:pt>
+                  <c:pt idx="98">
+                    <c:v>Design admin TC</c:v>
+                  </c:pt>
+                  <c:pt idx="100">
+                    <c:v>Complete TC for prev Trans</c:v>
+                  </c:pt>
+                  <c:pt idx="102">
+                    <c:v>Design transfer TC</c:v>
+                  </c:pt>
+                  <c:pt idx="104">
+                    <c:v>Review on admin TC</c:v>
+                  </c:pt>
+                  <c:pt idx="106">
+                    <c:v>Review on transfer and login TC</c:v>
+                  </c:pt>
+                  <c:pt idx="108">
+                    <c:v>Review on Reg-PT-Accounts TC</c:v>
+                  </c:pt>
+                  <c:pt idx="110">
+                    <c:v>Update TC up on review comments</c:v>
+                  </c:pt>
+                  <c:pt idx="112">
+                    <c:v>Update TC up on review comments</c:v>
+                  </c:pt>
+                  <c:pt idx="114">
+                    <c:v>Update Schedule</c:v>
                   </c:pt>
                 </c:lvl>
                 <c:lvl>
@@ -2349,9 +2613,9 @@
                     <c:v>Development and Testing</c:v>
                   </c:pt>
                   <c:pt idx="91">
-                    <c:v>Testing</c:v>
-                  </c:pt>
-                  <c:pt idx="96">
+                    <c:v>Development and Testing</c:v>
+                  </c:pt>
+                  <c:pt idx="116">
                     <c:v>Delivery</c:v>
                   </c:pt>
                 </c:lvl>
@@ -2360,10 +2624,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>ProjectTimeline!$I$32:$I$133</c:f>
+              <c:f>ProjectTimeline!$I$32:$I$153</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="102"/>
+                <c:ptCount val="122"/>
                 <c:pt idx="5">
                   <c:v>0</c:v>
                 </c:pt>
@@ -2496,13 +2760,43 @@
                 <c:pt idx="92">
                   <c:v>0</c:v>
                 </c:pt>
-                <c:pt idx="93">
+                <c:pt idx="94">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="96">
                   <c:v>0</c:v>
                 </c:pt>
+                <c:pt idx="98">
+                  <c:v>0</c:v>
+                </c:pt>
                 <c:pt idx="100">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="108">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="110">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="112">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="114">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="116">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="120">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -2540,9 +2834,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:f>ProjectTimeline!$A$32:$B$133</c:f>
+              <c:f>ProjectTimeline!$A$32:$B$153</c:f>
               <c:multiLvlStrCache>
-                <c:ptCount val="97"/>
+                <c:ptCount val="117"/>
                 <c:lvl>
                   <c:pt idx="5">
                     <c:v>Responsibility Assignment Matrix</c:v>
@@ -2663,6 +2957,42 @@
                   </c:pt>
                   <c:pt idx="88">
                     <c:v>Design.TC.Previous TR Page.Front</c:v>
+                  </c:pt>
+                  <c:pt idx="92">
+                    <c:v>Optmize login TC</c:v>
+                  </c:pt>
+                  <c:pt idx="94">
+                    <c:v>Complete TC for Reg</c:v>
+                  </c:pt>
+                  <c:pt idx="96">
+                    <c:v>Complete TC for Accounts </c:v>
+                  </c:pt>
+                  <c:pt idx="98">
+                    <c:v>Design admin TC</c:v>
+                  </c:pt>
+                  <c:pt idx="100">
+                    <c:v>Complete TC for prev Trans</c:v>
+                  </c:pt>
+                  <c:pt idx="102">
+                    <c:v>Design transfer TC</c:v>
+                  </c:pt>
+                  <c:pt idx="104">
+                    <c:v>Review on admin TC</c:v>
+                  </c:pt>
+                  <c:pt idx="106">
+                    <c:v>Review on transfer and login TC</c:v>
+                  </c:pt>
+                  <c:pt idx="108">
+                    <c:v>Review on Reg-PT-Accounts TC</c:v>
+                  </c:pt>
+                  <c:pt idx="110">
+                    <c:v>Update TC up on review comments</c:v>
+                  </c:pt>
+                  <c:pt idx="112">
+                    <c:v>Update TC up on review comments</c:v>
+                  </c:pt>
+                  <c:pt idx="114">
+                    <c:v>Update Schedule</c:v>
                   </c:pt>
                 </c:lvl>
                 <c:lvl>
@@ -2679,9 +3009,9 @@
                     <c:v>Development and Testing</c:v>
                   </c:pt>
                   <c:pt idx="91">
-                    <c:v>Testing</c:v>
-                  </c:pt>
-                  <c:pt idx="96">
+                    <c:v>Development and Testing</c:v>
+                  </c:pt>
+                  <c:pt idx="116">
                     <c:v>Delivery</c:v>
                   </c:pt>
                 </c:lvl>
@@ -2690,10 +3020,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>ProjectTimeline!$J$32:$J$133</c:f>
+              <c:f>ProjectTimeline!$J$32:$J$153</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="102"/>
+                <c:ptCount val="122"/>
                 <c:pt idx="5">
                   <c:v>0</c:v>
                 </c:pt>
@@ -2826,13 +3156,43 @@
                 <c:pt idx="92">
                   <c:v>0</c:v>
                 </c:pt>
-                <c:pt idx="93">
+                <c:pt idx="94">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="96">
                   <c:v>0</c:v>
                 </c:pt>
+                <c:pt idx="98">
+                  <c:v>0</c:v>
+                </c:pt>
                 <c:pt idx="100">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="108">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="110">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="112">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="114">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="116">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="120">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -2870,9 +3230,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:f>ProjectTimeline!$A$32:$B$133</c:f>
+              <c:f>ProjectTimeline!$A$32:$B$153</c:f>
               <c:multiLvlStrCache>
-                <c:ptCount val="97"/>
+                <c:ptCount val="117"/>
                 <c:lvl>
                   <c:pt idx="5">
                     <c:v>Responsibility Assignment Matrix</c:v>
@@ -2993,6 +3353,42 @@
                   </c:pt>
                   <c:pt idx="88">
                     <c:v>Design.TC.Previous TR Page.Front</c:v>
+                  </c:pt>
+                  <c:pt idx="92">
+                    <c:v>Optmize login TC</c:v>
+                  </c:pt>
+                  <c:pt idx="94">
+                    <c:v>Complete TC for Reg</c:v>
+                  </c:pt>
+                  <c:pt idx="96">
+                    <c:v>Complete TC for Accounts </c:v>
+                  </c:pt>
+                  <c:pt idx="98">
+                    <c:v>Design admin TC</c:v>
+                  </c:pt>
+                  <c:pt idx="100">
+                    <c:v>Complete TC for prev Trans</c:v>
+                  </c:pt>
+                  <c:pt idx="102">
+                    <c:v>Design transfer TC</c:v>
+                  </c:pt>
+                  <c:pt idx="104">
+                    <c:v>Review on admin TC</c:v>
+                  </c:pt>
+                  <c:pt idx="106">
+                    <c:v>Review on transfer and login TC</c:v>
+                  </c:pt>
+                  <c:pt idx="108">
+                    <c:v>Review on Reg-PT-Accounts TC</c:v>
+                  </c:pt>
+                  <c:pt idx="110">
+                    <c:v>Update TC up on review comments</c:v>
+                  </c:pt>
+                  <c:pt idx="112">
+                    <c:v>Update TC up on review comments</c:v>
+                  </c:pt>
+                  <c:pt idx="114">
+                    <c:v>Update Schedule</c:v>
                   </c:pt>
                 </c:lvl>
                 <c:lvl>
@@ -3009,9 +3405,9 @@
                     <c:v>Development and Testing</c:v>
                   </c:pt>
                   <c:pt idx="91">
-                    <c:v>Testing</c:v>
-                  </c:pt>
-                  <c:pt idx="96">
+                    <c:v>Development and Testing</c:v>
+                  </c:pt>
+                  <c:pt idx="116">
                     <c:v>Delivery</c:v>
                   </c:pt>
                 </c:lvl>
@@ -3020,10 +3416,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>ProjectTimeline!$K$32:$K$133</c:f>
+              <c:f>ProjectTimeline!$K$32:$K$153</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="102"/>
+                <c:ptCount val="122"/>
                 <c:pt idx="5">
                   <c:v>0</c:v>
                 </c:pt>
@@ -3156,13 +3552,43 @@
                 <c:pt idx="92">
                   <c:v>0</c:v>
                 </c:pt>
-                <c:pt idx="93">
+                <c:pt idx="94">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="96">
                   <c:v>0</c:v>
                 </c:pt>
+                <c:pt idx="98">
+                  <c:v>0</c:v>
+                </c:pt>
                 <c:pt idx="100">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="108">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="110">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="112">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="114">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="116">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="120">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -3200,9 +3626,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:f>ProjectTimeline!$A$32:$B$133</c:f>
+              <c:f>ProjectTimeline!$A$32:$B$153</c:f>
               <c:multiLvlStrCache>
-                <c:ptCount val="97"/>
+                <c:ptCount val="117"/>
                 <c:lvl>
                   <c:pt idx="5">
                     <c:v>Responsibility Assignment Matrix</c:v>
@@ -3323,6 +3749,42 @@
                   </c:pt>
                   <c:pt idx="88">
                     <c:v>Design.TC.Previous TR Page.Front</c:v>
+                  </c:pt>
+                  <c:pt idx="92">
+                    <c:v>Optmize login TC</c:v>
+                  </c:pt>
+                  <c:pt idx="94">
+                    <c:v>Complete TC for Reg</c:v>
+                  </c:pt>
+                  <c:pt idx="96">
+                    <c:v>Complete TC for Accounts </c:v>
+                  </c:pt>
+                  <c:pt idx="98">
+                    <c:v>Design admin TC</c:v>
+                  </c:pt>
+                  <c:pt idx="100">
+                    <c:v>Complete TC for prev Trans</c:v>
+                  </c:pt>
+                  <c:pt idx="102">
+                    <c:v>Design transfer TC</c:v>
+                  </c:pt>
+                  <c:pt idx="104">
+                    <c:v>Review on admin TC</c:v>
+                  </c:pt>
+                  <c:pt idx="106">
+                    <c:v>Review on transfer and login TC</c:v>
+                  </c:pt>
+                  <c:pt idx="108">
+                    <c:v>Review on Reg-PT-Accounts TC</c:v>
+                  </c:pt>
+                  <c:pt idx="110">
+                    <c:v>Update TC up on review comments</c:v>
+                  </c:pt>
+                  <c:pt idx="112">
+                    <c:v>Update TC up on review comments</c:v>
+                  </c:pt>
+                  <c:pt idx="114">
+                    <c:v>Update Schedule</c:v>
                   </c:pt>
                 </c:lvl>
                 <c:lvl>
@@ -3339,9 +3801,9 @@
                     <c:v>Development and Testing</c:v>
                   </c:pt>
                   <c:pt idx="91">
-                    <c:v>Testing</c:v>
-                  </c:pt>
-                  <c:pt idx="96">
+                    <c:v>Development and Testing</c:v>
+                  </c:pt>
+                  <c:pt idx="116">
                     <c:v>Delivery</c:v>
                   </c:pt>
                 </c:lvl>
@@ -3350,10 +3812,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>ProjectTimeline!$L$32:$L$133</c:f>
+              <c:f>ProjectTimeline!$L$32:$L$153</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="102"/>
+                <c:ptCount val="122"/>
                 <c:pt idx="5">
                   <c:v>0</c:v>
                 </c:pt>
@@ -3481,18 +3943,48 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="91">
-                  <c:v>11</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="92">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="93">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="96">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="100">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="108">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="110">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="112">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="114">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="116">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="120">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -3514,8 +4006,8 @@
         </c:dLbls>
         <c:gapWidth val="20"/>
         <c:overlap val="100"/>
-        <c:axId val="1824398448"/>
-        <c:axId val="1824394096"/>
+        <c:axId val="-1070894080"/>
+        <c:axId val="-852247744"/>
       </c:barChart>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
@@ -3525,7 +4017,7 @@
           <c:order val="7"/>
           <c:tx>
             <c:strRef>
-              <c:f>ProjectTimeline!$B$138</c:f>
+              <c:f>ProjectTimeline!$B$158</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3616,7 +4108,7 @@
           </c:dLbls>
           <c:xVal>
             <c:numRef>
-              <c:f>(ProjectTimeline!$C$138,ProjectTimeline!$C$138)</c:f>
+              <c:f>(ProjectTimeline!$C$158,ProjectTimeline!$C$158)</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy;@</c:formatCode>
                 <c:ptCount val="2"/>
@@ -3631,7 +4123,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>ProjectTimeline!$D$138:$E$138</c:f>
+              <c:f>ProjectTimeline!$D$158:$E$158</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="2"/>
@@ -3656,7 +4148,7 @@
           <c:order val="8"/>
           <c:tx>
             <c:strRef>
-              <c:f>ProjectTimeline!$B$139</c:f>
+              <c:f>ProjectTimeline!$B$159</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3771,7 +4263,7 @@
           </c:dLbls>
           <c:xVal>
             <c:numRef>
-              <c:f>(ProjectTimeline!$C$139,ProjectTimeline!$C$139)</c:f>
+              <c:f>(ProjectTimeline!$C$159,ProjectTimeline!$C$159)</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy;@</c:formatCode>
                 <c:ptCount val="2"/>
@@ -3786,7 +4278,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>ProjectTimeline!$D$139:$E$139</c:f>
+              <c:f>ProjectTimeline!$D$159:$E$159</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="2"/>
@@ -3811,7 +4303,7 @@
           <c:order val="9"/>
           <c:tx>
             <c:strRef>
-              <c:f>ProjectTimeline!$B$140</c:f>
+              <c:f>ProjectTimeline!$B$160</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3902,7 +4394,7 @@
           </c:dLbls>
           <c:xVal>
             <c:numRef>
-              <c:f>(ProjectTimeline!$C$140,ProjectTimeline!$C$140)</c:f>
+              <c:f>(ProjectTimeline!$C$160,ProjectTimeline!$C$160)</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy;@</c:formatCode>
                 <c:ptCount val="2"/>
@@ -3917,7 +4409,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>ProjectTimeline!$D$140:$E$140</c:f>
+              <c:f>ProjectTimeline!$D$160:$E$160</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="2"/>
@@ -3942,7 +4434,7 @@
           <c:order val="10"/>
           <c:tx>
             <c:strRef>
-              <c:f>ProjectTimeline!$B$141</c:f>
+              <c:f>ProjectTimeline!$B$161</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -4033,7 +4525,7 @@
           </c:dLbls>
           <c:xVal>
             <c:numRef>
-              <c:f>(ProjectTimeline!$C$141,ProjectTimeline!$C$141)</c:f>
+              <c:f>(ProjectTimeline!$C$161,ProjectTimeline!$C$161)</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy;@</c:formatCode>
                 <c:ptCount val="2"/>
@@ -4048,7 +4540,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>ProjectTimeline!$D$141:$E$141</c:f>
+              <c:f>ProjectTimeline!$D$161:$E$161</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="2"/>
@@ -4076,11 +4568,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1824404976"/>
-        <c:axId val="1824395184"/>
+        <c:axId val="-852251552"/>
+        <c:axId val="-852245024"/>
       </c:scatterChart>
       <c:catAx>
-        <c:axId val="1824398448"/>
+        <c:axId val="-1070894080"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -4137,7 +4629,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1824394096"/>
+        <c:crossAx val="-852247744"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4147,7 +4639,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1824394096"/>
+        <c:axId val="-852247744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="43646"/>
@@ -4206,13 +4698,13 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1824398448"/>
+        <c:crossAx val="-1070894080"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="30"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1824395184"/>
+        <c:axId val="-852245024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -4223,13 +4715,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1824404976"/>
+        <c:crossAx val="-852251552"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="1"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1824404976"/>
+        <c:axId val="-852251552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4239,7 +4731,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1824395184"/>
+        <c:crossAx val="-852245024"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4848,7 +5340,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{F44686F1-DCE1-4D18-A327-C5E0B87F1EF6}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F44686F1-DCE1-4D18-A327-C5E0B87F1EF6}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4898,7 +5390,7 @@
         <xdr:cNvPr id="5" name="Chart 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{83273588-A5A1-4D9D-B78C-30406444437C}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{83273588-A5A1-4D9D-B78C-30406444437C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4941,7 +5433,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{F5E0D6A9-E059-4B8E-90BD-4CA99306D6EF}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F5E0D6A9-E059-4B8E-90BD-4CA99306D6EF}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5242,10 +5734,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:O141"/>
+  <dimension ref="A1:O161"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A78" zoomScaleNormal="100" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="A94" sqref="A94:XFD94"/>
+    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A26" zoomScaleNormal="100" zoomScalePageLayoutView="85" workbookViewId="0">
+      <selection activeCell="M146" sqref="M146"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -5264,7 +5756,7 @@
   <sheetData>
     <row r="1" spans="1:15" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B1" s="67"/>
       <c r="C1" s="8"/>
@@ -5289,18 +5781,21 @@
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="O3" s="11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="10" spans="1:15" ht="50.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="15" spans="1:15" ht="144" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="24" spans="1:13" ht="141" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="25" spans="1:13" ht="32.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="26" spans="1:13" ht="180.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="27" spans="1:13" ht="44.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="30" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B30" s="59" t="s">
         <v>10</v>
       </c>
       <c r="C30" s="34" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F30" s="61" t="s">
         <v>25</v>
@@ -5350,7 +5845,7 @@
         <v>22</v>
       </c>
       <c r="M31" s="68" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="32" spans="1:13" s="7" customFormat="1" ht="15" hidden="1" x14ac:dyDescent="0.2">
@@ -5428,7 +5923,7 @@
     </row>
     <row r="37" spans="1:13" s="7" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B37" s="31" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C37" s="32">
         <v>43582</v>
@@ -5440,11 +5935,11 @@
         <v>21</v>
       </c>
       <c r="F37" s="64">
-        <f t="shared" ref="F37:F125" si="0">IF(ISBLANK(C37),0,C37)</f>
+        <f t="shared" ref="F37:F122" si="0">IF(ISBLANK(C37),0,C37)</f>
         <v>43582</v>
       </c>
       <c r="G37" s="65">
-        <f t="shared" ref="G37:L132" si="1">IF(ISBLANK($D37),0,IF($E37=G$31,$D37-$C37+1,0))</f>
+        <f t="shared" ref="G37:L152" si="1">IF(ISBLANK($D37),0,IF($E37=G$31,$D37-$C37+1,0))</f>
         <v>5</v>
       </c>
       <c r="H37" s="65">
@@ -5468,7 +5963,7 @@
         <v>0</v>
       </c>
       <c r="M37" s="66" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="38" spans="1:13" s="7" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -5489,7 +5984,7 @@
     <row r="39" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A39" s="30"/>
       <c r="B39" s="31" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C39" s="32">
         <v>43583</v>
@@ -5523,7 +6018,7 @@
         <v>0</v>
       </c>
       <c r="M39" s="66" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="40" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
@@ -5544,7 +6039,7 @@
     <row r="41" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A41" s="30"/>
       <c r="B41" s="31" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C41" s="32">
         <v>43583</v>
@@ -5583,7 +6078,7 @@
         <v>0</v>
       </c>
       <c r="M41" s="66" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="42" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
@@ -5604,7 +6099,7 @@
     <row r="43" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A43" s="30"/>
       <c r="B43" s="31" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C43" s="32">
         <v>43584</v>
@@ -5643,7 +6138,7 @@
         <v>0</v>
       </c>
       <c r="M43" s="66" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="44" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
@@ -5664,7 +6159,7 @@
     <row r="45" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A45" s="30"/>
       <c r="B45" s="31" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C45" s="32">
         <v>43584</v>
@@ -5673,7 +6168,7 @@
         <v>43585</v>
       </c>
       <c r="E45" s="12" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F45" s="64">
         <v>43584</v>
@@ -5697,7 +6192,7 @@
         <v>0</v>
       </c>
       <c r="M45" s="66" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="46" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
@@ -5718,7 +6213,7 @@
     <row r="47" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A47" s="30"/>
       <c r="B47" s="31" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C47" s="32">
         <v>43585</v>
@@ -5756,7 +6251,7 @@
         <v>0</v>
       </c>
       <c r="M47" s="66" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="48" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
@@ -5794,7 +6289,7 @@
     <row r="50" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A50" s="30"/>
       <c r="B50" s="31" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C50" s="32">
         <v>43583</v>
@@ -5834,7 +6329,7 @@
         <v>0</v>
       </c>
       <c r="M50" s="66" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="51" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
@@ -5855,7 +6350,7 @@
     <row r="52" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A52" s="30"/>
       <c r="B52" s="31" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C52" s="32">
         <v>43584</v>
@@ -5895,7 +6390,7 @@
         <v>0</v>
       </c>
       <c r="M52" s="66" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="53" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
@@ -5916,7 +6411,7 @@
     <row r="54" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A54" s="30"/>
       <c r="B54" s="31" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C54" s="32">
         <v>43585</v>
@@ -5956,7 +6451,7 @@
         <v>0</v>
       </c>
       <c r="M54" s="66" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="55" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
@@ -5977,7 +6472,7 @@
     <row r="56" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A56" s="30"/>
       <c r="B56" s="31" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C56" s="32">
         <v>43586</v>
@@ -6017,7 +6512,7 @@
         <v>0</v>
       </c>
       <c r="M56" s="66" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="57" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
@@ -6038,7 +6533,7 @@
     <row r="58" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A58" s="30"/>
       <c r="B58" s="31" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C58" s="32">
         <v>43586</v>
@@ -6078,7 +6573,7 @@
         <v>0</v>
       </c>
       <c r="M58" s="66" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="59" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
@@ -6146,7 +6641,7 @@
     <row r="63" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A63" s="30"/>
       <c r="B63" s="31" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C63" s="32">
         <v>43590</v>
@@ -6185,7 +6680,7 @@
         <v>0</v>
       </c>
       <c r="M63" s="66" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="64" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
@@ -6206,7 +6701,7 @@
     <row r="65" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A65" s="30"/>
       <c r="B65" s="31" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C65" s="32">
         <v>43590</v>
@@ -6239,7 +6734,7 @@
         <v>0</v>
       </c>
       <c r="M65" s="66" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="66" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
@@ -6260,7 +6755,7 @@
     <row r="67" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A67" s="30"/>
       <c r="B67" s="31" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C67" s="32">
         <v>43590</v>
@@ -6299,7 +6794,7 @@
         <v>0</v>
       </c>
       <c r="M67" s="66" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="68" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
@@ -6320,7 +6815,7 @@
     <row r="69" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A69" s="30"/>
       <c r="B69" s="31" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C69" s="32">
         <v>43591</v>
@@ -6353,7 +6848,7 @@
         <v>0</v>
       </c>
       <c r="M69" s="66" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="70" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
@@ -6374,7 +6869,7 @@
     <row r="71" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A71" s="30"/>
       <c r="B71" s="31" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C71" s="32">
         <v>43591</v>
@@ -6407,7 +6902,7 @@
         <v>0</v>
       </c>
       <c r="M71" s="66" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="72" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
@@ -6428,7 +6923,7 @@
     <row r="73" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A73" s="30"/>
       <c r="B73" s="31" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C73" s="32">
         <v>43592</v>
@@ -6461,7 +6956,7 @@
         <v>0</v>
       </c>
       <c r="M73" s="66" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="74" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
@@ -6482,7 +6977,7 @@
     <row r="75" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A75" s="30"/>
       <c r="B75" s="31" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C75" s="32">
         <v>43594</v>
@@ -6521,7 +7016,7 @@
         <v>0</v>
       </c>
       <c r="M75" s="66" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="76" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
@@ -6542,7 +7037,7 @@
     <row r="77" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A77" s="30"/>
       <c r="B77" s="31" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C77" s="32">
         <v>43594</v>
@@ -6575,7 +7070,7 @@
         <v>0</v>
       </c>
       <c r="M77" s="66" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="78" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
@@ -6596,7 +7091,7 @@
     <row r="79" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A79" s="30"/>
       <c r="B79" s="31" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C79" s="32">
         <v>43594</v>
@@ -6629,7 +7124,7 @@
         <v>0</v>
       </c>
       <c r="M79" s="66" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="80" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
@@ -6650,7 +7145,7 @@
     <row r="81" spans="1:13" s="7" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A81" s="30"/>
       <c r="B81" s="31" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C81" s="32">
         <v>43594</v>
@@ -6683,7 +7178,7 @@
         <v>0</v>
       </c>
       <c r="M81" s="69" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="82" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
@@ -6703,7 +7198,7 @@
     </row>
     <row r="83" spans="1:13" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A83" s="30" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B83" s="31"/>
       <c r="C83" s="32">
@@ -6747,7 +7242,7 @@
     <row r="84" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A84" s="70"/>
       <c r="B84" s="31" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C84" s="32">
         <v>43597</v>
@@ -6787,7 +7282,7 @@
         <v>0</v>
       </c>
       <c r="M84" s="66" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="85" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
@@ -6808,7 +7303,7 @@
     <row r="86" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A86" s="30"/>
       <c r="B86" s="31" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C86" s="32">
         <v>43597</v>
@@ -6848,7 +7343,7 @@
         <v>0</v>
       </c>
       <c r="M86" s="66" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="87" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
@@ -6868,7 +7363,7 @@
     <row r="88" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A88" s="30"/>
       <c r="B88" s="31" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C88" s="32">
         <v>43597</v>
@@ -6908,7 +7403,7 @@
         <v>0</v>
       </c>
       <c r="M88" s="66" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="89" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
@@ -6929,7 +7424,7 @@
     <row r="90" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A90" s="30"/>
       <c r="B90" s="31" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C90" s="32">
         <v>43597</v>
@@ -6962,7 +7457,7 @@
         <v>0</v>
       </c>
       <c r="M90" s="66" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="91" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
@@ -6983,7 +7478,7 @@
     <row r="92" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A92" s="30"/>
       <c r="B92" s="31" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C92" s="32">
         <v>43598</v>
@@ -7016,7 +7511,7 @@
         <v>0</v>
       </c>
       <c r="M92" s="66" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="93" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
@@ -7036,7 +7531,7 @@
     <row r="94" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A94" s="30"/>
       <c r="B94" s="31" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C94" s="32">
         <v>43598</v>
@@ -7069,7 +7564,7 @@
         <v>0</v>
       </c>
       <c r="M94" s="66" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="95" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
@@ -7090,7 +7585,7 @@
     <row r="96" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A96" s="30"/>
       <c r="B96" s="31" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C96" s="32">
         <v>43598</v>
@@ -7123,7 +7618,7 @@
         <v>0</v>
       </c>
       <c r="M96" s="66" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="97" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
@@ -7144,7 +7639,7 @@
     <row r="98" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A98" s="30"/>
       <c r="B98" s="31" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C98" s="32">
         <v>43598</v>
@@ -7177,7 +7672,7 @@
         <v>0</v>
       </c>
       <c r="M98" s="66" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="99" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
@@ -7198,7 +7693,7 @@
     <row r="100" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A100" s="30"/>
       <c r="B100" s="31" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C100" s="32">
         <v>43599</v>
@@ -7231,7 +7726,7 @@
         <v>0</v>
       </c>
       <c r="M100" s="66" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="101" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
@@ -7252,7 +7747,7 @@
     <row r="102" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A102" s="30"/>
       <c r="B102" s="31" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C102" s="32">
         <v>43599</v>
@@ -7285,7 +7780,7 @@
         <v>0</v>
       </c>
       <c r="M102" s="66" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="103" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
@@ -7305,7 +7800,7 @@
     <row r="104" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A104" s="30"/>
       <c r="B104" s="31" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C104" s="32">
         <v>43599</v>
@@ -7338,7 +7833,7 @@
         <v>0</v>
       </c>
       <c r="M104" s="66" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="105" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
@@ -7359,7 +7854,7 @@
     <row r="106" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A106" s="30"/>
       <c r="B106" s="31" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C106" s="32">
         <v>43600</v>
@@ -7392,7 +7887,7 @@
         <v>0</v>
       </c>
       <c r="M106" s="66" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="107" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
@@ -7413,7 +7908,7 @@
     <row r="108" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A108" s="30"/>
       <c r="B108" s="31" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C108" s="32">
         <v>43600</v>
@@ -7446,7 +7941,7 @@
         <v>0</v>
       </c>
       <c r="M108" s="66" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="109" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
@@ -7467,7 +7962,7 @@
     <row r="110" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A110" s="30"/>
       <c r="B110" s="31" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C110" s="32">
         <v>43600</v>
@@ -7500,7 +7995,7 @@
         <v>0</v>
       </c>
       <c r="M110" s="66" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="111" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
@@ -7520,7 +8015,7 @@
     <row r="112" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A112" s="30"/>
       <c r="B112" s="31" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C112" s="32">
         <v>43600</v>
@@ -7553,7 +8048,7 @@
         <v>0</v>
       </c>
       <c r="M112" s="66" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="113" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
@@ -7574,7 +8069,7 @@
     <row r="114" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A114" s="30"/>
       <c r="B114" s="31" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C114" s="32">
         <v>43600</v>
@@ -7607,7 +8102,7 @@
         <v>0</v>
       </c>
       <c r="M114" s="66" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="115" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
@@ -7628,7 +8123,7 @@
     <row r="116" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A116" s="30"/>
       <c r="B116" s="31" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C116" s="32">
         <v>43600</v>
@@ -7661,7 +8156,7 @@
         <v>0</v>
       </c>
       <c r="M116" s="66" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="117" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
@@ -7682,7 +8177,7 @@
     <row r="118" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A118" s="30"/>
       <c r="B118" s="31" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C118" s="32">
         <v>43600</v>
@@ -7715,7 +8210,7 @@
         <v>0</v>
       </c>
       <c r="M118" s="66" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="119" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
@@ -7736,7 +8231,7 @@
     <row r="120" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A120" s="30"/>
       <c r="B120" s="31" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C120" s="32">
         <v>43601</v>
@@ -7769,7 +8264,7 @@
         <v>0</v>
       </c>
       <c r="M120" s="66" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="121" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
@@ -7825,24 +8320,15 @@
       </c>
       <c r="M122" s="66"/>
     </row>
-    <row r="123" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:13" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A123" s="30" t="s">
-        <v>61</v>
+        <v>118</v>
       </c>
       <c r="B123" s="31"/>
-      <c r="C123" s="32">
-        <v>43603</v>
-      </c>
-      <c r="D123" s="33">
-        <v>43613</v>
-      </c>
-      <c r="E123" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="F123" s="64">
-        <f>IF(ISBLANK(C123),0,C123)</f>
-        <v>43603</v>
-      </c>
+      <c r="C123" s="32"/>
+      <c r="D123" s="33"/>
+      <c r="E123" s="12"/>
+      <c r="F123" s="64"/>
       <c r="G123" s="65">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -7865,21 +8351,26 @@
       </c>
       <c r="L123" s="66">
         <f t="shared" si="1"/>
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="M123" s="66"/>
     </row>
     <row r="124" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A124" s="30"/>
-      <c r="B124" s="31"/>
-      <c r="C124" s="32"/>
-      <c r="D124" s="33"/>
+      <c r="B124" s="31" t="s">
+        <v>126</v>
+      </c>
+      <c r="C124" s="32">
+        <v>43604</v>
+      </c>
+      <c r="D124" s="33">
+        <v>43604</v>
+      </c>
       <c r="E124" s="12" t="s">
         <v>22</v>
       </c>
       <c r="F124" s="64">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <v>43604</v>
       </c>
       <c r="G124" s="65">
         <f t="shared" si="1"/>
@@ -7903,71 +8394,78 @@
       </c>
       <c r="L124" s="66">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="M124" s="66"/>
+        <v>1</v>
+      </c>
+      <c r="M124" s="66" t="s">
+        <v>122</v>
+      </c>
     </row>
     <row r="125" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A125" s="30"/>
       <c r="B125" s="31"/>
       <c r="C125" s="32"/>
       <c r="D125" s="33"/>
-      <c r="E125" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="F125" s="64">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G125" s="65">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="H125" s="65">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="I125" s="65">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J125" s="65">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="K125" s="65">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="L125" s="66">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
+      <c r="E125" s="12"/>
+      <c r="F125" s="64"/>
+      <c r="G125" s="65"/>
+      <c r="H125" s="65"/>
+      <c r="I125" s="65"/>
+      <c r="J125" s="65"/>
+      <c r="K125" s="65"/>
+      <c r="L125" s="66"/>
       <c r="M125" s="66"/>
     </row>
     <row r="126" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A126" s="30"/>
-      <c r="B126" s="31"/>
-      <c r="C126" s="32"/>
-      <c r="D126" s="33"/>
-      <c r="E126" s="12"/>
-      <c r="F126" s="64"/>
-      <c r="G126" s="65"/>
-      <c r="H126" s="65"/>
-      <c r="I126" s="65"/>
-      <c r="J126" s="65"/>
-      <c r="K126" s="65"/>
-      <c r="L126" s="66"/>
-      <c r="M126" s="66"/>
+      <c r="B126" s="31" t="s">
+        <v>121</v>
+      </c>
+      <c r="C126" s="32">
+        <v>43604</v>
+      </c>
+      <c r="D126" s="33">
+        <v>43604</v>
+      </c>
+      <c r="E126" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="F126" s="64">
+        <v>43604</v>
+      </c>
+      <c r="G126" s="65">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H126" s="65">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I126" s="65">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J126" s="65">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K126" s="65">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L126" s="66">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="M126" s="66" t="s">
+        <v>123</v>
+      </c>
     </row>
     <row r="127" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A127" s="30"/>
       <c r="B127" s="31"/>
       <c r="C127" s="32"/>
       <c r="D127" s="33"/>
-      <c r="E127" s="12" t="s">
-        <v>22</v>
-      </c>
+      <c r="E127" s="12"/>
       <c r="F127" s="64"/>
       <c r="G127" s="65"/>
       <c r="H127" s="65"/>
@@ -7978,22 +8476,21 @@
       <c r="M127" s="66"/>
     </row>
     <row r="128" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A128" s="30" t="s">
-        <v>83</v>
-      </c>
-      <c r="B128" s="31"/>
+      <c r="A128" s="30"/>
+      <c r="B128" s="31" t="s">
+        <v>124</v>
+      </c>
       <c r="C128" s="32">
-        <v>43610</v>
+        <v>43605</v>
       </c>
       <c r="D128" s="33">
-        <v>43613</v>
+        <v>43605</v>
       </c>
       <c r="E128" s="12" t="s">
-        <v>82</v>
+        <v>22</v>
       </c>
       <c r="F128" s="64">
-        <f t="shared" ref="F128" si="4">IF(ISBLANK(C128),0,C128)</f>
-        <v>43610</v>
+        <v>43605</v>
       </c>
       <c r="G128" s="65">
         <f t="shared" si="1"/>
@@ -8017,18 +8514,18 @@
       </c>
       <c r="L128" s="66">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="M128" s="66"/>
+        <v>1</v>
+      </c>
+      <c r="M128" s="66" t="s">
+        <v>123</v>
+      </c>
     </row>
     <row r="129" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A129" s="30"/>
       <c r="B129" s="31"/>
       <c r="C129" s="32"/>
       <c r="D129" s="33"/>
-      <c r="E129" s="12" t="s">
-        <v>82</v>
-      </c>
+      <c r="E129" s="12"/>
       <c r="F129" s="64"/>
       <c r="G129" s="65"/>
       <c r="H129" s="65"/>
@@ -8040,29 +8537,55 @@
     </row>
     <row r="130" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A130" s="30"/>
-      <c r="B130" s="31"/>
-      <c r="C130" s="32"/>
-      <c r="D130" s="33"/>
+      <c r="B130" s="31" t="s">
+        <v>125</v>
+      </c>
+      <c r="C130" s="32">
+        <v>43605</v>
+      </c>
+      <c r="D130" s="33">
+        <v>43606</v>
+      </c>
       <c r="E130" s="12" t="s">
-        <v>82</v>
-      </c>
-      <c r="F130" s="64"/>
-      <c r="G130" s="65"/>
-      <c r="H130" s="65"/>
-      <c r="I130" s="65"/>
-      <c r="J130" s="65"/>
-      <c r="K130" s="65"/>
-      <c r="L130" s="66"/>
-      <c r="M130" s="66"/>
+        <v>22</v>
+      </c>
+      <c r="F130" s="64">
+        <v>43605</v>
+      </c>
+      <c r="G130" s="65">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H130" s="65">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I130" s="65">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J130" s="65">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K130" s="65">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L130" s="66">
+        <f>IF(ISBLANK($D130),0,IF($E130=L$31,$D130-$C130+1,0))</f>
+        <v>2</v>
+      </c>
+      <c r="M130" s="66" t="s">
+        <v>122</v>
+      </c>
     </row>
     <row r="131" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A131" s="30"/>
       <c r="B131" s="31"/>
       <c r="C131" s="32"/>
       <c r="D131" s="33"/>
-      <c r="E131" s="12" t="s">
-        <v>82</v>
-      </c>
+      <c r="E131" s="12"/>
       <c r="F131" s="64"/>
       <c r="G131" s="65"/>
       <c r="H131" s="65"/>
@@ -8074,132 +8597,707 @@
     </row>
     <row r="132" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A132" s="30"/>
-      <c r="B132" s="31"/>
-      <c r="C132" s="32"/>
-      <c r="D132" s="33"/>
+      <c r="B132" s="31" t="s">
+        <v>127</v>
+      </c>
+      <c r="C132" s="32">
+        <v>43606</v>
+      </c>
+      <c r="D132" s="33">
+        <v>43606</v>
+      </c>
       <c r="E132" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="F132" s="64">
+        <v>43606</v>
+      </c>
+      <c r="G132" s="65">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H132" s="65">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I132" s="65">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J132" s="65">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K132" s="65">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L132" s="66">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="M132" s="66" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="133" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A133" s="30"/>
+      <c r="B133" s="31"/>
+      <c r="C133" s="32"/>
+      <c r="D133" s="33"/>
+      <c r="E133" s="12"/>
+      <c r="F133" s="64"/>
+      <c r="G133" s="65"/>
+      <c r="H133" s="65"/>
+      <c r="I133" s="65"/>
+      <c r="J133" s="65"/>
+      <c r="K133" s="65"/>
+      <c r="L133" s="66"/>
+      <c r="M133" s="66"/>
+    </row>
+    <row r="134" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A134" s="30"/>
+      <c r="B134" s="31" t="s">
+        <v>128</v>
+      </c>
+      <c r="C134" s="32">
+        <v>43607</v>
+      </c>
+      <c r="D134" s="33">
+        <v>43608</v>
+      </c>
+      <c r="E134" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="F134" s="64">
+        <v>43607</v>
+      </c>
+      <c r="G134" s="65">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H134" s="65">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I134" s="65">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J134" s="65">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K134" s="65">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L134" s="66">
+        <f>IF(ISBLANK($D134),0,IF($E134=L$31,$D134-$C134+1,0))</f>
+        <v>2</v>
+      </c>
+      <c r="M134" s="66" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="135" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A135" s="30"/>
+      <c r="B135" s="31"/>
+      <c r="C135" s="32"/>
+      <c r="D135" s="33"/>
+      <c r="E135" s="12"/>
+      <c r="F135" s="64"/>
+      <c r="G135" s="65"/>
+      <c r="H135" s="65"/>
+      <c r="I135" s="65"/>
+      <c r="J135" s="65"/>
+      <c r="K135" s="65"/>
+      <c r="L135" s="66"/>
+      <c r="M135" s="66"/>
+    </row>
+    <row r="136" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A136" s="30"/>
+      <c r="B136" s="31" t="s">
+        <v>129</v>
+      </c>
+      <c r="C136" s="32">
+        <v>43607</v>
+      </c>
+      <c r="D136" s="33">
+        <v>43607</v>
+      </c>
+      <c r="E136" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="F136" s="64">
+        <v>43607</v>
+      </c>
+      <c r="G136" s="65">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H136" s="65">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I136" s="65">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J136" s="65">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K136" s="65">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L136" s="66">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="M136" s="66" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="137" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A137" s="30"/>
+      <c r="B137" s="31"/>
+      <c r="C137" s="32"/>
+      <c r="D137" s="33"/>
+      <c r="E137" s="12"/>
+      <c r="F137" s="64"/>
+      <c r="G137" s="65"/>
+      <c r="H137" s="65"/>
+      <c r="I137" s="65"/>
+      <c r="J137" s="65"/>
+      <c r="K137" s="65"/>
+      <c r="L137" s="66"/>
+      <c r="M137" s="66"/>
+    </row>
+    <row r="138" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A138" s="30"/>
+      <c r="B138" s="31" t="s">
+        <v>130</v>
+      </c>
+      <c r="C138" s="32">
+        <v>43608</v>
+      </c>
+      <c r="D138" s="33">
+        <v>43608</v>
+      </c>
+      <c r="E138" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="F138" s="64">
+        <v>43608</v>
+      </c>
+      <c r="G138" s="65">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H138" s="65">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I138" s="65">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J138" s="65">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K138" s="65">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L138" s="66">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="M138" s="66" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="139" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A139" s="30"/>
+      <c r="B139" s="31"/>
+      <c r="C139" s="32"/>
+      <c r="D139" s="33"/>
+      <c r="E139" s="12"/>
+      <c r="F139" s="64"/>
+      <c r="G139" s="65"/>
+      <c r="H139" s="65"/>
+      <c r="I139" s="65"/>
+      <c r="J139" s="65"/>
+      <c r="K139" s="65"/>
+      <c r="L139" s="66"/>
+      <c r="M139" s="66"/>
+    </row>
+    <row r="140" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A140" s="30"/>
+      <c r="B140" s="31" t="s">
+        <v>132</v>
+      </c>
+      <c r="C140" s="32">
+        <v>43608</v>
+      </c>
+      <c r="D140" s="33">
+        <v>43609</v>
+      </c>
+      <c r="E140" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="F140" s="64">
+        <v>43608</v>
+      </c>
+      <c r="G140" s="65">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H140" s="65">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I140" s="65">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J140" s="65">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K140" s="65">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L140" s="66">
+        <f>IF(ISBLANK($D140),0,IF($E140=L$31,$D140-$C140+1,0))</f>
+        <v>2</v>
+      </c>
+      <c r="M140" s="66" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="141" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A141" s="30"/>
+      <c r="B141" s="31"/>
+      <c r="C141" s="32"/>
+      <c r="D141" s="33"/>
+      <c r="E141" s="12"/>
+      <c r="F141" s="64"/>
+      <c r="G141" s="65"/>
+      <c r="H141" s="65"/>
+      <c r="I141" s="65"/>
+      <c r="J141" s="65"/>
+      <c r="K141" s="65"/>
+      <c r="L141" s="66"/>
+      <c r="M141" s="66"/>
+    </row>
+    <row r="142" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A142" s="30"/>
+      <c r="B142" s="31" t="s">
+        <v>131</v>
+      </c>
+      <c r="C142" s="32">
+        <v>43608</v>
+      </c>
+      <c r="D142" s="33">
+        <v>43609</v>
+      </c>
+      <c r="E142" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="F142" s="64">
+        <v>43608</v>
+      </c>
+      <c r="G142" s="65">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H142" s="65">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I142" s="65">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J142" s="65">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K142" s="65">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L142" s="66">
+        <f>IF(ISBLANK($D142),0,IF($E142=L$31,$D142-$C142+1,0))</f>
+        <v>2</v>
+      </c>
+      <c r="M142" s="66" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="143" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A143" s="30"/>
+      <c r="B143" s="31"/>
+      <c r="C143" s="32"/>
+      <c r="D143" s="33"/>
+      <c r="E143" s="12"/>
+      <c r="F143" s="64"/>
+      <c r="G143" s="65"/>
+      <c r="H143" s="65"/>
+      <c r="I143" s="65"/>
+      <c r="J143" s="65"/>
+      <c r="K143" s="65"/>
+      <c r="L143" s="66"/>
+      <c r="M143" s="66"/>
+    </row>
+    <row r="144" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A144" s="30"/>
+      <c r="B144" s="31" t="s">
+        <v>131</v>
+      </c>
+      <c r="C144" s="32">
+        <v>43609</v>
+      </c>
+      <c r="D144" s="33">
+        <v>43609</v>
+      </c>
+      <c r="E144" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="F144" s="64">
+        <v>43609</v>
+      </c>
+      <c r="G144" s="65">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H144" s="65">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I144" s="65">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J144" s="65">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K144" s="65">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L144" s="66">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="M144" s="66" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="145" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A145" s="30"/>
+      <c r="B145" s="31"/>
+      <c r="C145" s="32"/>
+      <c r="D145" s="33"/>
+      <c r="E145" s="12"/>
+      <c r="F145" s="64"/>
+      <c r="G145" s="65"/>
+      <c r="H145" s="65"/>
+      <c r="I145" s="65"/>
+      <c r="J145" s="65"/>
+      <c r="K145" s="65"/>
+      <c r="L145" s="66"/>
+      <c r="M145" s="66"/>
+    </row>
+    <row r="146" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A146" s="30"/>
+      <c r="B146" s="31" t="s">
+        <v>94</v>
+      </c>
+      <c r="C146" s="32">
+        <v>43609</v>
+      </c>
+      <c r="D146" s="33">
+        <v>43609</v>
+      </c>
+      <c r="E146" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="F146" s="64">
+        <v>43609</v>
+      </c>
+      <c r="G146" s="65">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H146" s="65">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I146" s="65">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J146" s="65">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K146" s="65">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L146" s="66">
+        <f>IF(ISBLANK($D146),0,IF($E146=L$31,$D146-$C146+1,0))</f>
+        <v>1</v>
+      </c>
+      <c r="M146" s="66" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="147" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A147" s="30"/>
+      <c r="B147" s="31"/>
+      <c r="C147" s="32"/>
+      <c r="D147" s="33"/>
+      <c r="E147" s="12"/>
+      <c r="F147" s="64"/>
+      <c r="G147" s="65"/>
+      <c r="H147" s="65"/>
+      <c r="I147" s="65"/>
+      <c r="J147" s="65"/>
+      <c r="K147" s="65"/>
+      <c r="L147" s="66"/>
+      <c r="M147" s="66"/>
+    </row>
+    <row r="148" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A148" s="30" t="s">
         <v>82</v>
       </c>
-      <c r="F132" s="64">
-        <f>IF(ISBLANK(C132),0,C132)</f>
-        <v>0</v>
-      </c>
-      <c r="G132" s="65">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="H132" s="65">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="I132" s="65">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J132" s="65">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="K132" s="65">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="L132" s="66">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="M132" s="66"/>
-    </row>
-    <row r="133" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A133" s="24"/>
-      <c r="B133" s="25"/>
-      <c r="C133" s="26" t="s">
+      <c r="B148" s="31"/>
+      <c r="C148" s="32">
+        <v>43610</v>
+      </c>
+      <c r="D148" s="33">
+        <v>43613</v>
+      </c>
+      <c r="E148" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="F148" s="64">
+        <f t="shared" ref="F148" si="4">IF(ISBLANK(C148),0,C148)</f>
+        <v>43610</v>
+      </c>
+      <c r="G148" s="65">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H148" s="65">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I148" s="65">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J148" s="65">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K148" s="65">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L148" s="66">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M148" s="66"/>
+    </row>
+    <row r="149" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A149" s="30"/>
+      <c r="B149" s="31"/>
+      <c r="C149" s="32"/>
+      <c r="D149" s="33"/>
+      <c r="E149" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="F149" s="64"/>
+      <c r="G149" s="65"/>
+      <c r="H149" s="65"/>
+      <c r="I149" s="65"/>
+      <c r="J149" s="65"/>
+      <c r="K149" s="65"/>
+      <c r="L149" s="66"/>
+      <c r="M149" s="66"/>
+    </row>
+    <row r="150" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A150" s="30"/>
+      <c r="B150" s="31"/>
+      <c r="C150" s="32"/>
+      <c r="D150" s="33"/>
+      <c r="E150" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="F150" s="64"/>
+      <c r="G150" s="65"/>
+      <c r="H150" s="65"/>
+      <c r="I150" s="65"/>
+      <c r="J150" s="65"/>
+      <c r="K150" s="65"/>
+      <c r="L150" s="66"/>
+      <c r="M150" s="66"/>
+    </row>
+    <row r="151" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A151" s="30"/>
+      <c r="B151" s="31"/>
+      <c r="C151" s="32"/>
+      <c r="D151" s="33"/>
+      <c r="E151" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="F151" s="64"/>
+      <c r="G151" s="65"/>
+      <c r="H151" s="65"/>
+      <c r="I151" s="65"/>
+      <c r="J151" s="65"/>
+      <c r="K151" s="65"/>
+      <c r="L151" s="66"/>
+      <c r="M151" s="66"/>
+    </row>
+    <row r="152" spans="1:13" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A152" s="30"/>
+      <c r="B152" s="31"/>
+      <c r="C152" s="32"/>
+      <c r="D152" s="33"/>
+      <c r="E152" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="F152" s="64">
+        <f>IF(ISBLANK(C152),0,C152)</f>
+        <v>0</v>
+      </c>
+      <c r="G152" s="65">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H152" s="65">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I152" s="65">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J152" s="65">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K152" s="65">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L152" s="66">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M152" s="66"/>
+    </row>
+    <row r="153" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A153" s="24"/>
+      <c r="B153" s="25"/>
+      <c r="C153" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="D133" s="27"/>
-      <c r="E133" s="27"/>
-      <c r="F133" s="28"/>
-      <c r="G133" s="28"/>
-      <c r="H133" s="28"/>
-      <c r="I133" s="28"/>
-      <c r="J133" s="28"/>
-      <c r="K133" s="28"/>
-      <c r="L133" s="29"/>
-      <c r="M133" s="29"/>
-    </row>
-    <row r="137" spans="1:13" ht="24" x14ac:dyDescent="0.2">
-      <c r="B137" s="19" t="s">
+      <c r="D153" s="27"/>
+      <c r="E153" s="27"/>
+      <c r="F153" s="28"/>
+      <c r="G153" s="28"/>
+      <c r="H153" s="28"/>
+      <c r="I153" s="28"/>
+      <c r="J153" s="28"/>
+      <c r="K153" s="28"/>
+      <c r="L153" s="29"/>
+      <c r="M153" s="29"/>
+    </row>
+    <row r="157" spans="1:13" ht="24" x14ac:dyDescent="0.2">
+      <c r="B157" s="19" t="s">
         <v>46</v>
       </c>
-      <c r="C137" s="19" t="s">
+      <c r="C157" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="D137" s="60" t="s">
+      <c r="D157" s="60" t="s">
         <v>48</v>
       </c>
-      <c r="E137" s="60" t="s">
+      <c r="E157" s="60" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="138" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B138" s="31" t="s">
+    <row r="158" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B158" s="31" t="s">
         <v>42</v>
       </c>
-      <c r="C138" s="57">
+      <c r="C158" s="57">
         <v>43588</v>
       </c>
-      <c r="D138" s="58">
+      <c r="D158" s="58">
         <v>0.5</v>
       </c>
-      <c r="E138" s="58">
+      <c r="E158" s="58">
         <v>0.95</v>
       </c>
     </row>
-    <row r="139" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B139" s="31" t="s">
+    <row r="159" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B159" s="31" t="s">
         <v>43</v>
       </c>
-      <c r="C139" s="57">
+      <c r="C159" s="57">
         <v>43595</v>
       </c>
-      <c r="D139" s="58">
+      <c r="D159" s="58">
         <v>0.25</v>
       </c>
-      <c r="E139" s="58">
+      <c r="E159" s="58">
         <v>0.95</v>
       </c>
     </row>
-    <row r="140" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B140" s="31" t="s">
+    <row r="160" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B160" s="31" t="s">
         <v>44</v>
       </c>
-      <c r="C140" s="57">
+      <c r="C160" s="57">
         <v>43602</v>
       </c>
-      <c r="D140" s="58">
+      <c r="D160" s="58">
         <v>0.1</v>
       </c>
-      <c r="E140" s="58">
+      <c r="E160" s="58">
         <v>0.95</v>
       </c>
     </row>
-    <row r="141" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B141" s="31" t="s">
+    <row r="161" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B161" s="31" t="s">
         <v>45</v>
       </c>
-      <c r="C141" s="57">
+      <c r="C161" s="57">
         <v>43609</v>
       </c>
-      <c r="D141" s="58">
+      <c r="D161" s="58">
         <v>0.3</v>
       </c>
-      <c r="E141" s="58">
+      <c r="E161" s="58">
         <v>0.95</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" sqref="E32:E132">
+    <dataValidation type="list" allowBlank="1" sqref="E32:E152">
       <formula1>$G$31:$L$31</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>